<commit_message>
* Add emissive texture for SC-B-HUS * Add emissive thermal module to SC-B-HUS config * Add particle and sound effects to SC-B-BPC (Launch Abort System) * Fix inverted interior nodes on SC-C-FB 5m and 8m parts * Add auto-brakes to landing leg module; should resolve issues of them sliding (SC-C-LM mostly) * Fix missing faces on bottom of ladder for LC5-POD * Update texture for LC2-POD (diff/spec/norm) * Update texture for LC3-POD (diff/spec/norm) * Update texture for LC5-POD (diff/spec/norm) * Add glow texture for LC2-POD (needs lighting module) * Add glow texture for LC3-POD (needs lighting module) * Add glow texture for LC5-POD (needs lighting module) * Adjust interior seating position in LC3-POD-IVA; testing out various positioning... will likely not keep this positioning either, it was just the last one I had tested
</commit_message>
<xml_diff>
--- a/GameData/SSTU/Parts/Parts-MassCalc.xlsx
+++ b/GameData/SSTU/Parts/Parts-MassCalc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="parts" sheetId="1" r:id="rId1"/>
@@ -1033,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y150"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
@@ -30401,43 +30401,153 @@
     </row>
   </sheetData>
   <mergeCells count="208">
-    <mergeCell ref="AX119:BC119"/>
-    <mergeCell ref="BF119:BK119"/>
-    <mergeCell ref="AX120:BC120"/>
-    <mergeCell ref="BF120:BK120"/>
-    <mergeCell ref="AX116:BC116"/>
-    <mergeCell ref="BF116:BK116"/>
-    <mergeCell ref="AX117:BC117"/>
-    <mergeCell ref="BF117:BK117"/>
-    <mergeCell ref="AX118:BC118"/>
-    <mergeCell ref="BF118:BK118"/>
-    <mergeCell ref="AX94:BC94"/>
-    <mergeCell ref="BF94:BK94"/>
-    <mergeCell ref="AX95:BC95"/>
-    <mergeCell ref="BF95:BK95"/>
-    <mergeCell ref="AX96:BC96"/>
-    <mergeCell ref="BF96:BK96"/>
-    <mergeCell ref="AX72:BC72"/>
-    <mergeCell ref="BF72:BK72"/>
-    <mergeCell ref="AX92:BC92"/>
-    <mergeCell ref="BF92:BK92"/>
-    <mergeCell ref="AX93:BC93"/>
-    <mergeCell ref="BF93:BK93"/>
-    <mergeCell ref="BF23:BK23"/>
-    <mergeCell ref="AX24:BC24"/>
-    <mergeCell ref="BF24:BK24"/>
-    <mergeCell ref="AX69:BC69"/>
-    <mergeCell ref="BF69:BK69"/>
-    <mergeCell ref="AX70:BC70"/>
-    <mergeCell ref="BF70:BK70"/>
-    <mergeCell ref="AX71:BC71"/>
-    <mergeCell ref="BF71:BK71"/>
-    <mergeCell ref="AX47:BC47"/>
-    <mergeCell ref="BF47:BK47"/>
-    <mergeCell ref="AX48:BC48"/>
-    <mergeCell ref="BF48:BK48"/>
-    <mergeCell ref="AX68:BC68"/>
-    <mergeCell ref="BF68:BK68"/>
+    <mergeCell ref="R117:W117"/>
+    <mergeCell ref="R118:W118"/>
+    <mergeCell ref="B120:G120"/>
+    <mergeCell ref="J20:O20"/>
+    <mergeCell ref="J21:O21"/>
+    <mergeCell ref="J22:O22"/>
+    <mergeCell ref="J23:O23"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="J44:O44"/>
+    <mergeCell ref="J45:O45"/>
+    <mergeCell ref="J46:O46"/>
+    <mergeCell ref="J47:O47"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="B96:G96"/>
+    <mergeCell ref="B116:G116"/>
+    <mergeCell ref="B117:G117"/>
+    <mergeCell ref="B118:G118"/>
+    <mergeCell ref="B119:G119"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="B71:G71"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="B92:G92"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="B94:G94"/>
+    <mergeCell ref="Z117:AE117"/>
+    <mergeCell ref="Z118:AE118"/>
+    <mergeCell ref="J117:O117"/>
+    <mergeCell ref="J118:O118"/>
+    <mergeCell ref="J119:O119"/>
+    <mergeCell ref="J120:O120"/>
+    <mergeCell ref="R20:W20"/>
+    <mergeCell ref="R21:W21"/>
+    <mergeCell ref="R22:W22"/>
+    <mergeCell ref="R23:W23"/>
+    <mergeCell ref="R24:W24"/>
+    <mergeCell ref="R44:W44"/>
+    <mergeCell ref="J92:O92"/>
+    <mergeCell ref="J93:O93"/>
+    <mergeCell ref="J94:O94"/>
+    <mergeCell ref="J95:O95"/>
+    <mergeCell ref="J96:O96"/>
+    <mergeCell ref="J116:O116"/>
+    <mergeCell ref="J48:O48"/>
+    <mergeCell ref="J68:O68"/>
+    <mergeCell ref="J69:O69"/>
+    <mergeCell ref="J70:O70"/>
+    <mergeCell ref="J71:O71"/>
+    <mergeCell ref="J72:O72"/>
+    <mergeCell ref="Z116:AE116"/>
+    <mergeCell ref="Z48:AE48"/>
+    <mergeCell ref="Z68:AE68"/>
+    <mergeCell ref="Z69:AE69"/>
+    <mergeCell ref="Z70:AE70"/>
+    <mergeCell ref="Z71:AE71"/>
+    <mergeCell ref="Z72:AE72"/>
+    <mergeCell ref="R95:W95"/>
+    <mergeCell ref="R96:W96"/>
+    <mergeCell ref="R116:W116"/>
+    <mergeCell ref="R48:W48"/>
+    <mergeCell ref="R68:W68"/>
+    <mergeCell ref="R69:W69"/>
+    <mergeCell ref="R71:W71"/>
+    <mergeCell ref="R72:W72"/>
+    <mergeCell ref="R92:W92"/>
+    <mergeCell ref="R93:W93"/>
+    <mergeCell ref="R94:W94"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="Y1:AE1"/>
+    <mergeCell ref="Z92:AE92"/>
+    <mergeCell ref="Z93:AE93"/>
+    <mergeCell ref="Z94:AE94"/>
+    <mergeCell ref="Z95:AE95"/>
+    <mergeCell ref="Z96:AE96"/>
+    <mergeCell ref="R45:W45"/>
+    <mergeCell ref="R46:W46"/>
+    <mergeCell ref="R47:W47"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B68:G68"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="R120:W120"/>
+    <mergeCell ref="Z20:AE20"/>
+    <mergeCell ref="Z21:AE21"/>
+    <mergeCell ref="Z22:AE22"/>
+    <mergeCell ref="R119:W119"/>
+    <mergeCell ref="R70:W70"/>
+    <mergeCell ref="AH46:AM46"/>
+    <mergeCell ref="AH47:AM47"/>
+    <mergeCell ref="AH48:AM48"/>
+    <mergeCell ref="AH68:AM68"/>
+    <mergeCell ref="AH71:AM71"/>
+    <mergeCell ref="AH72:AM72"/>
+    <mergeCell ref="AH92:AM92"/>
+    <mergeCell ref="AH93:AM93"/>
+    <mergeCell ref="AH44:AM44"/>
+    <mergeCell ref="AH45:AM45"/>
+    <mergeCell ref="Z23:AE23"/>
+    <mergeCell ref="Z24:AE24"/>
+    <mergeCell ref="Z44:AE44"/>
+    <mergeCell ref="Z45:AE45"/>
+    <mergeCell ref="Z46:AE46"/>
+    <mergeCell ref="Z47:AE47"/>
+    <mergeCell ref="Z119:AE119"/>
+    <mergeCell ref="Z120:AE120"/>
+    <mergeCell ref="AG1:AM1"/>
+    <mergeCell ref="AH20:AM20"/>
+    <mergeCell ref="AH21:AM21"/>
+    <mergeCell ref="AH22:AM22"/>
+    <mergeCell ref="AH23:AM23"/>
+    <mergeCell ref="AH24:AM24"/>
+    <mergeCell ref="AH119:AM119"/>
+    <mergeCell ref="AH120:AM120"/>
+    <mergeCell ref="AO1:AU1"/>
+    <mergeCell ref="AP20:AU20"/>
+    <mergeCell ref="AP21:AU21"/>
+    <mergeCell ref="AP22:AU22"/>
+    <mergeCell ref="AP23:AU23"/>
+    <mergeCell ref="AP24:AU24"/>
+    <mergeCell ref="AP44:AU44"/>
+    <mergeCell ref="AP45:AU45"/>
+    <mergeCell ref="AH94:AM94"/>
+    <mergeCell ref="AH95:AM95"/>
+    <mergeCell ref="AH96:AM96"/>
+    <mergeCell ref="AH116:AM116"/>
+    <mergeCell ref="AH117:AM117"/>
+    <mergeCell ref="AH118:AM118"/>
+    <mergeCell ref="AH69:AM69"/>
+    <mergeCell ref="AH70:AM70"/>
+    <mergeCell ref="AP118:AU118"/>
+    <mergeCell ref="AP119:AU119"/>
+    <mergeCell ref="AP120:AU120"/>
+    <mergeCell ref="AP71:AU71"/>
+    <mergeCell ref="AP72:AU72"/>
+    <mergeCell ref="AP92:AU92"/>
+    <mergeCell ref="AP93:AU93"/>
+    <mergeCell ref="AP94:AU94"/>
+    <mergeCell ref="AP95:AU95"/>
     <mergeCell ref="AW1:BC1"/>
     <mergeCell ref="BE1:BK1"/>
     <mergeCell ref="AX20:BC20"/>
@@ -30462,153 +30572,43 @@
     <mergeCell ref="AX22:BC22"/>
     <mergeCell ref="BF22:BK22"/>
     <mergeCell ref="AX23:BC23"/>
-    <mergeCell ref="AP118:AU118"/>
-    <mergeCell ref="AP119:AU119"/>
-    <mergeCell ref="AP120:AU120"/>
-    <mergeCell ref="AP71:AU71"/>
-    <mergeCell ref="AP72:AU72"/>
-    <mergeCell ref="AP92:AU92"/>
-    <mergeCell ref="AP93:AU93"/>
-    <mergeCell ref="AP94:AU94"/>
-    <mergeCell ref="AP95:AU95"/>
-    <mergeCell ref="AG1:AM1"/>
-    <mergeCell ref="AH20:AM20"/>
-    <mergeCell ref="AH21:AM21"/>
-    <mergeCell ref="AH22:AM22"/>
-    <mergeCell ref="AH23:AM23"/>
-    <mergeCell ref="AH24:AM24"/>
-    <mergeCell ref="AH119:AM119"/>
-    <mergeCell ref="AH120:AM120"/>
-    <mergeCell ref="AO1:AU1"/>
-    <mergeCell ref="AP20:AU20"/>
-    <mergeCell ref="AP21:AU21"/>
-    <mergeCell ref="AP22:AU22"/>
-    <mergeCell ref="AP23:AU23"/>
-    <mergeCell ref="AP24:AU24"/>
-    <mergeCell ref="AP44:AU44"/>
-    <mergeCell ref="AP45:AU45"/>
-    <mergeCell ref="AH94:AM94"/>
-    <mergeCell ref="AH95:AM95"/>
-    <mergeCell ref="AH96:AM96"/>
-    <mergeCell ref="AH116:AM116"/>
-    <mergeCell ref="AH117:AM117"/>
-    <mergeCell ref="AH118:AM118"/>
-    <mergeCell ref="AH69:AM69"/>
-    <mergeCell ref="AH70:AM70"/>
-    <mergeCell ref="R120:W120"/>
-    <mergeCell ref="Z20:AE20"/>
-    <mergeCell ref="Z21:AE21"/>
-    <mergeCell ref="Z22:AE22"/>
-    <mergeCell ref="R119:W119"/>
-    <mergeCell ref="R70:W70"/>
-    <mergeCell ref="AH46:AM46"/>
-    <mergeCell ref="AH47:AM47"/>
-    <mergeCell ref="AH48:AM48"/>
-    <mergeCell ref="AH68:AM68"/>
-    <mergeCell ref="AH71:AM71"/>
-    <mergeCell ref="AH72:AM72"/>
-    <mergeCell ref="AH92:AM92"/>
-    <mergeCell ref="AH93:AM93"/>
-    <mergeCell ref="AH44:AM44"/>
-    <mergeCell ref="AH45:AM45"/>
-    <mergeCell ref="Z23:AE23"/>
-    <mergeCell ref="Z24:AE24"/>
-    <mergeCell ref="Z44:AE44"/>
-    <mergeCell ref="Z45:AE45"/>
-    <mergeCell ref="Z46:AE46"/>
-    <mergeCell ref="Z47:AE47"/>
-    <mergeCell ref="Z119:AE119"/>
-    <mergeCell ref="Z120:AE120"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="Y1:AE1"/>
-    <mergeCell ref="Z92:AE92"/>
-    <mergeCell ref="Z93:AE93"/>
-    <mergeCell ref="Z94:AE94"/>
-    <mergeCell ref="Z95:AE95"/>
-    <mergeCell ref="Z96:AE96"/>
-    <mergeCell ref="R45:W45"/>
-    <mergeCell ref="R46:W46"/>
-    <mergeCell ref="R47:W47"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B68:G68"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="Z116:AE116"/>
-    <mergeCell ref="Z48:AE48"/>
-    <mergeCell ref="Z68:AE68"/>
-    <mergeCell ref="Z69:AE69"/>
-    <mergeCell ref="Z70:AE70"/>
-    <mergeCell ref="Z71:AE71"/>
-    <mergeCell ref="Z72:AE72"/>
-    <mergeCell ref="R95:W95"/>
-    <mergeCell ref="R96:W96"/>
-    <mergeCell ref="R116:W116"/>
-    <mergeCell ref="R48:W48"/>
-    <mergeCell ref="R68:W68"/>
-    <mergeCell ref="R69:W69"/>
-    <mergeCell ref="R71:W71"/>
-    <mergeCell ref="R72:W72"/>
-    <mergeCell ref="R92:W92"/>
-    <mergeCell ref="R93:W93"/>
-    <mergeCell ref="R94:W94"/>
-    <mergeCell ref="Z117:AE117"/>
-    <mergeCell ref="Z118:AE118"/>
-    <mergeCell ref="J117:O117"/>
-    <mergeCell ref="J118:O118"/>
-    <mergeCell ref="J119:O119"/>
-    <mergeCell ref="J120:O120"/>
-    <mergeCell ref="R20:W20"/>
-    <mergeCell ref="R21:W21"/>
-    <mergeCell ref="R22:W22"/>
-    <mergeCell ref="R23:W23"/>
-    <mergeCell ref="R24:W24"/>
-    <mergeCell ref="R44:W44"/>
-    <mergeCell ref="J92:O92"/>
-    <mergeCell ref="J93:O93"/>
-    <mergeCell ref="J94:O94"/>
-    <mergeCell ref="J95:O95"/>
-    <mergeCell ref="J96:O96"/>
-    <mergeCell ref="J116:O116"/>
-    <mergeCell ref="J48:O48"/>
-    <mergeCell ref="J68:O68"/>
-    <mergeCell ref="J69:O69"/>
-    <mergeCell ref="J70:O70"/>
-    <mergeCell ref="J71:O71"/>
-    <mergeCell ref="J72:O72"/>
-    <mergeCell ref="R117:W117"/>
-    <mergeCell ref="R118:W118"/>
-    <mergeCell ref="B120:G120"/>
-    <mergeCell ref="J20:O20"/>
-    <mergeCell ref="J21:O21"/>
-    <mergeCell ref="J22:O22"/>
-    <mergeCell ref="J23:O23"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="J44:O44"/>
-    <mergeCell ref="J45:O45"/>
-    <mergeCell ref="J46:O46"/>
-    <mergeCell ref="J47:O47"/>
-    <mergeCell ref="B95:G95"/>
-    <mergeCell ref="B96:G96"/>
-    <mergeCell ref="B116:G116"/>
-    <mergeCell ref="B117:G117"/>
-    <mergeCell ref="B118:G118"/>
-    <mergeCell ref="B119:G119"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="B92:G92"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="B94:G94"/>
+    <mergeCell ref="BF23:BK23"/>
+    <mergeCell ref="AX24:BC24"/>
+    <mergeCell ref="BF24:BK24"/>
+    <mergeCell ref="AX69:BC69"/>
+    <mergeCell ref="BF69:BK69"/>
+    <mergeCell ref="AX70:BC70"/>
+    <mergeCell ref="BF70:BK70"/>
+    <mergeCell ref="AX71:BC71"/>
+    <mergeCell ref="BF71:BK71"/>
+    <mergeCell ref="AX47:BC47"/>
+    <mergeCell ref="BF47:BK47"/>
+    <mergeCell ref="AX48:BC48"/>
+    <mergeCell ref="BF48:BK48"/>
+    <mergeCell ref="AX68:BC68"/>
+    <mergeCell ref="BF68:BK68"/>
+    <mergeCell ref="AX94:BC94"/>
+    <mergeCell ref="BF94:BK94"/>
+    <mergeCell ref="AX95:BC95"/>
+    <mergeCell ref="BF95:BK95"/>
+    <mergeCell ref="AX96:BC96"/>
+    <mergeCell ref="BF96:BK96"/>
+    <mergeCell ref="AX72:BC72"/>
+    <mergeCell ref="BF72:BK72"/>
+    <mergeCell ref="AX92:BC92"/>
+    <mergeCell ref="BF92:BK92"/>
+    <mergeCell ref="AX93:BC93"/>
+    <mergeCell ref="BF93:BK93"/>
+    <mergeCell ref="AX119:BC119"/>
+    <mergeCell ref="BF119:BK119"/>
+    <mergeCell ref="AX120:BC120"/>
+    <mergeCell ref="BF120:BK120"/>
+    <mergeCell ref="AX116:BC116"/>
+    <mergeCell ref="BF116:BK116"/>
+    <mergeCell ref="AX117:BC117"/>
+    <mergeCell ref="BF117:BK117"/>
+    <mergeCell ref="AX118:BC118"/>
+    <mergeCell ref="BF118:BK118"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
@@ -30619,7 +30619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -50512,6 +50512,198 @@
     </row>
   </sheetData>
   <mergeCells count="208">
+    <mergeCell ref="AW1:BC1"/>
+    <mergeCell ref="BE1:BK1"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="J20:O20"/>
+    <mergeCell ref="R20:W20"/>
+    <mergeCell ref="Z20:AE20"/>
+    <mergeCell ref="AH20:AM20"/>
+    <mergeCell ref="AP20:AU20"/>
+    <mergeCell ref="AX20:BC20"/>
+    <mergeCell ref="BF20:BK20"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="Y1:AE1"/>
+    <mergeCell ref="AG1:AM1"/>
+    <mergeCell ref="AO1:AU1"/>
+    <mergeCell ref="AX21:BC21"/>
+    <mergeCell ref="BF21:BK21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="J22:O22"/>
+    <mergeCell ref="R22:W22"/>
+    <mergeCell ref="Z22:AE22"/>
+    <mergeCell ref="AH22:AM22"/>
+    <mergeCell ref="AP22:AU22"/>
+    <mergeCell ref="AX22:BC22"/>
+    <mergeCell ref="BF22:BK22"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="J21:O21"/>
+    <mergeCell ref="R21:W21"/>
+    <mergeCell ref="Z21:AE21"/>
+    <mergeCell ref="AH21:AM21"/>
+    <mergeCell ref="AP21:AU21"/>
+    <mergeCell ref="AX23:BC23"/>
+    <mergeCell ref="BF23:BK23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="R24:W24"/>
+    <mergeCell ref="Z24:AE24"/>
+    <mergeCell ref="AH24:AM24"/>
+    <mergeCell ref="AP24:AU24"/>
+    <mergeCell ref="AX24:BC24"/>
+    <mergeCell ref="BF24:BK24"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="J23:O23"/>
+    <mergeCell ref="R23:W23"/>
+    <mergeCell ref="Z23:AE23"/>
+    <mergeCell ref="AH23:AM23"/>
+    <mergeCell ref="AP23:AU23"/>
+    <mergeCell ref="AX44:BC44"/>
+    <mergeCell ref="BF44:BK44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="J45:O45"/>
+    <mergeCell ref="R45:W45"/>
+    <mergeCell ref="Z45:AE45"/>
+    <mergeCell ref="AH45:AM45"/>
+    <mergeCell ref="AP45:AU45"/>
+    <mergeCell ref="AX45:BC45"/>
+    <mergeCell ref="BF45:BK45"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="J44:O44"/>
+    <mergeCell ref="R44:W44"/>
+    <mergeCell ref="Z44:AE44"/>
+    <mergeCell ref="AH44:AM44"/>
+    <mergeCell ref="AP44:AU44"/>
+    <mergeCell ref="AX46:BC46"/>
+    <mergeCell ref="BF46:BK46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="J47:O47"/>
+    <mergeCell ref="R47:W47"/>
+    <mergeCell ref="Z47:AE47"/>
+    <mergeCell ref="AH47:AM47"/>
+    <mergeCell ref="AP47:AU47"/>
+    <mergeCell ref="AX47:BC47"/>
+    <mergeCell ref="BF47:BK47"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="J46:O46"/>
+    <mergeCell ref="R46:W46"/>
+    <mergeCell ref="Z46:AE46"/>
+    <mergeCell ref="AH46:AM46"/>
+    <mergeCell ref="AP46:AU46"/>
+    <mergeCell ref="AX48:BC48"/>
+    <mergeCell ref="BF48:BK48"/>
+    <mergeCell ref="B68:G68"/>
+    <mergeCell ref="J68:O68"/>
+    <mergeCell ref="R68:W68"/>
+    <mergeCell ref="Z68:AE68"/>
+    <mergeCell ref="AH68:AM68"/>
+    <mergeCell ref="AP68:AU68"/>
+    <mergeCell ref="AX68:BC68"/>
+    <mergeCell ref="BF68:BK68"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="J48:O48"/>
+    <mergeCell ref="R48:W48"/>
+    <mergeCell ref="Z48:AE48"/>
+    <mergeCell ref="AH48:AM48"/>
+    <mergeCell ref="AP48:AU48"/>
+    <mergeCell ref="AX69:BC69"/>
+    <mergeCell ref="BF69:BK69"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="J70:O70"/>
+    <mergeCell ref="R70:W70"/>
+    <mergeCell ref="Z70:AE70"/>
+    <mergeCell ref="AH70:AM70"/>
+    <mergeCell ref="AP70:AU70"/>
+    <mergeCell ref="AX70:BC70"/>
+    <mergeCell ref="BF70:BK70"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="J69:O69"/>
+    <mergeCell ref="R69:W69"/>
+    <mergeCell ref="Z69:AE69"/>
+    <mergeCell ref="AH69:AM69"/>
+    <mergeCell ref="AP69:AU69"/>
+    <mergeCell ref="AX71:BC71"/>
+    <mergeCell ref="BF71:BK71"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="J72:O72"/>
+    <mergeCell ref="R72:W72"/>
+    <mergeCell ref="Z72:AE72"/>
+    <mergeCell ref="AH72:AM72"/>
+    <mergeCell ref="AP72:AU72"/>
+    <mergeCell ref="AX72:BC72"/>
+    <mergeCell ref="BF72:BK72"/>
+    <mergeCell ref="B71:G71"/>
+    <mergeCell ref="J71:O71"/>
+    <mergeCell ref="R71:W71"/>
+    <mergeCell ref="Z71:AE71"/>
+    <mergeCell ref="AH71:AM71"/>
+    <mergeCell ref="AP71:AU71"/>
+    <mergeCell ref="AX92:BC92"/>
+    <mergeCell ref="BF92:BK92"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="J93:O93"/>
+    <mergeCell ref="R93:W93"/>
+    <mergeCell ref="Z93:AE93"/>
+    <mergeCell ref="AH93:AM93"/>
+    <mergeCell ref="AP93:AU93"/>
+    <mergeCell ref="AX93:BC93"/>
+    <mergeCell ref="BF93:BK93"/>
+    <mergeCell ref="B92:G92"/>
+    <mergeCell ref="J92:O92"/>
+    <mergeCell ref="R92:W92"/>
+    <mergeCell ref="Z92:AE92"/>
+    <mergeCell ref="AH92:AM92"/>
+    <mergeCell ref="AP92:AU92"/>
+    <mergeCell ref="AX94:BC94"/>
+    <mergeCell ref="BF94:BK94"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="J95:O95"/>
+    <mergeCell ref="R95:W95"/>
+    <mergeCell ref="Z95:AE95"/>
+    <mergeCell ref="AH95:AM95"/>
+    <mergeCell ref="AP95:AU95"/>
+    <mergeCell ref="AX95:BC95"/>
+    <mergeCell ref="BF95:BK95"/>
+    <mergeCell ref="B94:G94"/>
+    <mergeCell ref="J94:O94"/>
+    <mergeCell ref="R94:W94"/>
+    <mergeCell ref="Z94:AE94"/>
+    <mergeCell ref="AH94:AM94"/>
+    <mergeCell ref="AP94:AU94"/>
+    <mergeCell ref="AX96:BC96"/>
+    <mergeCell ref="BF96:BK96"/>
+    <mergeCell ref="B116:G116"/>
+    <mergeCell ref="J116:O116"/>
+    <mergeCell ref="R116:W116"/>
+    <mergeCell ref="Z116:AE116"/>
+    <mergeCell ref="AH116:AM116"/>
+    <mergeCell ref="AP116:AU116"/>
+    <mergeCell ref="AX116:BC116"/>
+    <mergeCell ref="BF116:BK116"/>
+    <mergeCell ref="B96:G96"/>
+    <mergeCell ref="J96:O96"/>
+    <mergeCell ref="R96:W96"/>
+    <mergeCell ref="Z96:AE96"/>
+    <mergeCell ref="AH96:AM96"/>
+    <mergeCell ref="AP96:AU96"/>
+    <mergeCell ref="AX117:BC117"/>
+    <mergeCell ref="BF117:BK117"/>
+    <mergeCell ref="B118:G118"/>
+    <mergeCell ref="J118:O118"/>
+    <mergeCell ref="R118:W118"/>
+    <mergeCell ref="Z118:AE118"/>
+    <mergeCell ref="AH118:AM118"/>
+    <mergeCell ref="AP118:AU118"/>
+    <mergeCell ref="AX118:BC118"/>
+    <mergeCell ref="BF118:BK118"/>
+    <mergeCell ref="B117:G117"/>
+    <mergeCell ref="J117:O117"/>
+    <mergeCell ref="R117:W117"/>
+    <mergeCell ref="Z117:AE117"/>
+    <mergeCell ref="AH117:AM117"/>
+    <mergeCell ref="AP117:AU117"/>
     <mergeCell ref="AX119:BC119"/>
     <mergeCell ref="BF119:BK119"/>
     <mergeCell ref="B120:G120"/>
@@ -50528,198 +50720,6 @@
     <mergeCell ref="Z119:AE119"/>
     <mergeCell ref="AH119:AM119"/>
     <mergeCell ref="AP119:AU119"/>
-    <mergeCell ref="AX117:BC117"/>
-    <mergeCell ref="BF117:BK117"/>
-    <mergeCell ref="B118:G118"/>
-    <mergeCell ref="J118:O118"/>
-    <mergeCell ref="R118:W118"/>
-    <mergeCell ref="Z118:AE118"/>
-    <mergeCell ref="AH118:AM118"/>
-    <mergeCell ref="AP118:AU118"/>
-    <mergeCell ref="AX118:BC118"/>
-    <mergeCell ref="BF118:BK118"/>
-    <mergeCell ref="B117:G117"/>
-    <mergeCell ref="J117:O117"/>
-    <mergeCell ref="R117:W117"/>
-    <mergeCell ref="Z117:AE117"/>
-    <mergeCell ref="AH117:AM117"/>
-    <mergeCell ref="AP117:AU117"/>
-    <mergeCell ref="AX96:BC96"/>
-    <mergeCell ref="BF96:BK96"/>
-    <mergeCell ref="B116:G116"/>
-    <mergeCell ref="J116:O116"/>
-    <mergeCell ref="R116:W116"/>
-    <mergeCell ref="Z116:AE116"/>
-    <mergeCell ref="AH116:AM116"/>
-    <mergeCell ref="AP116:AU116"/>
-    <mergeCell ref="AX116:BC116"/>
-    <mergeCell ref="BF116:BK116"/>
-    <mergeCell ref="B96:G96"/>
-    <mergeCell ref="J96:O96"/>
-    <mergeCell ref="R96:W96"/>
-    <mergeCell ref="Z96:AE96"/>
-    <mergeCell ref="AH96:AM96"/>
-    <mergeCell ref="AP96:AU96"/>
-    <mergeCell ref="AX94:BC94"/>
-    <mergeCell ref="BF94:BK94"/>
-    <mergeCell ref="B95:G95"/>
-    <mergeCell ref="J95:O95"/>
-    <mergeCell ref="R95:W95"/>
-    <mergeCell ref="Z95:AE95"/>
-    <mergeCell ref="AH95:AM95"/>
-    <mergeCell ref="AP95:AU95"/>
-    <mergeCell ref="AX95:BC95"/>
-    <mergeCell ref="BF95:BK95"/>
-    <mergeCell ref="B94:G94"/>
-    <mergeCell ref="J94:O94"/>
-    <mergeCell ref="R94:W94"/>
-    <mergeCell ref="Z94:AE94"/>
-    <mergeCell ref="AH94:AM94"/>
-    <mergeCell ref="AP94:AU94"/>
-    <mergeCell ref="AX92:BC92"/>
-    <mergeCell ref="BF92:BK92"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="J93:O93"/>
-    <mergeCell ref="R93:W93"/>
-    <mergeCell ref="Z93:AE93"/>
-    <mergeCell ref="AH93:AM93"/>
-    <mergeCell ref="AP93:AU93"/>
-    <mergeCell ref="AX93:BC93"/>
-    <mergeCell ref="BF93:BK93"/>
-    <mergeCell ref="B92:G92"/>
-    <mergeCell ref="J92:O92"/>
-    <mergeCell ref="R92:W92"/>
-    <mergeCell ref="Z92:AE92"/>
-    <mergeCell ref="AH92:AM92"/>
-    <mergeCell ref="AP92:AU92"/>
-    <mergeCell ref="AX71:BC71"/>
-    <mergeCell ref="BF71:BK71"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="J72:O72"/>
-    <mergeCell ref="R72:W72"/>
-    <mergeCell ref="Z72:AE72"/>
-    <mergeCell ref="AH72:AM72"/>
-    <mergeCell ref="AP72:AU72"/>
-    <mergeCell ref="AX72:BC72"/>
-    <mergeCell ref="BF72:BK72"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="J71:O71"/>
-    <mergeCell ref="R71:W71"/>
-    <mergeCell ref="Z71:AE71"/>
-    <mergeCell ref="AH71:AM71"/>
-    <mergeCell ref="AP71:AU71"/>
-    <mergeCell ref="AX69:BC69"/>
-    <mergeCell ref="BF69:BK69"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="J70:O70"/>
-    <mergeCell ref="R70:W70"/>
-    <mergeCell ref="Z70:AE70"/>
-    <mergeCell ref="AH70:AM70"/>
-    <mergeCell ref="AP70:AU70"/>
-    <mergeCell ref="AX70:BC70"/>
-    <mergeCell ref="BF70:BK70"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="J69:O69"/>
-    <mergeCell ref="R69:W69"/>
-    <mergeCell ref="Z69:AE69"/>
-    <mergeCell ref="AH69:AM69"/>
-    <mergeCell ref="AP69:AU69"/>
-    <mergeCell ref="AX48:BC48"/>
-    <mergeCell ref="BF48:BK48"/>
-    <mergeCell ref="B68:G68"/>
-    <mergeCell ref="J68:O68"/>
-    <mergeCell ref="R68:W68"/>
-    <mergeCell ref="Z68:AE68"/>
-    <mergeCell ref="AH68:AM68"/>
-    <mergeCell ref="AP68:AU68"/>
-    <mergeCell ref="AX68:BC68"/>
-    <mergeCell ref="BF68:BK68"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="J48:O48"/>
-    <mergeCell ref="R48:W48"/>
-    <mergeCell ref="Z48:AE48"/>
-    <mergeCell ref="AH48:AM48"/>
-    <mergeCell ref="AP48:AU48"/>
-    <mergeCell ref="AX46:BC46"/>
-    <mergeCell ref="BF46:BK46"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="J47:O47"/>
-    <mergeCell ref="R47:W47"/>
-    <mergeCell ref="Z47:AE47"/>
-    <mergeCell ref="AH47:AM47"/>
-    <mergeCell ref="AP47:AU47"/>
-    <mergeCell ref="AX47:BC47"/>
-    <mergeCell ref="BF47:BK47"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="J46:O46"/>
-    <mergeCell ref="R46:W46"/>
-    <mergeCell ref="Z46:AE46"/>
-    <mergeCell ref="AH46:AM46"/>
-    <mergeCell ref="AP46:AU46"/>
-    <mergeCell ref="AX44:BC44"/>
-    <mergeCell ref="BF44:BK44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="J45:O45"/>
-    <mergeCell ref="R45:W45"/>
-    <mergeCell ref="Z45:AE45"/>
-    <mergeCell ref="AH45:AM45"/>
-    <mergeCell ref="AP45:AU45"/>
-    <mergeCell ref="AX45:BC45"/>
-    <mergeCell ref="BF45:BK45"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="J44:O44"/>
-    <mergeCell ref="R44:W44"/>
-    <mergeCell ref="Z44:AE44"/>
-    <mergeCell ref="AH44:AM44"/>
-    <mergeCell ref="AP44:AU44"/>
-    <mergeCell ref="AX23:BC23"/>
-    <mergeCell ref="BF23:BK23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="R24:W24"/>
-    <mergeCell ref="Z24:AE24"/>
-    <mergeCell ref="AH24:AM24"/>
-    <mergeCell ref="AP24:AU24"/>
-    <mergeCell ref="AX24:BC24"/>
-    <mergeCell ref="BF24:BK24"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="J23:O23"/>
-    <mergeCell ref="R23:W23"/>
-    <mergeCell ref="Z23:AE23"/>
-    <mergeCell ref="AH23:AM23"/>
-    <mergeCell ref="AP23:AU23"/>
-    <mergeCell ref="AX21:BC21"/>
-    <mergeCell ref="BF21:BK21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="J22:O22"/>
-    <mergeCell ref="R22:W22"/>
-    <mergeCell ref="Z22:AE22"/>
-    <mergeCell ref="AH22:AM22"/>
-    <mergeCell ref="AP22:AU22"/>
-    <mergeCell ref="AX22:BC22"/>
-    <mergeCell ref="BF22:BK22"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="J21:O21"/>
-    <mergeCell ref="R21:W21"/>
-    <mergeCell ref="Z21:AE21"/>
-    <mergeCell ref="AH21:AM21"/>
-    <mergeCell ref="AP21:AU21"/>
-    <mergeCell ref="AW1:BC1"/>
-    <mergeCell ref="BE1:BK1"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="J20:O20"/>
-    <mergeCell ref="R20:W20"/>
-    <mergeCell ref="Z20:AE20"/>
-    <mergeCell ref="AH20:AM20"/>
-    <mergeCell ref="AP20:AU20"/>
-    <mergeCell ref="AX20:BC20"/>
-    <mergeCell ref="BF20:BK20"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="Y1:AE1"/>
-    <mergeCell ref="AG1:AM1"/>
-    <mergeCell ref="AO1:AU1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -70606,6 +70606,198 @@
     </row>
   </sheetData>
   <mergeCells count="208">
+    <mergeCell ref="AW1:BC1"/>
+    <mergeCell ref="BE1:BK1"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="J20:O20"/>
+    <mergeCell ref="R20:W20"/>
+    <mergeCell ref="Z20:AE20"/>
+    <mergeCell ref="AH20:AM20"/>
+    <mergeCell ref="AP20:AU20"/>
+    <mergeCell ref="AX20:BC20"/>
+    <mergeCell ref="BF20:BK20"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="Y1:AE1"/>
+    <mergeCell ref="AG1:AM1"/>
+    <mergeCell ref="AO1:AU1"/>
+    <mergeCell ref="AX21:BC21"/>
+    <mergeCell ref="BF21:BK21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="J22:O22"/>
+    <mergeCell ref="R22:W22"/>
+    <mergeCell ref="Z22:AE22"/>
+    <mergeCell ref="AH22:AM22"/>
+    <mergeCell ref="AP22:AU22"/>
+    <mergeCell ref="AX22:BC22"/>
+    <mergeCell ref="BF22:BK22"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="J21:O21"/>
+    <mergeCell ref="R21:W21"/>
+    <mergeCell ref="Z21:AE21"/>
+    <mergeCell ref="AH21:AM21"/>
+    <mergeCell ref="AP21:AU21"/>
+    <mergeCell ref="AX23:BC23"/>
+    <mergeCell ref="BF23:BK23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="R24:W24"/>
+    <mergeCell ref="Z24:AE24"/>
+    <mergeCell ref="AH24:AM24"/>
+    <mergeCell ref="AP24:AU24"/>
+    <mergeCell ref="AX24:BC24"/>
+    <mergeCell ref="BF24:BK24"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="J23:O23"/>
+    <mergeCell ref="R23:W23"/>
+    <mergeCell ref="Z23:AE23"/>
+    <mergeCell ref="AH23:AM23"/>
+    <mergeCell ref="AP23:AU23"/>
+    <mergeCell ref="AX44:BC44"/>
+    <mergeCell ref="BF44:BK44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="J45:O45"/>
+    <mergeCell ref="R45:W45"/>
+    <mergeCell ref="Z45:AE45"/>
+    <mergeCell ref="AH45:AM45"/>
+    <mergeCell ref="AP45:AU45"/>
+    <mergeCell ref="AX45:BC45"/>
+    <mergeCell ref="BF45:BK45"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="J44:O44"/>
+    <mergeCell ref="R44:W44"/>
+    <mergeCell ref="Z44:AE44"/>
+    <mergeCell ref="AH44:AM44"/>
+    <mergeCell ref="AP44:AU44"/>
+    <mergeCell ref="AX46:BC46"/>
+    <mergeCell ref="BF46:BK46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="J47:O47"/>
+    <mergeCell ref="R47:W47"/>
+    <mergeCell ref="Z47:AE47"/>
+    <mergeCell ref="AH47:AM47"/>
+    <mergeCell ref="AP47:AU47"/>
+    <mergeCell ref="AX47:BC47"/>
+    <mergeCell ref="BF47:BK47"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="J46:O46"/>
+    <mergeCell ref="R46:W46"/>
+    <mergeCell ref="Z46:AE46"/>
+    <mergeCell ref="AH46:AM46"/>
+    <mergeCell ref="AP46:AU46"/>
+    <mergeCell ref="AX48:BC48"/>
+    <mergeCell ref="BF48:BK48"/>
+    <mergeCell ref="B68:G68"/>
+    <mergeCell ref="J68:O68"/>
+    <mergeCell ref="R68:W68"/>
+    <mergeCell ref="Z68:AE68"/>
+    <mergeCell ref="AH68:AM68"/>
+    <mergeCell ref="AP68:AU68"/>
+    <mergeCell ref="AX68:BC68"/>
+    <mergeCell ref="BF68:BK68"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="J48:O48"/>
+    <mergeCell ref="R48:W48"/>
+    <mergeCell ref="Z48:AE48"/>
+    <mergeCell ref="AH48:AM48"/>
+    <mergeCell ref="AP48:AU48"/>
+    <mergeCell ref="AX69:BC69"/>
+    <mergeCell ref="BF69:BK69"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="J70:O70"/>
+    <mergeCell ref="R70:W70"/>
+    <mergeCell ref="Z70:AE70"/>
+    <mergeCell ref="AH70:AM70"/>
+    <mergeCell ref="AP70:AU70"/>
+    <mergeCell ref="AX70:BC70"/>
+    <mergeCell ref="BF70:BK70"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="J69:O69"/>
+    <mergeCell ref="R69:W69"/>
+    <mergeCell ref="Z69:AE69"/>
+    <mergeCell ref="AH69:AM69"/>
+    <mergeCell ref="AP69:AU69"/>
+    <mergeCell ref="AX71:BC71"/>
+    <mergeCell ref="BF71:BK71"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="J72:O72"/>
+    <mergeCell ref="R72:W72"/>
+    <mergeCell ref="Z72:AE72"/>
+    <mergeCell ref="AH72:AM72"/>
+    <mergeCell ref="AP72:AU72"/>
+    <mergeCell ref="AX72:BC72"/>
+    <mergeCell ref="BF72:BK72"/>
+    <mergeCell ref="B71:G71"/>
+    <mergeCell ref="J71:O71"/>
+    <mergeCell ref="R71:W71"/>
+    <mergeCell ref="Z71:AE71"/>
+    <mergeCell ref="AH71:AM71"/>
+    <mergeCell ref="AP71:AU71"/>
+    <mergeCell ref="AX92:BC92"/>
+    <mergeCell ref="BF92:BK92"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="J93:O93"/>
+    <mergeCell ref="R93:W93"/>
+    <mergeCell ref="Z93:AE93"/>
+    <mergeCell ref="AH93:AM93"/>
+    <mergeCell ref="AP93:AU93"/>
+    <mergeCell ref="AX93:BC93"/>
+    <mergeCell ref="BF93:BK93"/>
+    <mergeCell ref="B92:G92"/>
+    <mergeCell ref="J92:O92"/>
+    <mergeCell ref="R92:W92"/>
+    <mergeCell ref="Z92:AE92"/>
+    <mergeCell ref="AH92:AM92"/>
+    <mergeCell ref="AP92:AU92"/>
+    <mergeCell ref="AX94:BC94"/>
+    <mergeCell ref="BF94:BK94"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="J95:O95"/>
+    <mergeCell ref="R95:W95"/>
+    <mergeCell ref="Z95:AE95"/>
+    <mergeCell ref="AH95:AM95"/>
+    <mergeCell ref="AP95:AU95"/>
+    <mergeCell ref="AX95:BC95"/>
+    <mergeCell ref="BF95:BK95"/>
+    <mergeCell ref="B94:G94"/>
+    <mergeCell ref="J94:O94"/>
+    <mergeCell ref="R94:W94"/>
+    <mergeCell ref="Z94:AE94"/>
+    <mergeCell ref="AH94:AM94"/>
+    <mergeCell ref="AP94:AU94"/>
+    <mergeCell ref="AX96:BC96"/>
+    <mergeCell ref="BF96:BK96"/>
+    <mergeCell ref="B116:G116"/>
+    <mergeCell ref="J116:O116"/>
+    <mergeCell ref="R116:W116"/>
+    <mergeCell ref="Z116:AE116"/>
+    <mergeCell ref="AH116:AM116"/>
+    <mergeCell ref="AP116:AU116"/>
+    <mergeCell ref="AX116:BC116"/>
+    <mergeCell ref="BF116:BK116"/>
+    <mergeCell ref="B96:G96"/>
+    <mergeCell ref="J96:O96"/>
+    <mergeCell ref="R96:W96"/>
+    <mergeCell ref="Z96:AE96"/>
+    <mergeCell ref="AH96:AM96"/>
+    <mergeCell ref="AP96:AU96"/>
+    <mergeCell ref="AX117:BC117"/>
+    <mergeCell ref="BF117:BK117"/>
+    <mergeCell ref="B118:G118"/>
+    <mergeCell ref="J118:O118"/>
+    <mergeCell ref="R118:W118"/>
+    <mergeCell ref="Z118:AE118"/>
+    <mergeCell ref="AH118:AM118"/>
+    <mergeCell ref="AP118:AU118"/>
+    <mergeCell ref="AX118:BC118"/>
+    <mergeCell ref="BF118:BK118"/>
+    <mergeCell ref="B117:G117"/>
+    <mergeCell ref="J117:O117"/>
+    <mergeCell ref="R117:W117"/>
+    <mergeCell ref="Z117:AE117"/>
+    <mergeCell ref="AH117:AM117"/>
+    <mergeCell ref="AP117:AU117"/>
     <mergeCell ref="AX119:BC119"/>
     <mergeCell ref="BF119:BK119"/>
     <mergeCell ref="B120:G120"/>
@@ -70622,198 +70814,6 @@
     <mergeCell ref="Z119:AE119"/>
     <mergeCell ref="AH119:AM119"/>
     <mergeCell ref="AP119:AU119"/>
-    <mergeCell ref="AX117:BC117"/>
-    <mergeCell ref="BF117:BK117"/>
-    <mergeCell ref="B118:G118"/>
-    <mergeCell ref="J118:O118"/>
-    <mergeCell ref="R118:W118"/>
-    <mergeCell ref="Z118:AE118"/>
-    <mergeCell ref="AH118:AM118"/>
-    <mergeCell ref="AP118:AU118"/>
-    <mergeCell ref="AX118:BC118"/>
-    <mergeCell ref="BF118:BK118"/>
-    <mergeCell ref="B117:G117"/>
-    <mergeCell ref="J117:O117"/>
-    <mergeCell ref="R117:W117"/>
-    <mergeCell ref="Z117:AE117"/>
-    <mergeCell ref="AH117:AM117"/>
-    <mergeCell ref="AP117:AU117"/>
-    <mergeCell ref="AX96:BC96"/>
-    <mergeCell ref="BF96:BK96"/>
-    <mergeCell ref="B116:G116"/>
-    <mergeCell ref="J116:O116"/>
-    <mergeCell ref="R116:W116"/>
-    <mergeCell ref="Z116:AE116"/>
-    <mergeCell ref="AH116:AM116"/>
-    <mergeCell ref="AP116:AU116"/>
-    <mergeCell ref="AX116:BC116"/>
-    <mergeCell ref="BF116:BK116"/>
-    <mergeCell ref="B96:G96"/>
-    <mergeCell ref="J96:O96"/>
-    <mergeCell ref="R96:W96"/>
-    <mergeCell ref="Z96:AE96"/>
-    <mergeCell ref="AH96:AM96"/>
-    <mergeCell ref="AP96:AU96"/>
-    <mergeCell ref="AX94:BC94"/>
-    <mergeCell ref="BF94:BK94"/>
-    <mergeCell ref="B95:G95"/>
-    <mergeCell ref="J95:O95"/>
-    <mergeCell ref="R95:W95"/>
-    <mergeCell ref="Z95:AE95"/>
-    <mergeCell ref="AH95:AM95"/>
-    <mergeCell ref="AP95:AU95"/>
-    <mergeCell ref="AX95:BC95"/>
-    <mergeCell ref="BF95:BK95"/>
-    <mergeCell ref="B94:G94"/>
-    <mergeCell ref="J94:O94"/>
-    <mergeCell ref="R94:W94"/>
-    <mergeCell ref="Z94:AE94"/>
-    <mergeCell ref="AH94:AM94"/>
-    <mergeCell ref="AP94:AU94"/>
-    <mergeCell ref="AX92:BC92"/>
-    <mergeCell ref="BF92:BK92"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="J93:O93"/>
-    <mergeCell ref="R93:W93"/>
-    <mergeCell ref="Z93:AE93"/>
-    <mergeCell ref="AH93:AM93"/>
-    <mergeCell ref="AP93:AU93"/>
-    <mergeCell ref="AX93:BC93"/>
-    <mergeCell ref="BF93:BK93"/>
-    <mergeCell ref="B92:G92"/>
-    <mergeCell ref="J92:O92"/>
-    <mergeCell ref="R92:W92"/>
-    <mergeCell ref="Z92:AE92"/>
-    <mergeCell ref="AH92:AM92"/>
-    <mergeCell ref="AP92:AU92"/>
-    <mergeCell ref="AX71:BC71"/>
-    <mergeCell ref="BF71:BK71"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="J72:O72"/>
-    <mergeCell ref="R72:W72"/>
-    <mergeCell ref="Z72:AE72"/>
-    <mergeCell ref="AH72:AM72"/>
-    <mergeCell ref="AP72:AU72"/>
-    <mergeCell ref="AX72:BC72"/>
-    <mergeCell ref="BF72:BK72"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="J71:O71"/>
-    <mergeCell ref="R71:W71"/>
-    <mergeCell ref="Z71:AE71"/>
-    <mergeCell ref="AH71:AM71"/>
-    <mergeCell ref="AP71:AU71"/>
-    <mergeCell ref="AX69:BC69"/>
-    <mergeCell ref="BF69:BK69"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="J70:O70"/>
-    <mergeCell ref="R70:W70"/>
-    <mergeCell ref="Z70:AE70"/>
-    <mergeCell ref="AH70:AM70"/>
-    <mergeCell ref="AP70:AU70"/>
-    <mergeCell ref="AX70:BC70"/>
-    <mergeCell ref="BF70:BK70"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="J69:O69"/>
-    <mergeCell ref="R69:W69"/>
-    <mergeCell ref="Z69:AE69"/>
-    <mergeCell ref="AH69:AM69"/>
-    <mergeCell ref="AP69:AU69"/>
-    <mergeCell ref="AX48:BC48"/>
-    <mergeCell ref="BF48:BK48"/>
-    <mergeCell ref="B68:G68"/>
-    <mergeCell ref="J68:O68"/>
-    <mergeCell ref="R68:W68"/>
-    <mergeCell ref="Z68:AE68"/>
-    <mergeCell ref="AH68:AM68"/>
-    <mergeCell ref="AP68:AU68"/>
-    <mergeCell ref="AX68:BC68"/>
-    <mergeCell ref="BF68:BK68"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="J48:O48"/>
-    <mergeCell ref="R48:W48"/>
-    <mergeCell ref="Z48:AE48"/>
-    <mergeCell ref="AH48:AM48"/>
-    <mergeCell ref="AP48:AU48"/>
-    <mergeCell ref="AX46:BC46"/>
-    <mergeCell ref="BF46:BK46"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="J47:O47"/>
-    <mergeCell ref="R47:W47"/>
-    <mergeCell ref="Z47:AE47"/>
-    <mergeCell ref="AH47:AM47"/>
-    <mergeCell ref="AP47:AU47"/>
-    <mergeCell ref="AX47:BC47"/>
-    <mergeCell ref="BF47:BK47"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="J46:O46"/>
-    <mergeCell ref="R46:W46"/>
-    <mergeCell ref="Z46:AE46"/>
-    <mergeCell ref="AH46:AM46"/>
-    <mergeCell ref="AP46:AU46"/>
-    <mergeCell ref="AX44:BC44"/>
-    <mergeCell ref="BF44:BK44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="J45:O45"/>
-    <mergeCell ref="R45:W45"/>
-    <mergeCell ref="Z45:AE45"/>
-    <mergeCell ref="AH45:AM45"/>
-    <mergeCell ref="AP45:AU45"/>
-    <mergeCell ref="AX45:BC45"/>
-    <mergeCell ref="BF45:BK45"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="J44:O44"/>
-    <mergeCell ref="R44:W44"/>
-    <mergeCell ref="Z44:AE44"/>
-    <mergeCell ref="AH44:AM44"/>
-    <mergeCell ref="AP44:AU44"/>
-    <mergeCell ref="AX23:BC23"/>
-    <mergeCell ref="BF23:BK23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="R24:W24"/>
-    <mergeCell ref="Z24:AE24"/>
-    <mergeCell ref="AH24:AM24"/>
-    <mergeCell ref="AP24:AU24"/>
-    <mergeCell ref="AX24:BC24"/>
-    <mergeCell ref="BF24:BK24"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="J23:O23"/>
-    <mergeCell ref="R23:W23"/>
-    <mergeCell ref="Z23:AE23"/>
-    <mergeCell ref="AH23:AM23"/>
-    <mergeCell ref="AP23:AU23"/>
-    <mergeCell ref="AX21:BC21"/>
-    <mergeCell ref="BF21:BK21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="J22:O22"/>
-    <mergeCell ref="R22:W22"/>
-    <mergeCell ref="Z22:AE22"/>
-    <mergeCell ref="AH22:AM22"/>
-    <mergeCell ref="AP22:AU22"/>
-    <mergeCell ref="AX22:BC22"/>
-    <mergeCell ref="BF22:BK22"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="J21:O21"/>
-    <mergeCell ref="R21:W21"/>
-    <mergeCell ref="Z21:AE21"/>
-    <mergeCell ref="AH21:AM21"/>
-    <mergeCell ref="AP21:AU21"/>
-    <mergeCell ref="AW1:BC1"/>
-    <mergeCell ref="BE1:BK1"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="J20:O20"/>
-    <mergeCell ref="R20:W20"/>
-    <mergeCell ref="Z20:AE20"/>
-    <mergeCell ref="AH20:AM20"/>
-    <mergeCell ref="AP20:AU20"/>
-    <mergeCell ref="AX20:BC20"/>
-    <mergeCell ref="BF20:BK20"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="Y1:AE1"/>
-    <mergeCell ref="AG1:AM1"/>
-    <mergeCell ref="AO1:AU1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
* Remove some old deprecated assets * add prototype models for testing F1 and RS-68 geometry and gimbals * add part .cfg files for several RS-68 and F1 cluster setups * add part .cfg file for testing clustering of stock engines (LV-N x4 cluster) * add 0.625m tanks (only basic nosecones at the moment) * add 1.875m tanks (only basic nosecones at the moment) * add 6.25m tanks (only basic nosecones at the moment) * update naming on all tanks to more clearly specify their diameter * update breaking force and torque on all tanks to more sane values given their size and masses * re-arrange layout of config files in /data folder * fix up crash bug with custom fuel tank as root part * Move SC-C parts to 'deprecated' status.  They will be removed in full with the next release.
</commit_message>
<xml_diff>
--- a/GameData/SSTU/Parts/Parts-MassCalc.xlsx
+++ b/GameData/SSTU/Parts/Parts-MassCalc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="parts" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="dV-Calc-SC-B" sheetId="3" r:id="rId3"/>
     <sheet name="FuelTypes" sheetId="6" r:id="rId4"/>
     <sheet name="Resource Data" sheetId="5" r:id="rId5"/>
+    <sheet name="TankVolumes" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2058" uniqueCount="318">
   <si>
     <t>Part</t>
   </si>
@@ -865,6 +866,114 @@
   <si>
     <t>Entry Cost</t>
   </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Nose1</t>
+  </si>
+  <si>
+    <t>Nose2</t>
+  </si>
+  <si>
+    <t>Nose3</t>
+  </si>
+  <si>
+    <t>Nose4</t>
+  </si>
+  <si>
+    <t>Nose5</t>
+  </si>
+  <si>
+    <t>2-1-flat</t>
+  </si>
+  <si>
+    <t>2-1-long</t>
+  </si>
+  <si>
+    <t>2-1-short</t>
+  </si>
+  <si>
+    <t>4-3-flat</t>
+  </si>
+  <si>
+    <t>4-3-long</t>
+  </si>
+  <si>
+    <t>4-3-short</t>
+  </si>
+  <si>
+    <t>2-1-x2</t>
+  </si>
+  <si>
+    <t>2-1-x3</t>
+  </si>
+  <si>
+    <t>2-1-x4</t>
+  </si>
+  <si>
+    <t>1-1-x2</t>
+  </si>
+  <si>
+    <t>1-1-x3</t>
+  </si>
+  <si>
+    <t>1-1-x4</t>
+  </si>
+  <si>
+    <t>4-3-x2</t>
+  </si>
+  <si>
+    <t>4-3-x3</t>
+  </si>
+  <si>
+    <t>4-3-x4</t>
+  </si>
+  <si>
+    <t>3-2-flat</t>
+  </si>
+  <si>
+    <t>3-2-short</t>
+  </si>
+  <si>
+    <t>3-2-long</t>
+  </si>
+  <si>
+    <t>3-1-flat</t>
+  </si>
+  <si>
+    <t>3-1-long</t>
+  </si>
+  <si>
+    <t>3-1-short</t>
+  </si>
 </sst>
 </file>
 
@@ -1188,7 +1297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1251,6 +1360,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1558,8 +1668,8 @@
   <dimension ref="A1:AC301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47197,7 +47307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
@@ -69245,4 +69355,1597 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="11" width="12" style="34" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="34">
+        <v>6.25</v>
+      </c>
+      <c r="C1" s="34">
+        <v>5</v>
+      </c>
+      <c r="D1" s="34">
+        <v>3.75</v>
+      </c>
+      <c r="E1" s="34">
+        <v>2.5</v>
+      </c>
+      <c r="F1" s="34">
+        <v>1.875</v>
+      </c>
+      <c r="G1" s="34">
+        <v>1.25</v>
+      </c>
+      <c r="H1" s="34">
+        <v>0.625</v>
+      </c>
+      <c r="I1" s="34">
+        <v>6.61</v>
+      </c>
+      <c r="J1" s="34">
+        <v>8.4</v>
+      </c>
+      <c r="K1" s="34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" s="34">
+        <f>B1/C1</f>
+        <v>1.25</v>
+      </c>
+      <c r="C2" s="34">
+        <v>1</v>
+      </c>
+      <c r="D2" s="34">
+        <f>D1/$C$1</f>
+        <v>0.75</v>
+      </c>
+      <c r="E2" s="34">
+        <f t="shared" ref="E2:H2" si="0">E1/$C$1</f>
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="34">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+      <c r="G2" s="34">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="H2" s="34">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="I2" s="34">
+        <f t="shared" ref="I2" si="1">I1/$C$1</f>
+        <v>1.3220000000000001</v>
+      </c>
+      <c r="J2" s="34">
+        <f t="shared" ref="J2" si="2">J1/$C$1</f>
+        <v>1.6800000000000002</v>
+      </c>
+      <c r="K2" s="34">
+        <f t="shared" ref="K2" si="3">K1/$C$1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B3" s="34">
+        <f>B$2*B$2*B$2*$C3</f>
+        <v>191.40625</v>
+      </c>
+      <c r="C3" s="34">
+        <v>98</v>
+      </c>
+      <c r="D3" s="34">
+        <f>D$2*D$2*D$2*$C3</f>
+        <v>41.34375</v>
+      </c>
+      <c r="E3" s="34">
+        <f t="shared" ref="E3:K3" si="4">E$2*E$2*E$2*$C3</f>
+        <v>12.25</v>
+      </c>
+      <c r="F3" s="34">
+        <f t="shared" si="4"/>
+        <v>5.16796875</v>
+      </c>
+      <c r="G3" s="34">
+        <f t="shared" si="4"/>
+        <v>1.53125</v>
+      </c>
+      <c r="H3" s="34">
+        <f t="shared" si="4"/>
+        <v>0.19140625</v>
+      </c>
+      <c r="I3" s="34">
+        <f t="shared" si="4"/>
+        <v>226.42294830400004</v>
+      </c>
+      <c r="J3" s="34">
+        <f t="shared" si="4"/>
+        <v>464.67993600000011</v>
+      </c>
+      <c r="K3" s="34">
+        <f t="shared" si="4"/>
+        <v>784</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B4" s="34">
+        <f t="shared" ref="B4:K36" si="5">B$2*B$2*B$2*$C4</f>
+        <v>382.8125</v>
+      </c>
+      <c r="C4" s="34">
+        <v>196</v>
+      </c>
+      <c r="D4" s="34">
+        <f t="shared" si="5"/>
+        <v>82.6875</v>
+      </c>
+      <c r="E4" s="34">
+        <f t="shared" si="5"/>
+        <v>24.5</v>
+      </c>
+      <c r="F4" s="34">
+        <f t="shared" si="5"/>
+        <v>10.3359375</v>
+      </c>
+      <c r="G4" s="34">
+        <f t="shared" si="5"/>
+        <v>3.0625</v>
+      </c>
+      <c r="H4" s="34">
+        <f t="shared" si="5"/>
+        <v>0.3828125</v>
+      </c>
+      <c r="I4" s="34">
+        <f t="shared" si="5"/>
+        <v>452.84589660800009</v>
+      </c>
+      <c r="J4" s="34">
+        <f t="shared" si="5"/>
+        <v>929.35987200000022</v>
+      </c>
+      <c r="K4" s="34">
+        <f t="shared" si="5"/>
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" s="34">
+        <f t="shared" si="5"/>
+        <v>574.21875</v>
+      </c>
+      <c r="C5" s="34">
+        <v>294</v>
+      </c>
+      <c r="D5" s="34">
+        <f t="shared" si="5"/>
+        <v>124.03125</v>
+      </c>
+      <c r="E5" s="34">
+        <f t="shared" si="5"/>
+        <v>36.75</v>
+      </c>
+      <c r="F5" s="34">
+        <f t="shared" si="5"/>
+        <v>15.50390625</v>
+      </c>
+      <c r="G5" s="34">
+        <f t="shared" si="5"/>
+        <v>4.59375</v>
+      </c>
+      <c r="H5" s="34">
+        <f t="shared" si="5"/>
+        <v>0.57421875</v>
+      </c>
+      <c r="I5" s="34">
+        <f t="shared" si="5"/>
+        <v>679.26884491200019</v>
+      </c>
+      <c r="J5" s="34">
+        <f t="shared" si="5"/>
+        <v>1394.0398080000002</v>
+      </c>
+      <c r="K5" s="34">
+        <f t="shared" si="5"/>
+        <v>2352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6" s="34">
+        <f t="shared" si="5"/>
+        <v>765.625</v>
+      </c>
+      <c r="C6" s="34">
+        <v>392</v>
+      </c>
+      <c r="D6" s="34">
+        <f t="shared" si="5"/>
+        <v>165.375</v>
+      </c>
+      <c r="E6" s="34">
+        <f t="shared" si="5"/>
+        <v>49</v>
+      </c>
+      <c r="F6" s="34">
+        <f t="shared" si="5"/>
+        <v>20.671875</v>
+      </c>
+      <c r="G6" s="34">
+        <f t="shared" si="5"/>
+        <v>6.125</v>
+      </c>
+      <c r="H6" s="34">
+        <f t="shared" si="5"/>
+        <v>0.765625</v>
+      </c>
+      <c r="I6" s="34">
+        <f t="shared" si="5"/>
+        <v>905.69179321600018</v>
+      </c>
+      <c r="J6" s="34">
+        <f t="shared" si="5"/>
+        <v>1858.7197440000004</v>
+      </c>
+      <c r="K6" s="34">
+        <f t="shared" si="5"/>
+        <v>3136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>287</v>
+      </c>
+      <c r="B7" s="34">
+        <f t="shared" si="5"/>
+        <v>957.03125</v>
+      </c>
+      <c r="C7" s="34">
+        <v>490</v>
+      </c>
+      <c r="D7" s="34">
+        <f t="shared" si="5"/>
+        <v>206.71875</v>
+      </c>
+      <c r="E7" s="34">
+        <f t="shared" si="5"/>
+        <v>61.25</v>
+      </c>
+      <c r="F7" s="34">
+        <f t="shared" si="5"/>
+        <v>25.83984375</v>
+      </c>
+      <c r="G7" s="34">
+        <f t="shared" si="5"/>
+        <v>7.65625</v>
+      </c>
+      <c r="H7" s="34">
+        <f t="shared" si="5"/>
+        <v>0.95703125</v>
+      </c>
+      <c r="I7" s="34">
+        <f t="shared" si="5"/>
+        <v>1132.1147415200003</v>
+      </c>
+      <c r="J7" s="34">
+        <f t="shared" si="5"/>
+        <v>2323.3996800000004</v>
+      </c>
+      <c r="K7" s="34">
+        <f t="shared" si="5"/>
+        <v>3920</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B8" s="34">
+        <f t="shared" si="5"/>
+        <v>1152.34375</v>
+      </c>
+      <c r="C8" s="34">
+        <v>590</v>
+      </c>
+      <c r="D8" s="34">
+        <f t="shared" si="5"/>
+        <v>248.90625</v>
+      </c>
+      <c r="E8" s="34">
+        <f t="shared" si="5"/>
+        <v>73.75</v>
+      </c>
+      <c r="F8" s="34">
+        <f t="shared" si="5"/>
+        <v>31.11328125</v>
+      </c>
+      <c r="G8" s="34">
+        <f t="shared" si="5"/>
+        <v>9.21875</v>
+      </c>
+      <c r="H8" s="34">
+        <f t="shared" si="5"/>
+        <v>1.15234375</v>
+      </c>
+      <c r="I8" s="34">
+        <f t="shared" si="5"/>
+        <v>1363.1585663200003</v>
+      </c>
+      <c r="J8" s="34">
+        <f t="shared" si="5"/>
+        <v>2797.5628800000004</v>
+      </c>
+      <c r="K8" s="34">
+        <f t="shared" si="5"/>
+        <v>4720</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" s="34">
+        <f t="shared" si="5"/>
+        <v>1341.796875</v>
+      </c>
+      <c r="C9" s="34">
+        <v>687</v>
+      </c>
+      <c r="D9" s="34">
+        <f t="shared" si="5"/>
+        <v>289.828125</v>
+      </c>
+      <c r="E9" s="34">
+        <f t="shared" si="5"/>
+        <v>85.875</v>
+      </c>
+      <c r="F9" s="34">
+        <f t="shared" si="5"/>
+        <v>36.228515625</v>
+      </c>
+      <c r="G9" s="34">
+        <f t="shared" si="5"/>
+        <v>10.734375</v>
+      </c>
+      <c r="H9" s="34">
+        <f t="shared" si="5"/>
+        <v>1.341796875</v>
+      </c>
+      <c r="I9" s="34">
+        <f t="shared" si="5"/>
+        <v>1587.2710763760003</v>
+      </c>
+      <c r="J9" s="34">
+        <f t="shared" si="5"/>
+        <v>3257.5011840000006</v>
+      </c>
+      <c r="K9" s="34">
+        <f t="shared" si="5"/>
+        <v>5496</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B10" s="34">
+        <f t="shared" si="5"/>
+        <v>1533.203125</v>
+      </c>
+      <c r="C10" s="34">
+        <v>785</v>
+      </c>
+      <c r="D10" s="34">
+        <f t="shared" si="5"/>
+        <v>331.171875</v>
+      </c>
+      <c r="E10" s="34">
+        <f t="shared" si="5"/>
+        <v>98.125</v>
+      </c>
+      <c r="F10" s="34">
+        <f t="shared" si="5"/>
+        <v>41.396484375</v>
+      </c>
+      <c r="G10" s="34">
+        <f t="shared" si="5"/>
+        <v>12.265625</v>
+      </c>
+      <c r="H10" s="34">
+        <f t="shared" si="5"/>
+        <v>1.533203125</v>
+      </c>
+      <c r="I10" s="34">
+        <f t="shared" si="5"/>
+        <v>1813.6940246800004</v>
+      </c>
+      <c r="J10" s="34">
+        <f t="shared" si="5"/>
+        <v>3722.1811200000006</v>
+      </c>
+      <c r="K10" s="34">
+        <f t="shared" si="5"/>
+        <v>6280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>292</v>
+      </c>
+      <c r="B11" s="34">
+        <f t="shared" si="5"/>
+        <v>129.8828125</v>
+      </c>
+      <c r="C11" s="34">
+        <v>66.5</v>
+      </c>
+      <c r="D11" s="34">
+        <f t="shared" si="5"/>
+        <v>28.0546875</v>
+      </c>
+      <c r="E11" s="34">
+        <f t="shared" si="5"/>
+        <v>8.3125</v>
+      </c>
+      <c r="F11" s="34">
+        <f t="shared" si="5"/>
+        <v>3.5068359375</v>
+      </c>
+      <c r="G11" s="34">
+        <f t="shared" si="5"/>
+        <v>1.0390625</v>
+      </c>
+      <c r="H11" s="34">
+        <f t="shared" si="5"/>
+        <v>0.1298828125</v>
+      </c>
+      <c r="I11" s="34">
+        <f t="shared" si="5"/>
+        <v>153.64414349200004</v>
+      </c>
+      <c r="J11" s="34">
+        <f t="shared" si="5"/>
+        <v>315.31852800000007</v>
+      </c>
+      <c r="K11" s="34">
+        <f t="shared" si="5"/>
+        <v>532</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>293</v>
+      </c>
+      <c r="B12" s="34">
+        <f t="shared" si="5"/>
+        <v>168.9453125</v>
+      </c>
+      <c r="C12" s="34">
+        <v>86.5</v>
+      </c>
+      <c r="D12" s="34">
+        <f t="shared" si="5"/>
+        <v>36.4921875</v>
+      </c>
+      <c r="E12" s="34">
+        <f t="shared" si="5"/>
+        <v>10.8125</v>
+      </c>
+      <c r="F12" s="34">
+        <f t="shared" si="5"/>
+        <v>4.5615234375</v>
+      </c>
+      <c r="G12" s="34">
+        <f t="shared" si="5"/>
+        <v>1.3515625</v>
+      </c>
+      <c r="H12" s="34">
+        <f t="shared" si="5"/>
+        <v>0.1689453125</v>
+      </c>
+      <c r="I12" s="34">
+        <f t="shared" si="5"/>
+        <v>199.85290845200004</v>
+      </c>
+      <c r="J12" s="34">
+        <f t="shared" si="5"/>
+        <v>410.1511680000001</v>
+      </c>
+      <c r="K12" s="34">
+        <f t="shared" si="5"/>
+        <v>692</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>294</v>
+      </c>
+      <c r="B13" s="34">
+        <f t="shared" si="5"/>
+        <v>66.40625</v>
+      </c>
+      <c r="C13" s="34">
+        <v>34</v>
+      </c>
+      <c r="D13" s="34">
+        <f t="shared" si="5"/>
+        <v>14.34375</v>
+      </c>
+      <c r="E13" s="34">
+        <f t="shared" si="5"/>
+        <v>4.25</v>
+      </c>
+      <c r="F13" s="34">
+        <f t="shared" si="5"/>
+        <v>1.79296875</v>
+      </c>
+      <c r="G13" s="34">
+        <f t="shared" si="5"/>
+        <v>0.53125</v>
+      </c>
+      <c r="H13" s="34">
+        <f t="shared" si="5"/>
+        <v>6.640625E-2</v>
+      </c>
+      <c r="I13" s="34">
+        <f t="shared" si="5"/>
+        <v>78.554900432000011</v>
+      </c>
+      <c r="J13" s="34">
+        <f t="shared" si="5"/>
+        <v>161.21548800000002</v>
+      </c>
+      <c r="K13" s="34">
+        <f t="shared" si="5"/>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>295</v>
+      </c>
+      <c r="B14" s="34">
+        <f t="shared" si="5"/>
+        <v>48.828125</v>
+      </c>
+      <c r="C14" s="34">
+        <v>25</v>
+      </c>
+      <c r="D14" s="34">
+        <f t="shared" si="5"/>
+        <v>10.546875</v>
+      </c>
+      <c r="E14" s="34">
+        <f t="shared" si="5"/>
+        <v>3.125</v>
+      </c>
+      <c r="F14" s="34">
+        <f t="shared" si="5"/>
+        <v>1.318359375</v>
+      </c>
+      <c r="G14" s="34">
+        <f t="shared" si="5"/>
+        <v>0.390625</v>
+      </c>
+      <c r="H14" s="34">
+        <f t="shared" si="5"/>
+        <v>4.8828125E-2</v>
+      </c>
+      <c r="I14" s="34">
+        <f t="shared" si="5"/>
+        <v>57.76095620000001</v>
+      </c>
+      <c r="J14" s="34">
+        <f t="shared" si="5"/>
+        <v>118.54080000000002</v>
+      </c>
+      <c r="K14" s="34">
+        <f t="shared" si="5"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>296</v>
+      </c>
+      <c r="B15" s="34">
+        <f t="shared" si="5"/>
+        <v>118.1640625</v>
+      </c>
+      <c r="C15" s="34">
+        <v>60.5</v>
+      </c>
+      <c r="D15" s="34">
+        <f t="shared" si="5"/>
+        <v>25.5234375</v>
+      </c>
+      <c r="E15" s="34">
+        <f t="shared" si="5"/>
+        <v>7.5625</v>
+      </c>
+      <c r="F15" s="34">
+        <f t="shared" si="5"/>
+        <v>3.1904296875</v>
+      </c>
+      <c r="G15" s="34">
+        <f t="shared" si="5"/>
+        <v>0.9453125</v>
+      </c>
+      <c r="H15" s="34">
+        <f t="shared" si="5"/>
+        <v>0.1181640625</v>
+      </c>
+      <c r="I15" s="34">
+        <f t="shared" si="5"/>
+        <v>139.78151400400003</v>
+      </c>
+      <c r="J15" s="34">
+        <f t="shared" si="5"/>
+        <v>286.86873600000007</v>
+      </c>
+      <c r="K15" s="34">
+        <f t="shared" si="5"/>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>297</v>
+      </c>
+      <c r="B16" s="34">
+        <f t="shared" si="5"/>
+        <v>7.8125</v>
+      </c>
+      <c r="C16" s="34">
+        <v>4</v>
+      </c>
+      <c r="D16" s="34">
+        <f t="shared" si="5"/>
+        <v>1.6875</v>
+      </c>
+      <c r="E16" s="34">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="34">
+        <f t="shared" si="5"/>
+        <v>0.2109375</v>
+      </c>
+      <c r="G16" s="34">
+        <f t="shared" si="5"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H16" s="34">
+        <f t="shared" si="5"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="I16" s="34">
+        <f t="shared" si="5"/>
+        <v>9.2417529920000021</v>
+      </c>
+      <c r="J16" s="34">
+        <f t="shared" si="5"/>
+        <v>18.966528000000004</v>
+      </c>
+      <c r="K16" s="34">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>298</v>
+      </c>
+      <c r="B17" s="34">
+        <f t="shared" si="5"/>
+        <v>108.3984375</v>
+      </c>
+      <c r="C17" s="34">
+        <v>55.5</v>
+      </c>
+      <c r="D17" s="34">
+        <f t="shared" si="5"/>
+        <v>23.4140625</v>
+      </c>
+      <c r="E17" s="34">
+        <f t="shared" si="5"/>
+        <v>6.9375</v>
+      </c>
+      <c r="F17" s="34">
+        <f t="shared" si="5"/>
+        <v>2.9267578125</v>
+      </c>
+      <c r="G17" s="34">
+        <f t="shared" si="5"/>
+        <v>0.8671875</v>
+      </c>
+      <c r="H17" s="34">
+        <f t="shared" si="5"/>
+        <v>0.1083984375</v>
+      </c>
+      <c r="I17" s="34">
+        <f t="shared" si="5"/>
+        <v>128.22932276400002</v>
+      </c>
+      <c r="J17" s="34">
+        <f t="shared" si="5"/>
+        <v>263.16057600000005</v>
+      </c>
+      <c r="K17" s="34">
+        <f t="shared" si="5"/>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>299</v>
+      </c>
+      <c r="B18" s="34">
+        <f t="shared" si="5"/>
+        <v>52.734375</v>
+      </c>
+      <c r="C18" s="34">
+        <v>27</v>
+      </c>
+      <c r="D18" s="34">
+        <f t="shared" si="5"/>
+        <v>11.390625</v>
+      </c>
+      <c r="E18" s="34">
+        <f t="shared" si="5"/>
+        <v>3.375</v>
+      </c>
+      <c r="F18" s="34">
+        <f t="shared" si="5"/>
+        <v>1.423828125</v>
+      </c>
+      <c r="G18" s="34">
+        <f t="shared" si="5"/>
+        <v>0.421875</v>
+      </c>
+      <c r="H18" s="34">
+        <f t="shared" si="5"/>
+        <v>5.2734375E-2</v>
+      </c>
+      <c r="I18" s="34">
+        <f t="shared" si="5"/>
+        <v>62.381832696000018</v>
+      </c>
+      <c r="J18" s="34">
+        <f t="shared" si="5"/>
+        <v>128.02406400000004</v>
+      </c>
+      <c r="K18" s="34">
+        <f t="shared" si="5"/>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>300</v>
+      </c>
+      <c r="B19" s="34">
+        <f t="shared" si="5"/>
+        <v>9.765625</v>
+      </c>
+      <c r="C19" s="34">
+        <v>5</v>
+      </c>
+      <c r="D19" s="34">
+        <f t="shared" si="5"/>
+        <v>2.109375</v>
+      </c>
+      <c r="E19" s="34">
+        <f t="shared" si="5"/>
+        <v>0.625</v>
+      </c>
+      <c r="F19" s="34">
+        <f t="shared" si="5"/>
+        <v>0.263671875</v>
+      </c>
+      <c r="G19" s="34">
+        <f t="shared" si="5"/>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="H19" s="34">
+        <f t="shared" si="5"/>
+        <v>9.765625E-3</v>
+      </c>
+      <c r="I19" s="34">
+        <f t="shared" si="5"/>
+        <v>11.552191240000003</v>
+      </c>
+      <c r="J19" s="34">
+        <f t="shared" si="5"/>
+        <v>23.708160000000007</v>
+      </c>
+      <c r="K19" s="34">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>301</v>
+      </c>
+      <c r="B20" s="34">
+        <f t="shared" si="5"/>
+        <v>142.578125</v>
+      </c>
+      <c r="C20" s="34">
+        <v>73</v>
+      </c>
+      <c r="D20" s="34">
+        <f t="shared" si="5"/>
+        <v>30.796875</v>
+      </c>
+      <c r="E20" s="34">
+        <f t="shared" si="5"/>
+        <v>9.125</v>
+      </c>
+      <c r="F20" s="34">
+        <f t="shared" si="5"/>
+        <v>3.849609375</v>
+      </c>
+      <c r="G20" s="34">
+        <f t="shared" si="5"/>
+        <v>1.140625</v>
+      </c>
+      <c r="H20" s="34">
+        <f t="shared" si="5"/>
+        <v>0.142578125</v>
+      </c>
+      <c r="I20" s="34">
+        <f t="shared" si="5"/>
+        <v>168.66199210400003</v>
+      </c>
+      <c r="J20" s="34">
+        <f t="shared" si="5"/>
+        <v>346.13913600000006</v>
+      </c>
+      <c r="K20" s="34">
+        <f t="shared" si="5"/>
+        <v>584</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>302</v>
+      </c>
+      <c r="B21" s="34">
+        <f t="shared" si="5"/>
+        <v>70.3125</v>
+      </c>
+      <c r="C21" s="34">
+        <v>36</v>
+      </c>
+      <c r="D21" s="34">
+        <f t="shared" si="5"/>
+        <v>15.1875</v>
+      </c>
+      <c r="E21" s="34">
+        <f t="shared" si="5"/>
+        <v>4.5</v>
+      </c>
+      <c r="F21" s="34">
+        <f t="shared" si="5"/>
+        <v>1.8984375</v>
+      </c>
+      <c r="G21" s="34">
+        <f t="shared" si="5"/>
+        <v>0.5625</v>
+      </c>
+      <c r="H21" s="34">
+        <f t="shared" si="5"/>
+        <v>7.03125E-2</v>
+      </c>
+      <c r="I21" s="34">
+        <f t="shared" si="5"/>
+        <v>83.175776928000019</v>
+      </c>
+      <c r="J21" s="34">
+        <f t="shared" si="5"/>
+        <v>170.69875200000004</v>
+      </c>
+      <c r="K21" s="34">
+        <f t="shared" si="5"/>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>315</v>
+      </c>
+      <c r="B22" s="34">
+        <f t="shared" ref="B22:B24" si="6">B$2*B$2*B$2*$C22</f>
+        <v>9.66796875</v>
+      </c>
+      <c r="C22" s="34">
+        <v>4.95</v>
+      </c>
+      <c r="D22" s="34">
+        <f t="shared" ref="D22:D36" si="7">D$2*D$2*D$2*$C22</f>
+        <v>2.0882812500000001</v>
+      </c>
+      <c r="E22" s="34">
+        <f t="shared" ref="D22:K24" si="8">E$2*E$2*E$2*$C22</f>
+        <v>0.61875000000000002</v>
+      </c>
+      <c r="F22" s="34">
+        <f t="shared" si="8"/>
+        <v>0.26103515625000001</v>
+      </c>
+      <c r="G22" s="34">
+        <f t="shared" si="8"/>
+        <v>7.7343750000000003E-2</v>
+      </c>
+      <c r="H22" s="34">
+        <f t="shared" si="8"/>
+        <v>9.6679687500000003E-3</v>
+      </c>
+      <c r="I22" s="34">
+        <f t="shared" si="8"/>
+        <v>11.436669327600002</v>
+      </c>
+      <c r="J22" s="34">
+        <f t="shared" si="8"/>
+        <v>23.471078400000007</v>
+      </c>
+      <c r="K22" s="34">
+        <f t="shared" si="8"/>
+        <v>39.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>316</v>
+      </c>
+      <c r="B23" s="34">
+        <f t="shared" si="6"/>
+        <v>89.94140625</v>
+      </c>
+      <c r="C23" s="34">
+        <v>46.05</v>
+      </c>
+      <c r="D23" s="34">
+        <f t="shared" si="7"/>
+        <v>19.427343749999999</v>
+      </c>
+      <c r="E23" s="34">
+        <f t="shared" si="8"/>
+        <v>5.7562499999999996</v>
+      </c>
+      <c r="F23" s="34">
+        <f t="shared" si="8"/>
+        <v>2.4284179687499998</v>
+      </c>
+      <c r="G23" s="34">
+        <f t="shared" si="8"/>
+        <v>0.71953124999999996</v>
+      </c>
+      <c r="H23" s="34">
+        <f t="shared" si="8"/>
+        <v>8.9941406249999994E-2</v>
+      </c>
+      <c r="I23" s="34">
+        <f t="shared" si="8"/>
+        <v>106.39568132040002</v>
+      </c>
+      <c r="J23" s="34">
+        <f t="shared" si="8"/>
+        <v>218.35215360000004</v>
+      </c>
+      <c r="K23" s="34">
+        <f t="shared" si="8"/>
+        <v>368.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>317</v>
+      </c>
+      <c r="B24" s="34">
+        <f t="shared" si="6"/>
+        <v>46.2890625</v>
+      </c>
+      <c r="C24" s="34">
+        <v>23.7</v>
+      </c>
+      <c r="D24" s="34">
+        <f t="shared" si="7"/>
+        <v>9.9984374999999996</v>
+      </c>
+      <c r="E24" s="34">
+        <f t="shared" si="8"/>
+        <v>2.9624999999999999</v>
+      </c>
+      <c r="F24" s="34">
+        <f t="shared" si="8"/>
+        <v>1.2498046875</v>
+      </c>
+      <c r="G24" s="34">
+        <f t="shared" si="8"/>
+        <v>0.37031249999999999</v>
+      </c>
+      <c r="H24" s="34">
+        <f t="shared" si="8"/>
+        <v>4.6289062499999999E-2</v>
+      </c>
+      <c r="I24" s="34">
+        <f t="shared" si="8"/>
+        <v>54.757386477600008</v>
+      </c>
+      <c r="J24" s="34">
+        <f t="shared" si="8"/>
+        <v>112.37667840000002</v>
+      </c>
+      <c r="K24" s="34">
+        <f t="shared" si="8"/>
+        <v>189.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>312</v>
+      </c>
+      <c r="B25" s="34">
+        <f t="shared" si="5"/>
+        <v>13.671875</v>
+      </c>
+      <c r="C25" s="34">
+        <v>7</v>
+      </c>
+      <c r="D25" s="34">
+        <f t="shared" si="7"/>
+        <v>2.953125</v>
+      </c>
+      <c r="E25" s="34">
+        <f t="shared" si="5"/>
+        <v>0.875</v>
+      </c>
+      <c r="F25" s="34">
+        <f t="shared" si="5"/>
+        <v>0.369140625</v>
+      </c>
+      <c r="G25" s="34">
+        <f t="shared" si="5"/>
+        <v>0.109375</v>
+      </c>
+      <c r="H25" s="34">
+        <f t="shared" si="5"/>
+        <v>1.3671875E-2</v>
+      </c>
+      <c r="I25" s="34">
+        <f t="shared" si="5"/>
+        <v>16.173067736000004</v>
+      </c>
+      <c r="J25" s="34">
+        <f t="shared" si="5"/>
+        <v>33.191424000000005</v>
+      </c>
+      <c r="K25" s="34">
+        <f t="shared" si="5"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>313</v>
+      </c>
+      <c r="B26" s="34">
+        <f t="shared" si="5"/>
+        <v>130.95703125</v>
+      </c>
+      <c r="C26" s="34">
+        <v>67.05</v>
+      </c>
+      <c r="D26" s="34">
+        <f t="shared" si="7"/>
+        <v>28.286718749999999</v>
+      </c>
+      <c r="E26" s="34">
+        <f t="shared" si="5"/>
+        <v>8.3812499999999996</v>
+      </c>
+      <c r="F26" s="34">
+        <f t="shared" ref="F26:K27" si="9">F$2*F$2*F$2*$C26</f>
+        <v>3.5358398437499998</v>
+      </c>
+      <c r="G26" s="34">
+        <f t="shared" si="9"/>
+        <v>1.04765625</v>
+      </c>
+      <c r="H26" s="34">
+        <f t="shared" si="9"/>
+        <v>0.13095703124999999</v>
+      </c>
+      <c r="I26" s="34">
+        <f t="shared" si="9"/>
+        <v>154.91488452840002</v>
+      </c>
+      <c r="J26" s="34">
+        <f t="shared" si="9"/>
+        <v>317.92642560000007</v>
+      </c>
+      <c r="K26" s="34">
+        <f t="shared" si="9"/>
+        <v>536.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>314</v>
+      </c>
+      <c r="B27" s="34">
+        <f t="shared" ref="B27" si="10">B$2*B$2*B$2*$C27</f>
+        <v>64.35546875</v>
+      </c>
+      <c r="C27" s="34">
+        <v>32.950000000000003</v>
+      </c>
+      <c r="D27" s="34">
+        <f t="shared" si="7"/>
+        <v>13.900781250000001</v>
+      </c>
+      <c r="E27" s="34">
+        <f t="shared" ref="D27:E27" si="11">E$2*E$2*E$2*$C27</f>
+        <v>4.1187500000000004</v>
+      </c>
+      <c r="F27" s="34">
+        <f t="shared" si="9"/>
+        <v>1.7375976562500002</v>
+      </c>
+      <c r="G27" s="34">
+        <f t="shared" si="9"/>
+        <v>0.51484375000000004</v>
+      </c>
+      <c r="H27" s="34">
+        <f t="shared" si="9"/>
+        <v>6.4355468750000006E-2</v>
+      </c>
+      <c r="I27" s="34">
+        <f t="shared" si="9"/>
+        <v>76.12894027160003</v>
+      </c>
+      <c r="J27" s="34">
+        <f t="shared" si="9"/>
+        <v>156.23677440000006</v>
+      </c>
+      <c r="K27" s="34">
+        <f t="shared" si="9"/>
+        <v>263.60000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>306</v>
+      </c>
+      <c r="B28" s="34">
+        <f t="shared" si="5"/>
+        <v>148.4375</v>
+      </c>
+      <c r="C28" s="34">
+        <v>76</v>
+      </c>
+      <c r="D28" s="34">
+        <f t="shared" si="7"/>
+        <v>32.0625</v>
+      </c>
+      <c r="E28" s="34">
+        <f t="shared" si="5"/>
+        <v>9.5</v>
+      </c>
+      <c r="F28" s="34">
+        <f t="shared" si="5"/>
+        <v>4.0078125</v>
+      </c>
+      <c r="G28" s="34">
+        <f t="shared" si="5"/>
+        <v>1.1875</v>
+      </c>
+      <c r="H28" s="34">
+        <f t="shared" si="5"/>
+        <v>0.1484375</v>
+      </c>
+      <c r="I28" s="34">
+        <f t="shared" si="5"/>
+        <v>175.59330684800005</v>
+      </c>
+      <c r="J28" s="34">
+        <f t="shared" si="5"/>
+        <v>360.36403200000007</v>
+      </c>
+      <c r="K28" s="34">
+        <f t="shared" si="5"/>
+        <v>608</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>307</v>
+      </c>
+      <c r="B29" s="34">
+        <f t="shared" si="5"/>
+        <v>195.3125</v>
+      </c>
+      <c r="C29" s="34">
+        <v>100</v>
+      </c>
+      <c r="D29" s="34">
+        <f t="shared" si="7"/>
+        <v>42.1875</v>
+      </c>
+      <c r="E29" s="34">
+        <f t="shared" si="5"/>
+        <v>12.5</v>
+      </c>
+      <c r="F29" s="34">
+        <f t="shared" si="5"/>
+        <v>5.2734375</v>
+      </c>
+      <c r="G29" s="34">
+        <f t="shared" si="5"/>
+        <v>1.5625</v>
+      </c>
+      <c r="H29" s="34">
+        <f t="shared" si="5"/>
+        <v>0.1953125</v>
+      </c>
+      <c r="I29" s="34">
+        <f t="shared" si="5"/>
+        <v>231.04382480000004</v>
+      </c>
+      <c r="J29" s="34">
+        <f t="shared" si="5"/>
+        <v>474.16320000000007</v>
+      </c>
+      <c r="K29" s="34">
+        <f t="shared" si="5"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>308</v>
+      </c>
+      <c r="B30" s="34">
+        <f t="shared" si="5"/>
+        <v>248.046875</v>
+      </c>
+      <c r="C30" s="34">
+        <v>127</v>
+      </c>
+      <c r="D30" s="34">
+        <f t="shared" si="7"/>
+        <v>53.578125</v>
+      </c>
+      <c r="E30" s="34">
+        <f t="shared" si="5"/>
+        <v>15.875</v>
+      </c>
+      <c r="F30" s="34">
+        <f t="shared" si="5"/>
+        <v>6.697265625</v>
+      </c>
+      <c r="G30" s="34">
+        <f t="shared" si="5"/>
+        <v>1.984375</v>
+      </c>
+      <c r="H30" s="34">
+        <f t="shared" si="5"/>
+        <v>0.248046875</v>
+      </c>
+      <c r="I30" s="34">
+        <f t="shared" si="5"/>
+        <v>293.42565749600004</v>
+      </c>
+      <c r="J30" s="34">
+        <f t="shared" si="5"/>
+        <v>602.18726400000014</v>
+      </c>
+      <c r="K30" s="34">
+        <f t="shared" si="5"/>
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>309</v>
+      </c>
+      <c r="B31" s="34">
+        <f t="shared" si="5"/>
+        <v>107.421875</v>
+      </c>
+      <c r="C31" s="34">
+        <v>55</v>
+      </c>
+      <c r="D31" s="34">
+        <f t="shared" si="7"/>
+        <v>23.203125</v>
+      </c>
+      <c r="E31" s="34">
+        <f t="shared" si="5"/>
+        <v>6.875</v>
+      </c>
+      <c r="F31" s="34">
+        <f t="shared" si="5"/>
+        <v>2.900390625</v>
+      </c>
+      <c r="G31" s="34">
+        <f t="shared" si="5"/>
+        <v>0.859375</v>
+      </c>
+      <c r="H31" s="34">
+        <f t="shared" si="5"/>
+        <v>0.107421875</v>
+      </c>
+      <c r="I31" s="34">
+        <f t="shared" si="5"/>
+        <v>127.07410364000003</v>
+      </c>
+      <c r="J31" s="34">
+        <f t="shared" si="5"/>
+        <v>260.78976000000006</v>
+      </c>
+      <c r="K31" s="34">
+        <f t="shared" si="5"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>310</v>
+      </c>
+      <c r="B32" s="34">
+        <f t="shared" si="5"/>
+        <v>135.7421875</v>
+      </c>
+      <c r="C32" s="34">
+        <v>69.5</v>
+      </c>
+      <c r="D32" s="34">
+        <f t="shared" si="7"/>
+        <v>29.3203125</v>
+      </c>
+      <c r="E32" s="34">
+        <f t="shared" si="5"/>
+        <v>8.6875</v>
+      </c>
+      <c r="F32" s="34">
+        <f t="shared" si="5"/>
+        <v>3.6650390625</v>
+      </c>
+      <c r="G32" s="34">
+        <f t="shared" si="5"/>
+        <v>1.0859375</v>
+      </c>
+      <c r="H32" s="34">
+        <f t="shared" si="5"/>
+        <v>0.1357421875</v>
+      </c>
+      <c r="I32" s="34">
+        <f t="shared" si="5"/>
+        <v>160.57545823600003</v>
+      </c>
+      <c r="J32" s="34">
+        <f t="shared" si="5"/>
+        <v>329.54342400000007</v>
+      </c>
+      <c r="K32" s="34">
+        <f t="shared" si="5"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>311</v>
+      </c>
+      <c r="B33" s="34">
+        <f t="shared" si="5"/>
+        <v>166.9921875</v>
+      </c>
+      <c r="C33" s="34">
+        <v>85.5</v>
+      </c>
+      <c r="D33" s="34">
+        <f t="shared" si="7"/>
+        <v>36.0703125</v>
+      </c>
+      <c r="E33" s="34">
+        <f t="shared" si="5"/>
+        <v>10.6875</v>
+      </c>
+      <c r="F33" s="34">
+        <f t="shared" si="5"/>
+        <v>4.5087890625</v>
+      </c>
+      <c r="G33" s="34">
+        <f t="shared" si="5"/>
+        <v>1.3359375</v>
+      </c>
+      <c r="H33" s="34">
+        <f t="shared" si="5"/>
+        <v>0.1669921875</v>
+      </c>
+      <c r="I33" s="34">
+        <f t="shared" si="5"/>
+        <v>197.54247020400004</v>
+      </c>
+      <c r="J33" s="34">
+        <f t="shared" si="5"/>
+        <v>405.40953600000006</v>
+      </c>
+      <c r="K33" s="34">
+        <f t="shared" si="5"/>
+        <v>684</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>303</v>
+      </c>
+      <c r="B34" s="34">
+        <f t="shared" si="5"/>
+        <v>72.265625</v>
+      </c>
+      <c r="C34" s="34">
+        <v>37</v>
+      </c>
+      <c r="D34" s="34">
+        <f t="shared" si="7"/>
+        <v>15.609375</v>
+      </c>
+      <c r="E34" s="34">
+        <f t="shared" si="5"/>
+        <v>4.625</v>
+      </c>
+      <c r="F34" s="34">
+        <f t="shared" si="5"/>
+        <v>1.951171875</v>
+      </c>
+      <c r="G34" s="34">
+        <f t="shared" si="5"/>
+        <v>0.578125</v>
+      </c>
+      <c r="H34" s="34">
+        <f t="shared" si="5"/>
+        <v>7.2265625E-2</v>
+      </c>
+      <c r="I34" s="34">
+        <f t="shared" si="5"/>
+        <v>85.486215176000016</v>
+      </c>
+      <c r="J34" s="34">
+        <f t="shared" si="5"/>
+        <v>175.44038400000002</v>
+      </c>
+      <c r="K34" s="34">
+        <f t="shared" si="5"/>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>304</v>
+      </c>
+      <c r="B35" s="34">
+        <f t="shared" si="5"/>
+        <v>86.9140625</v>
+      </c>
+      <c r="C35" s="34">
+        <v>44.5</v>
+      </c>
+      <c r="D35" s="34">
+        <f t="shared" si="7"/>
+        <v>18.7734375</v>
+      </c>
+      <c r="E35" s="34">
+        <f t="shared" si="5"/>
+        <v>5.5625</v>
+      </c>
+      <c r="F35" s="34">
+        <f t="shared" si="5"/>
+        <v>2.3466796875</v>
+      </c>
+      <c r="G35" s="34">
+        <f t="shared" si="5"/>
+        <v>0.6953125</v>
+      </c>
+      <c r="H35" s="34">
+        <f t="shared" si="5"/>
+        <v>8.69140625E-2</v>
+      </c>
+      <c r="I35" s="34">
+        <f t="shared" si="5"/>
+        <v>102.81450203600002</v>
+      </c>
+      <c r="J35" s="34">
+        <f t="shared" si="5"/>
+        <v>211.00262400000005</v>
+      </c>
+      <c r="K35" s="34">
+        <f t="shared" si="5"/>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>305</v>
+      </c>
+      <c r="B36" s="34">
+        <f t="shared" si="5"/>
+        <v>102.5390625</v>
+      </c>
+      <c r="C36" s="34">
+        <v>52.5</v>
+      </c>
+      <c r="D36" s="34">
+        <f t="shared" si="7"/>
+        <v>22.1484375</v>
+      </c>
+      <c r="E36" s="34">
+        <f t="shared" si="5"/>
+        <v>6.5625</v>
+      </c>
+      <c r="F36" s="34">
+        <f t="shared" si="5"/>
+        <v>2.7685546875</v>
+      </c>
+      <c r="G36" s="34">
+        <f t="shared" si="5"/>
+        <v>0.8203125</v>
+      </c>
+      <c r="H36" s="34">
+        <f t="shared" si="5"/>
+        <v>0.1025390625</v>
+      </c>
+      <c r="I36" s="34">
+        <f t="shared" si="5"/>
+        <v>121.29800802000003</v>
+      </c>
+      <c r="J36" s="34">
+        <f t="shared" si="5"/>
+        <v>248.93568000000005</v>
+      </c>
+      <c r="K36" s="34">
+        <f t="shared" si="5"/>
+        <v>420</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
* CHANGE - Add some vertical scaling to MFT tanks.  YES it does distort the geometry, however for the range of scaling available the distortion is minimal.  If you don't like the distortion, don't use it (I don't like it either). * FIX - SSTUNodeFairing -- 'Jettison Fairing' action group should now properly say 'Jettison' while in editors (previously it said 'disable'). * FIX - SSTUEngineCluster - Fix vertical offset slider values not persisting. * FIX - SSTUModularFuelTank nulref when fairing module not present (MFT-D) * NEW PART - SC-TANK-MFT-D (Soyuz Booster) - Texture is WIP * NEW PART - SC-ADPT-SOYUZ - Tapered nose-adapter for Soyuz-style core tank (applicable to MFT-A and MFT-B) - Texture is WIP * NEW PART - SC-ENG-RD-107 (Placeholder) - Four-chamber engine specialized for use on MFT-D. - Will be replaced by proper RD107/108 in the future (no ETA). * FIX - Add stock effect groups for RBDC and PDC decouplers
</commit_message>
<xml_diff>
--- a/GameData/SSTU/Parts/Parts-MassCalc.xlsx
+++ b/GameData/SSTU/Parts/Parts-MassCalc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="parts" sheetId="1" r:id="rId1"/>
@@ -1533,13 +1533,25 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1554,26 +1566,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1881,7 +1881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M120" sqref="M120"/>
     </sheetView>
@@ -27764,45 +27764,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
       <c r="H1" s="12"/>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
       <c r="P1" s="12"/>
-      <c r="Q1" s="45" t="s">
+      <c r="Q1" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
       <c r="X1" s="12"/>
-      <c r="Y1" s="45" t="s">
+      <c r="Y1" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="45"/>
-      <c r="AC1" s="45"/>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
       <c r="AF1" s="12"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -29513,270 +29513,270 @@
       <c r="A20" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="42">
+      <c r="B20" s="46">
         <f>E19</f>
         <v>0</v>
       </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="44"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
       <c r="H20" s="12"/>
       <c r="I20" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J20" s="42">
+      <c r="J20" s="46">
         <f>M19</f>
         <v>0</v>
       </c>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="44"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="48"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R20" s="42">
+      <c r="R20" s="46">
         <f>U19</f>
         <v>0</v>
       </c>
-      <c r="S20" s="43"/>
-      <c r="T20" s="43"/>
-      <c r="U20" s="43"/>
-      <c r="V20" s="43"/>
-      <c r="W20" s="44"/>
+      <c r="S20" s="47"/>
+      <c r="T20" s="47"/>
+      <c r="U20" s="47"/>
+      <c r="V20" s="47"/>
+      <c r="W20" s="48"/>
       <c r="X20" s="12"/>
       <c r="Y20" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z20" s="42">
+      <c r="Z20" s="46">
         <f>AC19</f>
         <v>0</v>
       </c>
-      <c r="AA20" s="43"/>
-      <c r="AB20" s="43"/>
-      <c r="AC20" s="43"/>
-      <c r="AD20" s="43"/>
-      <c r="AE20" s="44"/>
+      <c r="AA20" s="47"/>
+      <c r="AB20" s="47"/>
+      <c r="AC20" s="47"/>
+      <c r="AD20" s="47"/>
+      <c r="AE20" s="48"/>
       <c r="AF20" s="12"/>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="42">
+      <c r="B21" s="46">
         <f>C19</f>
         <v>0</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="44"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="48"/>
       <c r="H21" s="12"/>
       <c r="I21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J21" s="42">
+      <c r="J21" s="46">
         <f>K19</f>
         <v>0</v>
       </c>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="43"/>
-      <c r="O21" s="44"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="48"/>
       <c r="P21" s="12"/>
       <c r="Q21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R21" s="42">
+      <c r="R21" s="46">
         <f>S19</f>
         <v>0</v>
       </c>
-      <c r="S21" s="43"/>
-      <c r="T21" s="43"/>
-      <c r="U21" s="43"/>
-      <c r="V21" s="43"/>
-      <c r="W21" s="44"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="47"/>
+      <c r="U21" s="47"/>
+      <c r="V21" s="47"/>
+      <c r="W21" s="48"/>
       <c r="X21" s="12"/>
       <c r="Y21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z21" s="42">
+      <c r="Z21" s="46">
         <f>AA19</f>
         <v>0</v>
       </c>
-      <c r="AA21" s="43"/>
-      <c r="AB21" s="43"/>
-      <c r="AC21" s="43"/>
-      <c r="AD21" s="43"/>
-      <c r="AE21" s="44"/>
+      <c r="AA21" s="47"/>
+      <c r="AB21" s="47"/>
+      <c r="AC21" s="47"/>
+      <c r="AD21" s="47"/>
+      <c r="AE21" s="48"/>
       <c r="AF21" s="12"/>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="42">
+      <c r="B22" s="46">
         <f>IFERROR((G19/10/B20),0)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="44"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="48"/>
       <c r="H22" s="12"/>
       <c r="I22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J22" s="42">
+      <c r="J22" s="46">
         <f>IFERROR((O19/10/J20),0)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="43"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="44"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="48"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R22" s="42">
+      <c r="R22" s="46">
         <f>IFERROR((W19/10/R20),0)</f>
         <v>0</v>
       </c>
-      <c r="S22" s="43"/>
-      <c r="T22" s="43"/>
-      <c r="U22" s="43"/>
-      <c r="V22" s="43"/>
-      <c r="W22" s="44"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="47"/>
+      <c r="U22" s="47"/>
+      <c r="V22" s="47"/>
+      <c r="W22" s="48"/>
       <c r="X22" s="12"/>
       <c r="Y22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z22" s="42">
+      <c r="Z22" s="46">
         <f>IFERROR((AE19/10/Z20),0)</f>
         <v>0</v>
       </c>
-      <c r="AA22" s="43"/>
-      <c r="AB22" s="43"/>
-      <c r="AC22" s="43"/>
-      <c r="AD22" s="43"/>
-      <c r="AE22" s="44"/>
+      <c r="AA22" s="47"/>
+      <c r="AB22" s="47"/>
+      <c r="AC22" s="47"/>
+      <c r="AD22" s="47"/>
+      <c r="AE22" s="48"/>
       <c r="AF22" s="12"/>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="42">
+      <c r="B23" s="46">
         <f>IFERROR((9.82 * F19) * LN(B20/C19),0)</f>
         <v>0</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="44"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="48"/>
       <c r="H23" s="12"/>
       <c r="I23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J23" s="42">
+      <c r="J23" s="46">
         <f>IFERROR((9.82 * N19) * LN(J20/K19),0)</f>
         <v>0</v>
       </c>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="44"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="48"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R23" s="42">
+      <c r="R23" s="46">
         <f>IFERROR((9.82 * V19) * LN(R20/S19),0)</f>
         <v>0</v>
       </c>
-      <c r="S23" s="43"/>
-      <c r="T23" s="43"/>
-      <c r="U23" s="43"/>
-      <c r="V23" s="43"/>
-      <c r="W23" s="44"/>
+      <c r="S23" s="47"/>
+      <c r="T23" s="47"/>
+      <c r="U23" s="47"/>
+      <c r="V23" s="47"/>
+      <c r="W23" s="48"/>
       <c r="X23" s="12"/>
       <c r="Y23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z23" s="42">
+      <c r="Z23" s="46">
         <f>IFERROR((9.82 * AD19) * LN(Z20/AA19),0)</f>
         <v>0</v>
       </c>
-      <c r="AA23" s="43"/>
-      <c r="AB23" s="43"/>
-      <c r="AC23" s="43"/>
-      <c r="AD23" s="43"/>
-      <c r="AE23" s="44"/>
+      <c r="AA23" s="47"/>
+      <c r="AB23" s="47"/>
+      <c r="AC23" s="47"/>
+      <c r="AD23" s="47"/>
+      <c r="AE23" s="48"/>
       <c r="AF23" s="12"/>
     </row>
     <row r="24" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="39">
+      <c r="B24" s="50">
         <f>B23</f>
         <v>0</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="41"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="52"/>
       <c r="H24" s="12"/>
       <c r="I24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J24" s="39">
+      <c r="J24" s="50">
         <f>J23</f>
         <v>0</v>
       </c>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="40"/>
-      <c r="O24" s="41"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="52"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R24" s="39">
+      <c r="R24" s="50">
         <f>R23</f>
         <v>0</v>
       </c>
-      <c r="S24" s="40"/>
-      <c r="T24" s="40"/>
-      <c r="U24" s="40"/>
-      <c r="V24" s="40"/>
-      <c r="W24" s="41"/>
+      <c r="S24" s="51"/>
+      <c r="T24" s="51"/>
+      <c r="U24" s="51"/>
+      <c r="V24" s="51"/>
+      <c r="W24" s="52"/>
       <c r="X24" s="12"/>
       <c r="Y24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z24" s="39">
+      <c r="Z24" s="50">
         <f>Z23</f>
         <v>0</v>
       </c>
-      <c r="AA24" s="40"/>
-      <c r="AB24" s="40"/>
-      <c r="AC24" s="40"/>
-      <c r="AD24" s="40"/>
-      <c r="AE24" s="41"/>
+      <c r="AA24" s="51"/>
+      <c r="AB24" s="51"/>
+      <c r="AC24" s="51"/>
+      <c r="AD24" s="51"/>
+      <c r="AE24" s="52"/>
       <c r="AF24" s="12"/>
     </row>
     <row r="25" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31517,270 +31517,270 @@
       <c r="A44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="42">
+      <c r="B44" s="46">
         <f>E43+B20</f>
         <v>11.923108687500001</v>
       </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="44"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="48"/>
       <c r="H44" s="12"/>
       <c r="I44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J44" s="42">
+      <c r="J44" s="46">
         <f>M43+J20</f>
         <v>0</v>
       </c>
-      <c r="K44" s="43"/>
-      <c r="L44" s="43"/>
-      <c r="M44" s="43"/>
-      <c r="N44" s="43"/>
-      <c r="O44" s="44"/>
+      <c r="K44" s="47"/>
+      <c r="L44" s="47"/>
+      <c r="M44" s="47"/>
+      <c r="N44" s="47"/>
+      <c r="O44" s="48"/>
       <c r="P44" s="12"/>
       <c r="Q44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R44" s="42">
+      <c r="R44" s="46">
         <f>U43+R20</f>
         <v>0</v>
       </c>
-      <c r="S44" s="43"/>
-      <c r="T44" s="43"/>
-      <c r="U44" s="43"/>
-      <c r="V44" s="43"/>
-      <c r="W44" s="44"/>
+      <c r="S44" s="47"/>
+      <c r="T44" s="47"/>
+      <c r="U44" s="47"/>
+      <c r="V44" s="47"/>
+      <c r="W44" s="48"/>
       <c r="X44" s="12"/>
       <c r="Y44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z44" s="42">
+      <c r="Z44" s="46">
         <f>AC43+Z20</f>
         <v>0</v>
       </c>
-      <c r="AA44" s="43"/>
-      <c r="AB44" s="43"/>
-      <c r="AC44" s="43"/>
-      <c r="AD44" s="43"/>
-      <c r="AE44" s="44"/>
+      <c r="AA44" s="47"/>
+      <c r="AB44" s="47"/>
+      <c r="AC44" s="47"/>
+      <c r="AD44" s="47"/>
+      <c r="AE44" s="48"/>
       <c r="AF44" s="12"/>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="42">
+      <c r="B45" s="46">
         <f>C43+B20</f>
         <v>2.9464924374999999</v>
       </c>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="44"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="48"/>
       <c r="H45" s="12"/>
       <c r="I45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J45" s="42">
+      <c r="J45" s="46">
         <f>K43+J20</f>
         <v>0</v>
       </c>
-      <c r="K45" s="43"/>
-      <c r="L45" s="43"/>
-      <c r="M45" s="43"/>
-      <c r="N45" s="43"/>
-      <c r="O45" s="44"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="47"/>
+      <c r="M45" s="47"/>
+      <c r="N45" s="47"/>
+      <c r="O45" s="48"/>
       <c r="P45" s="12"/>
       <c r="Q45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R45" s="42">
+      <c r="R45" s="46">
         <f>S43+R20</f>
         <v>0</v>
       </c>
-      <c r="S45" s="43"/>
-      <c r="T45" s="43"/>
-      <c r="U45" s="43"/>
-      <c r="V45" s="43"/>
-      <c r="W45" s="44"/>
+      <c r="S45" s="47"/>
+      <c r="T45" s="47"/>
+      <c r="U45" s="47"/>
+      <c r="V45" s="47"/>
+      <c r="W45" s="48"/>
       <c r="X45" s="12"/>
       <c r="Y45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z45" s="42">
+      <c r="Z45" s="46">
         <f>AA43+Z20</f>
         <v>0</v>
       </c>
-      <c r="AA45" s="43"/>
-      <c r="AB45" s="43"/>
-      <c r="AC45" s="43"/>
-      <c r="AD45" s="43"/>
-      <c r="AE45" s="44"/>
+      <c r="AA45" s="47"/>
+      <c r="AB45" s="47"/>
+      <c r="AC45" s="47"/>
+      <c r="AD45" s="47"/>
+      <c r="AE45" s="48"/>
       <c r="AF45" s="12"/>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="42">
+      <c r="B46" s="46">
         <f>IFERROR((G43/10/B44),0)</f>
         <v>0.56193398681538265</v>
       </c>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="44"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="48"/>
       <c r="H46" s="12"/>
       <c r="I46" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J46" s="42">
+      <c r="J46" s="46">
         <f>IFERROR((O43/10/J44),0)</f>
         <v>0</v>
       </c>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43"/>
-      <c r="M46" s="43"/>
-      <c r="N46" s="43"/>
-      <c r="O46" s="44"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="47"/>
+      <c r="M46" s="47"/>
+      <c r="N46" s="47"/>
+      <c r="O46" s="48"/>
       <c r="P46" s="12"/>
       <c r="Q46" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R46" s="42">
+      <c r="R46" s="46">
         <f>IFERROR((W43/10/R44),0)</f>
         <v>0</v>
       </c>
-      <c r="S46" s="43"/>
-      <c r="T46" s="43"/>
-      <c r="U46" s="43"/>
-      <c r="V46" s="43"/>
-      <c r="W46" s="44"/>
+      <c r="S46" s="47"/>
+      <c r="T46" s="47"/>
+      <c r="U46" s="47"/>
+      <c r="V46" s="47"/>
+      <c r="W46" s="48"/>
       <c r="X46" s="12"/>
       <c r="Y46" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z46" s="42">
+      <c r="Z46" s="46">
         <f>IFERROR((AE43/10/Z44),0)</f>
         <v>0</v>
       </c>
-      <c r="AA46" s="43"/>
-      <c r="AB46" s="43"/>
-      <c r="AC46" s="43"/>
-      <c r="AD46" s="43"/>
-      <c r="AE46" s="44"/>
+      <c r="AA46" s="47"/>
+      <c r="AB46" s="47"/>
+      <c r="AC46" s="47"/>
+      <c r="AD46" s="47"/>
+      <c r="AE46" s="48"/>
       <c r="AF46" s="12"/>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="42">
+      <c r="B47" s="46">
         <f>IFERROR((9.82 * F43) * LN(B44/B45),0)</f>
         <v>6245.7915133757406</v>
       </c>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="44"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="48"/>
       <c r="H47" s="12"/>
       <c r="I47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J47" s="42">
+      <c r="J47" s="46">
         <f>IFERROR((9.82 * N43) * LN(J44/J45),0)</f>
         <v>0</v>
       </c>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43"/>
-      <c r="M47" s="43"/>
-      <c r="N47" s="43"/>
-      <c r="O47" s="44"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="47"/>
+      <c r="M47" s="47"/>
+      <c r="N47" s="47"/>
+      <c r="O47" s="48"/>
       <c r="P47" s="12"/>
       <c r="Q47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R47" s="42">
+      <c r="R47" s="46">
         <f>IFERROR((9.82 * V43) * LN(R44/R45),0)</f>
         <v>0</v>
       </c>
-      <c r="S47" s="43"/>
-      <c r="T47" s="43"/>
-      <c r="U47" s="43"/>
-      <c r="V47" s="43"/>
-      <c r="W47" s="44"/>
+      <c r="S47" s="47"/>
+      <c r="T47" s="47"/>
+      <c r="U47" s="47"/>
+      <c r="V47" s="47"/>
+      <c r="W47" s="48"/>
       <c r="X47" s="12"/>
       <c r="Y47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z47" s="42">
+      <c r="Z47" s="46">
         <f>IFERROR((9.82 * AD43) * LN(Z44/Z45),0)</f>
         <v>0</v>
       </c>
-      <c r="AA47" s="43"/>
-      <c r="AB47" s="43"/>
-      <c r="AC47" s="43"/>
-      <c r="AD47" s="43"/>
-      <c r="AE47" s="44"/>
+      <c r="AA47" s="47"/>
+      <c r="AB47" s="47"/>
+      <c r="AC47" s="47"/>
+      <c r="AD47" s="47"/>
+      <c r="AE47" s="48"/>
       <c r="AF47" s="12"/>
     </row>
     <row r="48" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B48" s="39">
+      <c r="B48" s="50">
         <f>B47+B24</f>
         <v>6245.7915133757406</v>
       </c>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="41"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="52"/>
       <c r="H48" s="12"/>
       <c r="I48" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J48" s="39">
+      <c r="J48" s="50">
         <f>J47+J24</f>
         <v>0</v>
       </c>
-      <c r="K48" s="40"/>
-      <c r="L48" s="40"/>
-      <c r="M48" s="40"/>
-      <c r="N48" s="40"/>
-      <c r="O48" s="41"/>
+      <c r="K48" s="51"/>
+      <c r="L48" s="51"/>
+      <c r="M48" s="51"/>
+      <c r="N48" s="51"/>
+      <c r="O48" s="52"/>
       <c r="P48" s="12"/>
       <c r="Q48" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R48" s="39">
+      <c r="R48" s="50">
         <f>R47+R24</f>
         <v>0</v>
       </c>
-      <c r="S48" s="40"/>
-      <c r="T48" s="40"/>
-      <c r="U48" s="40"/>
-      <c r="V48" s="40"/>
-      <c r="W48" s="41"/>
+      <c r="S48" s="51"/>
+      <c r="T48" s="51"/>
+      <c r="U48" s="51"/>
+      <c r="V48" s="51"/>
+      <c r="W48" s="52"/>
       <c r="X48" s="12"/>
       <c r="Y48" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z48" s="39">
+      <c r="Z48" s="50">
         <f>Z47+Z24</f>
         <v>0</v>
       </c>
-      <c r="AA48" s="40"/>
-      <c r="AB48" s="40"/>
-      <c r="AC48" s="40"/>
-      <c r="AD48" s="40"/>
-      <c r="AE48" s="41"/>
+      <c r="AA48" s="51"/>
+      <c r="AB48" s="51"/>
+      <c r="AC48" s="51"/>
+      <c r="AD48" s="51"/>
+      <c r="AE48" s="52"/>
       <c r="AF48" s="12"/>
     </row>
     <row r="49" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33517,270 +33517,270 @@
       <c r="A68" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="42">
+      <c r="B68" s="46">
         <f>E67+B44</f>
         <v>11.923108687500001</v>
       </c>
-      <c r="C68" s="43"/>
-      <c r="D68" s="43"/>
-      <c r="E68" s="43"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="44"/>
+      <c r="C68" s="47"/>
+      <c r="D68" s="47"/>
+      <c r="E68" s="47"/>
+      <c r="F68" s="47"/>
+      <c r="G68" s="48"/>
       <c r="H68" s="12"/>
       <c r="I68" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J68" s="42">
+      <c r="J68" s="46">
         <f>M67+J44</f>
         <v>0</v>
       </c>
-      <c r="K68" s="43"/>
-      <c r="L68" s="43"/>
-      <c r="M68" s="43"/>
-      <c r="N68" s="43"/>
-      <c r="O68" s="44"/>
+      <c r="K68" s="47"/>
+      <c r="L68" s="47"/>
+      <c r="M68" s="47"/>
+      <c r="N68" s="47"/>
+      <c r="O68" s="48"/>
       <c r="P68" s="12"/>
       <c r="Q68" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R68" s="42">
+      <c r="R68" s="46">
         <f>U67+R44</f>
         <v>0</v>
       </c>
-      <c r="S68" s="43"/>
-      <c r="T68" s="43"/>
-      <c r="U68" s="43"/>
-      <c r="V68" s="43"/>
-      <c r="W68" s="44"/>
+      <c r="S68" s="47"/>
+      <c r="T68" s="47"/>
+      <c r="U68" s="47"/>
+      <c r="V68" s="47"/>
+      <c r="W68" s="48"/>
       <c r="X68" s="12"/>
       <c r="Y68" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z68" s="42">
+      <c r="Z68" s="46">
         <f>AC67+Z44</f>
         <v>0</v>
       </c>
-      <c r="AA68" s="43"/>
-      <c r="AB68" s="43"/>
-      <c r="AC68" s="43"/>
-      <c r="AD68" s="43"/>
-      <c r="AE68" s="44"/>
+      <c r="AA68" s="47"/>
+      <c r="AB68" s="47"/>
+      <c r="AC68" s="47"/>
+      <c r="AD68" s="47"/>
+      <c r="AE68" s="48"/>
       <c r="AF68" s="12"/>
     </row>
     <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="42">
+      <c r="B69" s="46">
         <f>C67+B44</f>
         <v>11.923108687500001</v>
       </c>
-      <c r="C69" s="43"/>
-      <c r="D69" s="43"/>
-      <c r="E69" s="43"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="44"/>
+      <c r="C69" s="47"/>
+      <c r="D69" s="47"/>
+      <c r="E69" s="47"/>
+      <c r="F69" s="47"/>
+      <c r="G69" s="48"/>
       <c r="H69" s="12"/>
       <c r="I69" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J69" s="42">
+      <c r="J69" s="46">
         <f>K67+J44</f>
         <v>0</v>
       </c>
-      <c r="K69" s="43"/>
-      <c r="L69" s="43"/>
-      <c r="M69" s="43"/>
-      <c r="N69" s="43"/>
-      <c r="O69" s="44"/>
+      <c r="K69" s="47"/>
+      <c r="L69" s="47"/>
+      <c r="M69" s="47"/>
+      <c r="N69" s="47"/>
+      <c r="O69" s="48"/>
       <c r="P69" s="12"/>
       <c r="Q69" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R69" s="42">
+      <c r="R69" s="46">
         <f>S67+R44</f>
         <v>0</v>
       </c>
-      <c r="S69" s="43"/>
-      <c r="T69" s="43"/>
-      <c r="U69" s="43"/>
-      <c r="V69" s="43"/>
-      <c r="W69" s="44"/>
+      <c r="S69" s="47"/>
+      <c r="T69" s="47"/>
+      <c r="U69" s="47"/>
+      <c r="V69" s="47"/>
+      <c r="W69" s="48"/>
       <c r="X69" s="12"/>
       <c r="Y69" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z69" s="42">
+      <c r="Z69" s="46">
         <f>AA67+Z44</f>
         <v>0</v>
       </c>
-      <c r="AA69" s="43"/>
-      <c r="AB69" s="43"/>
-      <c r="AC69" s="43"/>
-      <c r="AD69" s="43"/>
-      <c r="AE69" s="44"/>
+      <c r="AA69" s="47"/>
+      <c r="AB69" s="47"/>
+      <c r="AC69" s="47"/>
+      <c r="AD69" s="47"/>
+      <c r="AE69" s="48"/>
       <c r="AF69" s="12"/>
     </row>
     <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B70" s="42">
+      <c r="B70" s="46">
         <f>IFERROR((G67/10/B68),0)</f>
         <v>0</v>
       </c>
-      <c r="C70" s="43"/>
-      <c r="D70" s="43"/>
-      <c r="E70" s="43"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="44"/>
+      <c r="C70" s="47"/>
+      <c r="D70" s="47"/>
+      <c r="E70" s="47"/>
+      <c r="F70" s="47"/>
+      <c r="G70" s="48"/>
       <c r="H70" s="12"/>
       <c r="I70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J70" s="42">
+      <c r="J70" s="46">
         <f>IFERROR((O67/10/J68),0)</f>
         <v>0</v>
       </c>
-      <c r="K70" s="43"/>
-      <c r="L70" s="43"/>
-      <c r="M70" s="43"/>
-      <c r="N70" s="43"/>
-      <c r="O70" s="44"/>
+      <c r="K70" s="47"/>
+      <c r="L70" s="47"/>
+      <c r="M70" s="47"/>
+      <c r="N70" s="47"/>
+      <c r="O70" s="48"/>
       <c r="P70" s="12"/>
       <c r="Q70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R70" s="42">
+      <c r="R70" s="46">
         <f>IFERROR((W67/10/R68),0)</f>
         <v>0</v>
       </c>
-      <c r="S70" s="43"/>
-      <c r="T70" s="43"/>
-      <c r="U70" s="43"/>
-      <c r="V70" s="43"/>
-      <c r="W70" s="44"/>
+      <c r="S70" s="47"/>
+      <c r="T70" s="47"/>
+      <c r="U70" s="47"/>
+      <c r="V70" s="47"/>
+      <c r="W70" s="48"/>
       <c r="X70" s="12"/>
       <c r="Y70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z70" s="42">
+      <c r="Z70" s="46">
         <f>IFERROR((AE67/10/Z68),0)</f>
         <v>0</v>
       </c>
-      <c r="AA70" s="43"/>
-      <c r="AB70" s="43"/>
-      <c r="AC70" s="43"/>
-      <c r="AD70" s="43"/>
-      <c r="AE70" s="44"/>
+      <c r="AA70" s="47"/>
+      <c r="AB70" s="47"/>
+      <c r="AC70" s="47"/>
+      <c r="AD70" s="47"/>
+      <c r="AE70" s="48"/>
       <c r="AF70" s="12"/>
     </row>
     <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="42">
+      <c r="B71" s="46">
         <f>IFERROR((9.82 * F67) * LN(B68/B69),0)</f>
         <v>0</v>
       </c>
-      <c r="C71" s="43"/>
-      <c r="D71" s="43"/>
-      <c r="E71" s="43"/>
-      <c r="F71" s="43"/>
-      <c r="G71" s="44"/>
+      <c r="C71" s="47"/>
+      <c r="D71" s="47"/>
+      <c r="E71" s="47"/>
+      <c r="F71" s="47"/>
+      <c r="G71" s="48"/>
       <c r="H71" s="12"/>
       <c r="I71" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J71" s="42">
+      <c r="J71" s="46">
         <f>IFERROR((9.82 * N67) * LN(J68/J69),0)</f>
         <v>0</v>
       </c>
-      <c r="K71" s="43"/>
-      <c r="L71" s="43"/>
-      <c r="M71" s="43"/>
-      <c r="N71" s="43"/>
-      <c r="O71" s="44"/>
+      <c r="K71" s="47"/>
+      <c r="L71" s="47"/>
+      <c r="M71" s="47"/>
+      <c r="N71" s="47"/>
+      <c r="O71" s="48"/>
       <c r="P71" s="12"/>
       <c r="Q71" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R71" s="42">
+      <c r="R71" s="46">
         <f>IFERROR((9.82 * V67) * LN(R68/R69),0)</f>
         <v>0</v>
       </c>
-      <c r="S71" s="43"/>
-      <c r="T71" s="43"/>
-      <c r="U71" s="43"/>
-      <c r="V71" s="43"/>
-      <c r="W71" s="44"/>
+      <c r="S71" s="47"/>
+      <c r="T71" s="47"/>
+      <c r="U71" s="47"/>
+      <c r="V71" s="47"/>
+      <c r="W71" s="48"/>
       <c r="X71" s="12"/>
       <c r="Y71" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z71" s="42">
+      <c r="Z71" s="46">
         <f>IFERROR((9.82 * AD67) * LN(Z68/Z69),0)</f>
         <v>0</v>
       </c>
-      <c r="AA71" s="43"/>
-      <c r="AB71" s="43"/>
-      <c r="AC71" s="43"/>
-      <c r="AD71" s="43"/>
-      <c r="AE71" s="44"/>
+      <c r="AA71" s="47"/>
+      <c r="AB71" s="47"/>
+      <c r="AC71" s="47"/>
+      <c r="AD71" s="47"/>
+      <c r="AE71" s="48"/>
       <c r="AF71" s="12"/>
     </row>
     <row r="72" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="39">
+      <c r="B72" s="50">
         <f>B71+B48</f>
         <v>6245.7915133757406</v>
       </c>
-      <c r="C72" s="40"/>
-      <c r="D72" s="40"/>
-      <c r="E72" s="40"/>
-      <c r="F72" s="40"/>
-      <c r="G72" s="41"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="51"/>
+      <c r="E72" s="51"/>
+      <c r="F72" s="51"/>
+      <c r="G72" s="52"/>
       <c r="H72" s="12"/>
       <c r="I72" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J72" s="39">
+      <c r="J72" s="50">
         <f>J71+J48</f>
         <v>0</v>
       </c>
-      <c r="K72" s="40"/>
-      <c r="L72" s="40"/>
-      <c r="M72" s="40"/>
-      <c r="N72" s="40"/>
-      <c r="O72" s="41"/>
+      <c r="K72" s="51"/>
+      <c r="L72" s="51"/>
+      <c r="M72" s="51"/>
+      <c r="N72" s="51"/>
+      <c r="O72" s="52"/>
       <c r="P72" s="12"/>
       <c r="Q72" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R72" s="39">
+      <c r="R72" s="50">
         <f>R71+R48</f>
         <v>0</v>
       </c>
-      <c r="S72" s="40"/>
-      <c r="T72" s="40"/>
-      <c r="U72" s="40"/>
-      <c r="V72" s="40"/>
-      <c r="W72" s="41"/>
+      <c r="S72" s="51"/>
+      <c r="T72" s="51"/>
+      <c r="U72" s="51"/>
+      <c r="V72" s="51"/>
+      <c r="W72" s="52"/>
       <c r="X72" s="12"/>
       <c r="Y72" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z72" s="39">
+      <c r="Z72" s="50">
         <f>Z71+Z48</f>
         <v>0</v>
       </c>
-      <c r="AA72" s="40"/>
-      <c r="AB72" s="40"/>
-      <c r="AC72" s="40"/>
-      <c r="AD72" s="40"/>
-      <c r="AE72" s="41"/>
+      <c r="AA72" s="51"/>
+      <c r="AB72" s="51"/>
+      <c r="AC72" s="51"/>
+      <c r="AD72" s="51"/>
+      <c r="AE72" s="52"/>
       <c r="AF72" s="12"/>
     </row>
     <row r="73" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -35517,270 +35517,270 @@
       <c r="A92" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B92" s="42">
+      <c r="B92" s="46">
         <f>E91+B68</f>
         <v>11.923108687500001</v>
       </c>
-      <c r="C92" s="43"/>
-      <c r="D92" s="43"/>
-      <c r="E92" s="43"/>
-      <c r="F92" s="43"/>
-      <c r="G92" s="44"/>
+      <c r="C92" s="47"/>
+      <c r="D92" s="47"/>
+      <c r="E92" s="47"/>
+      <c r="F92" s="47"/>
+      <c r="G92" s="48"/>
       <c r="H92" s="12"/>
       <c r="I92" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J92" s="42">
+      <c r="J92" s="46">
         <f>M91+J68</f>
         <v>0</v>
       </c>
-      <c r="K92" s="43"/>
-      <c r="L92" s="43"/>
-      <c r="M92" s="43"/>
-      <c r="N92" s="43"/>
-      <c r="O92" s="44"/>
+      <c r="K92" s="47"/>
+      <c r="L92" s="47"/>
+      <c r="M92" s="47"/>
+      <c r="N92" s="47"/>
+      <c r="O92" s="48"/>
       <c r="P92" s="12"/>
       <c r="Q92" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R92" s="42">
+      <c r="R92" s="46">
         <f>U91+R68</f>
         <v>0</v>
       </c>
-      <c r="S92" s="43"/>
-      <c r="T92" s="43"/>
-      <c r="U92" s="43"/>
-      <c r="V92" s="43"/>
-      <c r="W92" s="44"/>
+      <c r="S92" s="47"/>
+      <c r="T92" s="47"/>
+      <c r="U92" s="47"/>
+      <c r="V92" s="47"/>
+      <c r="W92" s="48"/>
       <c r="X92" s="12"/>
       <c r="Y92" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z92" s="42">
+      <c r="Z92" s="46">
         <f>AC91+Z68</f>
         <v>0</v>
       </c>
-      <c r="AA92" s="43"/>
-      <c r="AB92" s="43"/>
-      <c r="AC92" s="43"/>
-      <c r="AD92" s="43"/>
-      <c r="AE92" s="44"/>
+      <c r="AA92" s="47"/>
+      <c r="AB92" s="47"/>
+      <c r="AC92" s="47"/>
+      <c r="AD92" s="47"/>
+      <c r="AE92" s="48"/>
       <c r="AF92" s="12"/>
     </row>
     <row r="93" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A93" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B93" s="42">
+      <c r="B93" s="46">
         <f>C91+B68</f>
         <v>11.923108687500001</v>
       </c>
-      <c r="C93" s="43"/>
-      <c r="D93" s="43"/>
-      <c r="E93" s="43"/>
-      <c r="F93" s="43"/>
-      <c r="G93" s="44"/>
+      <c r="C93" s="47"/>
+      <c r="D93" s="47"/>
+      <c r="E93" s="47"/>
+      <c r="F93" s="47"/>
+      <c r="G93" s="48"/>
       <c r="H93" s="12"/>
       <c r="I93" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J93" s="42">
+      <c r="J93" s="46">
         <f>K91+J68</f>
         <v>0</v>
       </c>
-      <c r="K93" s="43"/>
-      <c r="L93" s="43"/>
-      <c r="M93" s="43"/>
-      <c r="N93" s="43"/>
-      <c r="O93" s="44"/>
+      <c r="K93" s="47"/>
+      <c r="L93" s="47"/>
+      <c r="M93" s="47"/>
+      <c r="N93" s="47"/>
+      <c r="O93" s="48"/>
       <c r="P93" s="12"/>
       <c r="Q93" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R93" s="42">
+      <c r="R93" s="46">
         <f>S91+R68</f>
         <v>0</v>
       </c>
-      <c r="S93" s="43"/>
-      <c r="T93" s="43"/>
-      <c r="U93" s="43"/>
-      <c r="V93" s="43"/>
-      <c r="W93" s="44"/>
+      <c r="S93" s="47"/>
+      <c r="T93" s="47"/>
+      <c r="U93" s="47"/>
+      <c r="V93" s="47"/>
+      <c r="W93" s="48"/>
       <c r="X93" s="12"/>
       <c r="Y93" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z93" s="42">
+      <c r="Z93" s="46">
         <f>AA91+Z68</f>
         <v>0</v>
       </c>
-      <c r="AA93" s="43"/>
-      <c r="AB93" s="43"/>
-      <c r="AC93" s="43"/>
-      <c r="AD93" s="43"/>
-      <c r="AE93" s="44"/>
+      <c r="AA93" s="47"/>
+      <c r="AB93" s="47"/>
+      <c r="AC93" s="47"/>
+      <c r="AD93" s="47"/>
+      <c r="AE93" s="48"/>
       <c r="AF93" s="12"/>
     </row>
     <row r="94" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A94" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B94" s="42">
+      <c r="B94" s="46">
         <f>IFERROR((G91/10/B92),0)</f>
         <v>0</v>
       </c>
-      <c r="C94" s="43"/>
-      <c r="D94" s="43"/>
-      <c r="E94" s="43"/>
-      <c r="F94" s="43"/>
-      <c r="G94" s="44"/>
+      <c r="C94" s="47"/>
+      <c r="D94" s="47"/>
+      <c r="E94" s="47"/>
+      <c r="F94" s="47"/>
+      <c r="G94" s="48"/>
       <c r="H94" s="12"/>
       <c r="I94" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J94" s="42">
+      <c r="J94" s="46">
         <f>IFERROR((O91/10/J92),0)</f>
         <v>0</v>
       </c>
-      <c r="K94" s="43"/>
-      <c r="L94" s="43"/>
-      <c r="M94" s="43"/>
-      <c r="N94" s="43"/>
-      <c r="O94" s="44"/>
+      <c r="K94" s="47"/>
+      <c r="L94" s="47"/>
+      <c r="M94" s="47"/>
+      <c r="N94" s="47"/>
+      <c r="O94" s="48"/>
       <c r="P94" s="12"/>
       <c r="Q94" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R94" s="42">
+      <c r="R94" s="46">
         <f>IFERROR((W91/10/R92),0)</f>
         <v>0</v>
       </c>
-      <c r="S94" s="43"/>
-      <c r="T94" s="43"/>
-      <c r="U94" s="43"/>
-      <c r="V94" s="43"/>
-      <c r="W94" s="44"/>
+      <c r="S94" s="47"/>
+      <c r="T94" s="47"/>
+      <c r="U94" s="47"/>
+      <c r="V94" s="47"/>
+      <c r="W94" s="48"/>
       <c r="X94" s="12"/>
       <c r="Y94" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z94" s="42">
+      <c r="Z94" s="46">
         <f>IFERROR((AE91/10/Z92),0)</f>
         <v>0</v>
       </c>
-      <c r="AA94" s="43"/>
-      <c r="AB94" s="43"/>
-      <c r="AC94" s="43"/>
-      <c r="AD94" s="43"/>
-      <c r="AE94" s="44"/>
+      <c r="AA94" s="47"/>
+      <c r="AB94" s="47"/>
+      <c r="AC94" s="47"/>
+      <c r="AD94" s="47"/>
+      <c r="AE94" s="48"/>
       <c r="AF94" s="12"/>
     </row>
     <row r="95" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A95" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B95" s="42">
+      <c r="B95" s="46">
         <f>IFERROR((9.82 * F91) * LN(B92/B93),0)</f>
         <v>0</v>
       </c>
-      <c r="C95" s="43"/>
-      <c r="D95" s="43"/>
-      <c r="E95" s="43"/>
-      <c r="F95" s="43"/>
-      <c r="G95" s="44"/>
+      <c r="C95" s="47"/>
+      <c r="D95" s="47"/>
+      <c r="E95" s="47"/>
+      <c r="F95" s="47"/>
+      <c r="G95" s="48"/>
       <c r="H95" s="12"/>
       <c r="I95" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J95" s="42">
+      <c r="J95" s="46">
         <f>IFERROR((9.82 * N91) * LN(J92/J93),0)</f>
         <v>0</v>
       </c>
-      <c r="K95" s="43"/>
-      <c r="L95" s="43"/>
-      <c r="M95" s="43"/>
-      <c r="N95" s="43"/>
-      <c r="O95" s="44"/>
+      <c r="K95" s="47"/>
+      <c r="L95" s="47"/>
+      <c r="M95" s="47"/>
+      <c r="N95" s="47"/>
+      <c r="O95" s="48"/>
       <c r="P95" s="12"/>
       <c r="Q95" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R95" s="42">
+      <c r="R95" s="46">
         <f>IFERROR((9.82 * V91) * LN(R92/R93),0)</f>
         <v>0</v>
       </c>
-      <c r="S95" s="43"/>
-      <c r="T95" s="43"/>
-      <c r="U95" s="43"/>
-      <c r="V95" s="43"/>
-      <c r="W95" s="44"/>
+      <c r="S95" s="47"/>
+      <c r="T95" s="47"/>
+      <c r="U95" s="47"/>
+      <c r="V95" s="47"/>
+      <c r="W95" s="48"/>
       <c r="X95" s="12"/>
       <c r="Y95" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z95" s="42">
+      <c r="Z95" s="46">
         <f>IFERROR((9.82 * AD91) * LN(Z92/Z93),0)</f>
         <v>0</v>
       </c>
-      <c r="AA95" s="43"/>
-      <c r="AB95" s="43"/>
-      <c r="AC95" s="43"/>
-      <c r="AD95" s="43"/>
-      <c r="AE95" s="44"/>
+      <c r="AA95" s="47"/>
+      <c r="AB95" s="47"/>
+      <c r="AC95" s="47"/>
+      <c r="AD95" s="47"/>
+      <c r="AE95" s="48"/>
       <c r="AF95" s="12"/>
     </row>
     <row r="96" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B96" s="39">
+      <c r="B96" s="50">
         <f>B95+B72</f>
         <v>6245.7915133757406</v>
       </c>
-      <c r="C96" s="40"/>
-      <c r="D96" s="40"/>
-      <c r="E96" s="40"/>
-      <c r="F96" s="40"/>
-      <c r="G96" s="41"/>
+      <c r="C96" s="51"/>
+      <c r="D96" s="51"/>
+      <c r="E96" s="51"/>
+      <c r="F96" s="51"/>
+      <c r="G96" s="52"/>
       <c r="H96" s="12"/>
       <c r="I96" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J96" s="39">
+      <c r="J96" s="50">
         <f>J95+J72</f>
         <v>0</v>
       </c>
-      <c r="K96" s="40"/>
-      <c r="L96" s="40"/>
-      <c r="M96" s="40"/>
-      <c r="N96" s="40"/>
-      <c r="O96" s="41"/>
+      <c r="K96" s="51"/>
+      <c r="L96" s="51"/>
+      <c r="M96" s="51"/>
+      <c r="N96" s="51"/>
+      <c r="O96" s="52"/>
       <c r="P96" s="12"/>
       <c r="Q96" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R96" s="39">
+      <c r="R96" s="50">
         <f>R95+R72</f>
         <v>0</v>
       </c>
-      <c r="S96" s="40"/>
-      <c r="T96" s="40"/>
-      <c r="U96" s="40"/>
-      <c r="V96" s="40"/>
-      <c r="W96" s="41"/>
+      <c r="S96" s="51"/>
+      <c r="T96" s="51"/>
+      <c r="U96" s="51"/>
+      <c r="V96" s="51"/>
+      <c r="W96" s="52"/>
       <c r="X96" s="12"/>
       <c r="Y96" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z96" s="39">
+      <c r="Z96" s="50">
         <f>Z95+Z72</f>
         <v>0</v>
       </c>
-      <c r="AA96" s="40"/>
-      <c r="AB96" s="40"/>
-      <c r="AC96" s="40"/>
-      <c r="AD96" s="40"/>
-      <c r="AE96" s="41"/>
+      <c r="AA96" s="51"/>
+      <c r="AB96" s="51"/>
+      <c r="AC96" s="51"/>
+      <c r="AD96" s="51"/>
+      <c r="AE96" s="52"/>
       <c r="AF96" s="12"/>
     </row>
     <row r="97" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -37517,270 +37517,270 @@
       <c r="A116" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B116" s="42">
+      <c r="B116" s="46">
         <f>E115+B92</f>
         <v>11.923108687500001</v>
       </c>
-      <c r="C116" s="43"/>
-      <c r="D116" s="43"/>
-      <c r="E116" s="43"/>
-      <c r="F116" s="43"/>
-      <c r="G116" s="44"/>
+      <c r="C116" s="47"/>
+      <c r="D116" s="47"/>
+      <c r="E116" s="47"/>
+      <c r="F116" s="47"/>
+      <c r="G116" s="48"/>
       <c r="H116" s="12"/>
       <c r="I116" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J116" s="42">
+      <c r="J116" s="46">
         <f>M115+J92</f>
         <v>0</v>
       </c>
-      <c r="K116" s="43"/>
-      <c r="L116" s="43"/>
-      <c r="M116" s="43"/>
-      <c r="N116" s="43"/>
-      <c r="O116" s="44"/>
+      <c r="K116" s="47"/>
+      <c r="L116" s="47"/>
+      <c r="M116" s="47"/>
+      <c r="N116" s="47"/>
+      <c r="O116" s="48"/>
       <c r="P116" s="12"/>
       <c r="Q116" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R116" s="42">
+      <c r="R116" s="46">
         <f>U115+R92</f>
         <v>0</v>
       </c>
-      <c r="S116" s="43"/>
-      <c r="T116" s="43"/>
-      <c r="U116" s="43"/>
-      <c r="V116" s="43"/>
-      <c r="W116" s="44"/>
+      <c r="S116" s="47"/>
+      <c r="T116" s="47"/>
+      <c r="U116" s="47"/>
+      <c r="V116" s="47"/>
+      <c r="W116" s="48"/>
       <c r="X116" s="12"/>
       <c r="Y116" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z116" s="42">
+      <c r="Z116" s="46">
         <f>AC115+Z92</f>
         <v>0</v>
       </c>
-      <c r="AA116" s="43"/>
-      <c r="AB116" s="43"/>
-      <c r="AC116" s="43"/>
-      <c r="AD116" s="43"/>
-      <c r="AE116" s="44"/>
+      <c r="AA116" s="47"/>
+      <c r="AB116" s="47"/>
+      <c r="AC116" s="47"/>
+      <c r="AD116" s="47"/>
+      <c r="AE116" s="48"/>
       <c r="AF116" s="12"/>
     </row>
     <row r="117" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A117" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B117" s="42">
+      <c r="B117" s="46">
         <f>C115+B92</f>
         <v>11.923108687500001</v>
       </c>
-      <c r="C117" s="43"/>
-      <c r="D117" s="43"/>
-      <c r="E117" s="43"/>
-      <c r="F117" s="43"/>
-      <c r="G117" s="44"/>
+      <c r="C117" s="47"/>
+      <c r="D117" s="47"/>
+      <c r="E117" s="47"/>
+      <c r="F117" s="47"/>
+      <c r="G117" s="48"/>
       <c r="H117" s="12"/>
       <c r="I117" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J117" s="42">
+      <c r="J117" s="46">
         <f>K115+J92</f>
         <v>0</v>
       </c>
-      <c r="K117" s="43"/>
-      <c r="L117" s="43"/>
-      <c r="M117" s="43"/>
-      <c r="N117" s="43"/>
-      <c r="O117" s="44"/>
+      <c r="K117" s="47"/>
+      <c r="L117" s="47"/>
+      <c r="M117" s="47"/>
+      <c r="N117" s="47"/>
+      <c r="O117" s="48"/>
       <c r="P117" s="12"/>
       <c r="Q117" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R117" s="42">
+      <c r="R117" s="46">
         <f>S115+R92</f>
         <v>0</v>
       </c>
-      <c r="S117" s="43"/>
-      <c r="T117" s="43"/>
-      <c r="U117" s="43"/>
-      <c r="V117" s="43"/>
-      <c r="W117" s="44"/>
+      <c r="S117" s="47"/>
+      <c r="T117" s="47"/>
+      <c r="U117" s="47"/>
+      <c r="V117" s="47"/>
+      <c r="W117" s="48"/>
       <c r="X117" s="12"/>
       <c r="Y117" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z117" s="42">
+      <c r="Z117" s="46">
         <f>AA115+Z92</f>
         <v>0</v>
       </c>
-      <c r="AA117" s="43"/>
-      <c r="AB117" s="43"/>
-      <c r="AC117" s="43"/>
-      <c r="AD117" s="43"/>
-      <c r="AE117" s="44"/>
+      <c r="AA117" s="47"/>
+      <c r="AB117" s="47"/>
+      <c r="AC117" s="47"/>
+      <c r="AD117" s="47"/>
+      <c r="AE117" s="48"/>
       <c r="AF117" s="12"/>
     </row>
     <row r="118" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A118" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B118" s="42">
+      <c r="B118" s="46">
         <f>IFERROR((G115/10/B116),0)</f>
         <v>0</v>
       </c>
-      <c r="C118" s="43"/>
-      <c r="D118" s="43"/>
-      <c r="E118" s="43"/>
-      <c r="F118" s="43"/>
-      <c r="G118" s="44"/>
+      <c r="C118" s="47"/>
+      <c r="D118" s="47"/>
+      <c r="E118" s="47"/>
+      <c r="F118" s="47"/>
+      <c r="G118" s="48"/>
       <c r="H118" s="12"/>
       <c r="I118" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J118" s="42">
+      <c r="J118" s="46">
         <f>IFERROR((O115/10/J116),0)</f>
         <v>0</v>
       </c>
-      <c r="K118" s="43"/>
-      <c r="L118" s="43"/>
-      <c r="M118" s="43"/>
-      <c r="N118" s="43"/>
-      <c r="O118" s="44"/>
+      <c r="K118" s="47"/>
+      <c r="L118" s="47"/>
+      <c r="M118" s="47"/>
+      <c r="N118" s="47"/>
+      <c r="O118" s="48"/>
       <c r="P118" s="12"/>
       <c r="Q118" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R118" s="42">
+      <c r="R118" s="46">
         <f>IFERROR((W115/10/R116),0)</f>
         <v>0</v>
       </c>
-      <c r="S118" s="43"/>
-      <c r="T118" s="43"/>
-      <c r="U118" s="43"/>
-      <c r="V118" s="43"/>
-      <c r="W118" s="44"/>
+      <c r="S118" s="47"/>
+      <c r="T118" s="47"/>
+      <c r="U118" s="47"/>
+      <c r="V118" s="47"/>
+      <c r="W118" s="48"/>
       <c r="X118" s="12"/>
       <c r="Y118" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z118" s="42">
+      <c r="Z118" s="46">
         <f>IFERROR((AE115/10/Z116),0)</f>
         <v>0</v>
       </c>
-      <c r="AA118" s="43"/>
-      <c r="AB118" s="43"/>
-      <c r="AC118" s="43"/>
-      <c r="AD118" s="43"/>
-      <c r="AE118" s="44"/>
+      <c r="AA118" s="47"/>
+      <c r="AB118" s="47"/>
+      <c r="AC118" s="47"/>
+      <c r="AD118" s="47"/>
+      <c r="AE118" s="48"/>
       <c r="AF118" s="12"/>
     </row>
     <row r="119" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A119" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B119" s="42">
+      <c r="B119" s="46">
         <f>IFERROR((9.82 * F115) * LN(B116/B117),0)</f>
         <v>0</v>
       </c>
-      <c r="C119" s="43"/>
-      <c r="D119" s="43"/>
-      <c r="E119" s="43"/>
-      <c r="F119" s="43"/>
-      <c r="G119" s="44"/>
+      <c r="C119" s="47"/>
+      <c r="D119" s="47"/>
+      <c r="E119" s="47"/>
+      <c r="F119" s="47"/>
+      <c r="G119" s="48"/>
       <c r="H119" s="12"/>
       <c r="I119" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J119" s="42">
+      <c r="J119" s="46">
         <f>IFERROR((9.82 * N115) * LN(J116/J117),0)</f>
         <v>0</v>
       </c>
-      <c r="K119" s="43"/>
-      <c r="L119" s="43"/>
-      <c r="M119" s="43"/>
-      <c r="N119" s="43"/>
-      <c r="O119" s="44"/>
+      <c r="K119" s="47"/>
+      <c r="L119" s="47"/>
+      <c r="M119" s="47"/>
+      <c r="N119" s="47"/>
+      <c r="O119" s="48"/>
       <c r="P119" s="12"/>
       <c r="Q119" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R119" s="42">
+      <c r="R119" s="46">
         <f>IFERROR((9.82 * V115) * LN(R116/R117),0)</f>
         <v>0</v>
       </c>
-      <c r="S119" s="43"/>
-      <c r="T119" s="43"/>
-      <c r="U119" s="43"/>
-      <c r="V119" s="43"/>
-      <c r="W119" s="44"/>
+      <c r="S119" s="47"/>
+      <c r="T119" s="47"/>
+      <c r="U119" s="47"/>
+      <c r="V119" s="47"/>
+      <c r="W119" s="48"/>
       <c r="X119" s="12"/>
       <c r="Y119" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z119" s="42">
+      <c r="Z119" s="46">
         <f>IFERROR((9.82 * AD115) * LN(Z116/Z117),0)</f>
         <v>0</v>
       </c>
-      <c r="AA119" s="43"/>
-      <c r="AB119" s="43"/>
-      <c r="AC119" s="43"/>
-      <c r="AD119" s="43"/>
-      <c r="AE119" s="44"/>
+      <c r="AA119" s="47"/>
+      <c r="AB119" s="47"/>
+      <c r="AC119" s="47"/>
+      <c r="AD119" s="47"/>
+      <c r="AE119" s="48"/>
       <c r="AF119" s="12"/>
     </row>
     <row r="120" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B120" s="39">
+      <c r="B120" s="50">
         <f>B119+B96</f>
         <v>6245.7915133757406</v>
       </c>
-      <c r="C120" s="40"/>
-      <c r="D120" s="40"/>
-      <c r="E120" s="40"/>
-      <c r="F120" s="40"/>
-      <c r="G120" s="41"/>
+      <c r="C120" s="51"/>
+      <c r="D120" s="51"/>
+      <c r="E120" s="51"/>
+      <c r="F120" s="51"/>
+      <c r="G120" s="52"/>
       <c r="H120" s="12"/>
       <c r="I120" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J120" s="39">
+      <c r="J120" s="50">
         <f>J119+J96</f>
         <v>0</v>
       </c>
-      <c r="K120" s="40"/>
-      <c r="L120" s="40"/>
-      <c r="M120" s="40"/>
-      <c r="N120" s="40"/>
-      <c r="O120" s="41"/>
+      <c r="K120" s="51"/>
+      <c r="L120" s="51"/>
+      <c r="M120" s="51"/>
+      <c r="N120" s="51"/>
+      <c r="O120" s="52"/>
       <c r="P120" s="12"/>
       <c r="Q120" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R120" s="39">
+      <c r="R120" s="50">
         <f>R119+R96</f>
         <v>0</v>
       </c>
-      <c r="S120" s="40"/>
-      <c r="T120" s="40"/>
-      <c r="U120" s="40"/>
-      <c r="V120" s="40"/>
-      <c r="W120" s="41"/>
+      <c r="S120" s="51"/>
+      <c r="T120" s="51"/>
+      <c r="U120" s="51"/>
+      <c r="V120" s="51"/>
+      <c r="W120" s="52"/>
       <c r="X120" s="12"/>
       <c r="Y120" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z120" s="39">
+      <c r="Z120" s="50">
         <f>Z119+Z96</f>
         <v>0</v>
       </c>
-      <c r="AA120" s="40"/>
-      <c r="AB120" s="40"/>
-      <c r="AC120" s="40"/>
-      <c r="AD120" s="40"/>
-      <c r="AE120" s="41"/>
+      <c r="AA120" s="51"/>
+      <c r="AB120" s="51"/>
+      <c r="AC120" s="51"/>
+      <c r="AD120" s="51"/>
+      <c r="AE120" s="52"/>
       <c r="AF120" s="12"/>
     </row>
     <row r="121" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -37818,315 +37818,315 @@
       <c r="AF121" s="12"/>
     </row>
     <row r="122" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="46" t="s">
+      <c r="A122" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="B122" s="47"/>
-      <c r="C122" s="47"/>
-      <c r="D122" s="47"/>
-      <c r="E122" s="47"/>
-      <c r="F122" s="47"/>
-      <c r="G122" s="48"/>
+      <c r="B122" s="42"/>
+      <c r="C122" s="42"/>
+      <c r="D122" s="42"/>
+      <c r="E122" s="42"/>
+      <c r="F122" s="42"/>
+      <c r="G122" s="43"/>
       <c r="H122" s="12"/>
-      <c r="I122" s="46" t="s">
+      <c r="I122" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="J122" s="47"/>
-      <c r="K122" s="47"/>
-      <c r="L122" s="47"/>
-      <c r="M122" s="47"/>
-      <c r="N122" s="47"/>
-      <c r="O122" s="48"/>
+      <c r="J122" s="42"/>
+      <c r="K122" s="42"/>
+      <c r="L122" s="42"/>
+      <c r="M122" s="42"/>
+      <c r="N122" s="42"/>
+      <c r="O122" s="43"/>
       <c r="P122" s="12"/>
-      <c r="Q122" s="46" t="s">
+      <c r="Q122" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="R122" s="47"/>
-      <c r="S122" s="47"/>
-      <c r="T122" s="47"/>
-      <c r="U122" s="47"/>
-      <c r="V122" s="47"/>
-      <c r="W122" s="48"/>
+      <c r="R122" s="42"/>
+      <c r="S122" s="42"/>
+      <c r="T122" s="42"/>
+      <c r="U122" s="42"/>
+      <c r="V122" s="42"/>
+      <c r="W122" s="43"/>
       <c r="X122" s="12"/>
-      <c r="Y122" s="46" t="s">
+      <c r="Y122" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="Z122" s="47"/>
-      <c r="AA122" s="47"/>
-      <c r="AB122" s="47"/>
-      <c r="AC122" s="47"/>
-      <c r="AD122" s="47"/>
-      <c r="AE122" s="48"/>
+      <c r="Z122" s="42"/>
+      <c r="AA122" s="42"/>
+      <c r="AB122" s="42"/>
+      <c r="AC122" s="42"/>
+      <c r="AD122" s="42"/>
+      <c r="AE122" s="43"/>
       <c r="AF122" s="12"/>
     </row>
     <row r="123" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A123" s="51" t="s">
+      <c r="A123" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B123" s="51"/>
-      <c r="C123" s="51"/>
-      <c r="D123" s="50">
+      <c r="B123" s="44"/>
+      <c r="C123" s="44"/>
+      <c r="D123" s="45">
         <f>B115</f>
         <v>3</v>
       </c>
-      <c r="E123" s="50"/>
-      <c r="F123" s="50"/>
-      <c r="G123" s="50"/>
+      <c r="E123" s="45"/>
+      <c r="F123" s="45"/>
+      <c r="G123" s="45"/>
       <c r="H123" s="12"/>
-      <c r="I123" s="51" t="s">
+      <c r="I123" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="J123" s="51"/>
-      <c r="K123" s="51"/>
-      <c r="L123" s="50">
+      <c r="J123" s="44"/>
+      <c r="K123" s="44"/>
+      <c r="L123" s="45">
         <f>J115</f>
         <v>0</v>
       </c>
-      <c r="M123" s="50"/>
-      <c r="N123" s="50"/>
-      <c r="O123" s="50"/>
+      <c r="M123" s="45"/>
+      <c r="N123" s="45"/>
+      <c r="O123" s="45"/>
       <c r="P123" s="12"/>
-      <c r="Q123" s="51" t="s">
+      <c r="Q123" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="R123" s="51"/>
-      <c r="S123" s="51"/>
-      <c r="T123" s="50">
+      <c r="R123" s="44"/>
+      <c r="S123" s="44"/>
+      <c r="T123" s="45">
         <f>R115</f>
         <v>0</v>
       </c>
-      <c r="U123" s="50"/>
-      <c r="V123" s="50"/>
-      <c r="W123" s="50"/>
+      <c r="U123" s="45"/>
+      <c r="V123" s="45"/>
+      <c r="W123" s="45"/>
       <c r="X123" s="12"/>
-      <c r="Y123" s="51" t="s">
+      <c r="Y123" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="Z123" s="51"/>
-      <c r="AA123" s="51"/>
-      <c r="AB123" s="50">
+      <c r="Z123" s="44"/>
+      <c r="AA123" s="44"/>
+      <c r="AB123" s="45">
         <f>Z115</f>
         <v>0</v>
       </c>
-      <c r="AC123" s="50"/>
-      <c r="AD123" s="50"/>
-      <c r="AE123" s="50"/>
+      <c r="AC123" s="45"/>
+      <c r="AD123" s="45"/>
+      <c r="AE123" s="45"/>
       <c r="AF123" s="12"/>
     </row>
     <row r="124" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A124" s="52" t="s">
+      <c r="A124" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B124" s="52"/>
-      <c r="C124" s="52"/>
-      <c r="D124" s="49">
+      <c r="B124" s="39"/>
+      <c r="C124" s="39"/>
+      <c r="D124" s="40">
         <f>B116</f>
         <v>11.923108687500001</v>
       </c>
-      <c r="E124" s="49"/>
-      <c r="F124" s="49"/>
-      <c r="G124" s="49"/>
+      <c r="E124" s="40"/>
+      <c r="F124" s="40"/>
+      <c r="G124" s="40"/>
       <c r="H124" s="12"/>
-      <c r="I124" s="52" t="s">
+      <c r="I124" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="J124" s="52"/>
-      <c r="K124" s="52"/>
-      <c r="L124" s="49">
+      <c r="J124" s="39"/>
+      <c r="K124" s="39"/>
+      <c r="L124" s="40">
         <f>J116</f>
         <v>0</v>
       </c>
-      <c r="M124" s="49"/>
-      <c r="N124" s="49"/>
-      <c r="O124" s="49"/>
+      <c r="M124" s="40"/>
+      <c r="N124" s="40"/>
+      <c r="O124" s="40"/>
       <c r="P124" s="12"/>
-      <c r="Q124" s="52" t="s">
+      <c r="Q124" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="R124" s="52"/>
-      <c r="S124" s="52"/>
-      <c r="T124" s="49">
+      <c r="R124" s="39"/>
+      <c r="S124" s="39"/>
+      <c r="T124" s="40">
         <f>R116</f>
         <v>0</v>
       </c>
-      <c r="U124" s="49"/>
-      <c r="V124" s="49"/>
-      <c r="W124" s="49"/>
+      <c r="U124" s="40"/>
+      <c r="V124" s="40"/>
+      <c r="W124" s="40"/>
       <c r="X124" s="12"/>
-      <c r="Y124" s="52" t="s">
+      <c r="Y124" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="Z124" s="52"/>
-      <c r="AA124" s="52"/>
-      <c r="AB124" s="49">
+      <c r="Z124" s="39"/>
+      <c r="AA124" s="39"/>
+      <c r="AB124" s="40">
         <f>Z116</f>
         <v>0</v>
       </c>
-      <c r="AC124" s="49"/>
-      <c r="AD124" s="49"/>
-      <c r="AE124" s="49"/>
+      <c r="AC124" s="40"/>
+      <c r="AD124" s="40"/>
+      <c r="AE124" s="40"/>
       <c r="AF124" s="12"/>
     </row>
     <row r="125" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A125" s="52" t="s">
+      <c r="A125" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B125" s="52"/>
-      <c r="C125" s="52"/>
-      <c r="D125" s="49">
+      <c r="B125" s="39"/>
+      <c r="C125" s="39"/>
+      <c r="D125" s="40">
         <f>D115+D91+D67+D43+D19</f>
         <v>8.9766162500000011</v>
       </c>
-      <c r="E125" s="49"/>
-      <c r="F125" s="49"/>
-      <c r="G125" s="49"/>
+      <c r="E125" s="40"/>
+      <c r="F125" s="40"/>
+      <c r="G125" s="40"/>
       <c r="H125" s="12"/>
-      <c r="I125" s="52" t="s">
+      <c r="I125" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="J125" s="52"/>
-      <c r="K125" s="52"/>
-      <c r="L125" s="49">
+      <c r="J125" s="39"/>
+      <c r="K125" s="39"/>
+      <c r="L125" s="40">
         <f>L115+L91+L67+L43+L19</f>
         <v>0</v>
       </c>
-      <c r="M125" s="49"/>
-      <c r="N125" s="49"/>
-      <c r="O125" s="49"/>
+      <c r="M125" s="40"/>
+      <c r="N125" s="40"/>
+      <c r="O125" s="40"/>
       <c r="P125" s="12"/>
-      <c r="Q125" s="52" t="s">
+      <c r="Q125" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="R125" s="52"/>
-      <c r="S125" s="52"/>
-      <c r="T125" s="49">
+      <c r="R125" s="39"/>
+      <c r="S125" s="39"/>
+      <c r="T125" s="40">
         <f>T115+T91+T67+T43+T19</f>
         <v>0</v>
       </c>
-      <c r="U125" s="49"/>
-      <c r="V125" s="49"/>
-      <c r="W125" s="49"/>
+      <c r="U125" s="40"/>
+      <c r="V125" s="40"/>
+      <c r="W125" s="40"/>
       <c r="X125" s="12"/>
-      <c r="Y125" s="52" t="s">
+      <c r="Y125" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="Z125" s="52"/>
-      <c r="AA125" s="52"/>
-      <c r="AB125" s="49">
+      <c r="Z125" s="39"/>
+      <c r="AA125" s="39"/>
+      <c r="AB125" s="40">
         <f>AB115+AB91+AB67+AB43+AB19</f>
         <v>0</v>
       </c>
-      <c r="AC125" s="49"/>
-      <c r="AD125" s="49"/>
-      <c r="AE125" s="49"/>
+      <c r="AC125" s="40"/>
+      <c r="AD125" s="40"/>
+      <c r="AE125" s="40"/>
       <c r="AF125" s="12"/>
     </row>
     <row r="126" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A126" s="52" t="s">
+      <c r="A126" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B126" s="52"/>
-      <c r="C126" s="52"/>
-      <c r="D126" s="49">
+      <c r="B126" s="39"/>
+      <c r="C126" s="39"/>
+      <c r="D126" s="40">
         <f>D124-D125</f>
         <v>2.9464924374999999</v>
       </c>
-      <c r="E126" s="49"/>
-      <c r="F126" s="49"/>
-      <c r="G126" s="49"/>
+      <c r="E126" s="40"/>
+      <c r="F126" s="40"/>
+      <c r="G126" s="40"/>
       <c r="H126" s="12"/>
-      <c r="I126" s="52" t="s">
+      <c r="I126" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="J126" s="52"/>
-      <c r="K126" s="52"/>
-      <c r="L126" s="49">
+      <c r="J126" s="39"/>
+      <c r="K126" s="39"/>
+      <c r="L126" s="40">
         <f>L124-L125</f>
         <v>0</v>
       </c>
-      <c r="M126" s="49"/>
-      <c r="N126" s="49"/>
-      <c r="O126" s="49"/>
+      <c r="M126" s="40"/>
+      <c r="N126" s="40"/>
+      <c r="O126" s="40"/>
       <c r="P126" s="12"/>
-      <c r="Q126" s="52" t="s">
+      <c r="Q126" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="R126" s="52"/>
-      <c r="S126" s="52"/>
-      <c r="T126" s="49">
+      <c r="R126" s="39"/>
+      <c r="S126" s="39"/>
+      <c r="T126" s="40">
         <f>T124-T125</f>
         <v>0</v>
       </c>
-      <c r="U126" s="49"/>
-      <c r="V126" s="49"/>
-      <c r="W126" s="49"/>
+      <c r="U126" s="40"/>
+      <c r="V126" s="40"/>
+      <c r="W126" s="40"/>
       <c r="X126" s="12"/>
-      <c r="Y126" s="52" t="s">
+      <c r="Y126" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="Z126" s="52"/>
-      <c r="AA126" s="52"/>
-      <c r="AB126" s="49">
+      <c r="Z126" s="39"/>
+      <c r="AA126" s="39"/>
+      <c r="AB126" s="40">
         <f>AB124-AB125</f>
         <v>0</v>
       </c>
-      <c r="AC126" s="49"/>
-      <c r="AD126" s="49"/>
-      <c r="AE126" s="49"/>
+      <c r="AC126" s="40"/>
+      <c r="AD126" s="40"/>
+      <c r="AE126" s="40"/>
       <c r="AF126" s="12"/>
     </row>
     <row r="127" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A127" s="52" t="s">
+      <c r="A127" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="B127" s="52"/>
-      <c r="C127" s="52"/>
-      <c r="D127" s="49">
+      <c r="B127" s="39"/>
+      <c r="C127" s="39"/>
+      <c r="D127" s="40">
         <f>B120</f>
         <v>6245.7915133757406</v>
       </c>
-      <c r="E127" s="49"/>
-      <c r="F127" s="49"/>
-      <c r="G127" s="49"/>
+      <c r="E127" s="40"/>
+      <c r="F127" s="40"/>
+      <c r="G127" s="40"/>
       <c r="H127" s="12"/>
-      <c r="I127" s="52" t="s">
+      <c r="I127" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="J127" s="52"/>
-      <c r="K127" s="52"/>
-      <c r="L127" s="49">
+      <c r="J127" s="39"/>
+      <c r="K127" s="39"/>
+      <c r="L127" s="40">
         <f>J120</f>
         <v>0</v>
       </c>
-      <c r="M127" s="49"/>
-      <c r="N127" s="49"/>
-      <c r="O127" s="49"/>
+      <c r="M127" s="40"/>
+      <c r="N127" s="40"/>
+      <c r="O127" s="40"/>
       <c r="P127" s="12"/>
-      <c r="Q127" s="52" t="s">
+      <c r="Q127" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="R127" s="52"/>
-      <c r="S127" s="52"/>
-      <c r="T127" s="49">
+      <c r="R127" s="39"/>
+      <c r="S127" s="39"/>
+      <c r="T127" s="40">
         <f>R120</f>
         <v>0</v>
       </c>
-      <c r="U127" s="49"/>
-      <c r="V127" s="49"/>
-      <c r="W127" s="49"/>
+      <c r="U127" s="40"/>
+      <c r="V127" s="40"/>
+      <c r="W127" s="40"/>
       <c r="X127" s="12"/>
-      <c r="Y127" s="52" t="s">
+      <c r="Y127" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="Z127" s="52"/>
-      <c r="AA127" s="52"/>
-      <c r="AB127" s="49">
+      <c r="Z127" s="39"/>
+      <c r="AA127" s="39"/>
+      <c r="AB127" s="40">
         <f>Z120</f>
         <v>0</v>
       </c>
-      <c r="AC127" s="49"/>
-      <c r="AD127" s="49"/>
-      <c r="AE127" s="49"/>
+      <c r="AC127" s="40"/>
+      <c r="AD127" s="40"/>
+      <c r="AE127" s="40"/>
       <c r="AF127" s="12"/>
     </row>
     <row r="128" spans="1:32" x14ac:dyDescent="0.25">
@@ -38165,49 +38165,87 @@
     </row>
   </sheetData>
   <mergeCells count="148">
-    <mergeCell ref="Y127:AA127"/>
-    <mergeCell ref="AB127:AE127"/>
-    <mergeCell ref="Y122:AE122"/>
-    <mergeCell ref="Y123:AA123"/>
-    <mergeCell ref="AB123:AE123"/>
-    <mergeCell ref="Y124:AA124"/>
-    <mergeCell ref="AB124:AE124"/>
-    <mergeCell ref="Y125:AA125"/>
-    <mergeCell ref="AB125:AE125"/>
-    <mergeCell ref="Y126:AA126"/>
-    <mergeCell ref="AB126:AE126"/>
-    <mergeCell ref="I127:K127"/>
-    <mergeCell ref="L127:O127"/>
-    <mergeCell ref="Q122:W122"/>
-    <mergeCell ref="Q123:S123"/>
-    <mergeCell ref="T123:W123"/>
-    <mergeCell ref="Q124:S124"/>
-    <mergeCell ref="T124:W124"/>
-    <mergeCell ref="Q125:S125"/>
-    <mergeCell ref="T125:W125"/>
-    <mergeCell ref="Q126:S126"/>
-    <mergeCell ref="T126:W126"/>
-    <mergeCell ref="Q127:S127"/>
-    <mergeCell ref="T127:W127"/>
-    <mergeCell ref="I122:O122"/>
-    <mergeCell ref="I123:K123"/>
-    <mergeCell ref="L123:O123"/>
-    <mergeCell ref="I124:K124"/>
-    <mergeCell ref="L124:O124"/>
-    <mergeCell ref="I125:K125"/>
-    <mergeCell ref="L125:O125"/>
-    <mergeCell ref="I126:K126"/>
-    <mergeCell ref="L126:O126"/>
-    <mergeCell ref="D127:G127"/>
-    <mergeCell ref="D125:G125"/>
-    <mergeCell ref="D124:G124"/>
-    <mergeCell ref="D123:G123"/>
-    <mergeCell ref="A123:C123"/>
-    <mergeCell ref="A124:C124"/>
-    <mergeCell ref="A125:C125"/>
-    <mergeCell ref="A127:C127"/>
-    <mergeCell ref="A126:C126"/>
-    <mergeCell ref="D126:G126"/>
+    <mergeCell ref="B120:G120"/>
+    <mergeCell ref="J120:O120"/>
+    <mergeCell ref="R120:W120"/>
+    <mergeCell ref="Z120:AE120"/>
+    <mergeCell ref="B119:G119"/>
+    <mergeCell ref="J119:O119"/>
+    <mergeCell ref="R119:W119"/>
+    <mergeCell ref="Z119:AE119"/>
+    <mergeCell ref="B118:G118"/>
+    <mergeCell ref="J118:O118"/>
+    <mergeCell ref="R118:W118"/>
+    <mergeCell ref="Z118:AE118"/>
+    <mergeCell ref="B117:G117"/>
+    <mergeCell ref="J117:O117"/>
+    <mergeCell ref="R117:W117"/>
+    <mergeCell ref="Z117:AE117"/>
+    <mergeCell ref="B116:G116"/>
+    <mergeCell ref="J116:O116"/>
+    <mergeCell ref="R116:W116"/>
+    <mergeCell ref="Z116:AE116"/>
+    <mergeCell ref="B96:G96"/>
+    <mergeCell ref="J96:O96"/>
+    <mergeCell ref="R96:W96"/>
+    <mergeCell ref="Z96:AE96"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="J95:O95"/>
+    <mergeCell ref="R95:W95"/>
+    <mergeCell ref="Z95:AE95"/>
+    <mergeCell ref="B94:G94"/>
+    <mergeCell ref="J94:O94"/>
+    <mergeCell ref="R94:W94"/>
+    <mergeCell ref="Z94:AE94"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="J93:O93"/>
+    <mergeCell ref="R93:W93"/>
+    <mergeCell ref="Z93:AE93"/>
+    <mergeCell ref="B92:G92"/>
+    <mergeCell ref="J92:O92"/>
+    <mergeCell ref="R92:W92"/>
+    <mergeCell ref="Z92:AE92"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="J72:O72"/>
+    <mergeCell ref="R72:W72"/>
+    <mergeCell ref="Z72:AE72"/>
+    <mergeCell ref="B71:G71"/>
+    <mergeCell ref="J71:O71"/>
+    <mergeCell ref="R71:W71"/>
+    <mergeCell ref="Z71:AE71"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="J70:O70"/>
+    <mergeCell ref="R70:W70"/>
+    <mergeCell ref="Z70:AE70"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="J69:O69"/>
+    <mergeCell ref="R69:W69"/>
+    <mergeCell ref="Z69:AE69"/>
+    <mergeCell ref="B68:G68"/>
+    <mergeCell ref="J68:O68"/>
+    <mergeCell ref="R68:W68"/>
+    <mergeCell ref="Z68:AE68"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="J48:O48"/>
+    <mergeCell ref="R48:W48"/>
+    <mergeCell ref="Z48:AE48"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="J47:O47"/>
+    <mergeCell ref="R47:W47"/>
+    <mergeCell ref="Z47:AE47"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="J46:O46"/>
+    <mergeCell ref="R46:W46"/>
+    <mergeCell ref="Z46:AE46"/>
+    <mergeCell ref="Z45:AE45"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="J44:O44"/>
+    <mergeCell ref="R44:W44"/>
+    <mergeCell ref="Z44:AE44"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="R24:W24"/>
+    <mergeCell ref="Z24:AE24"/>
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="J20:O20"/>
     <mergeCell ref="R20:W20"/>
@@ -38232,87 +38270,49 @@
     <mergeCell ref="B45:G45"/>
     <mergeCell ref="J45:O45"/>
     <mergeCell ref="R45:W45"/>
-    <mergeCell ref="Z45:AE45"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="J44:O44"/>
-    <mergeCell ref="R44:W44"/>
-    <mergeCell ref="Z44:AE44"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="R24:W24"/>
-    <mergeCell ref="Z24:AE24"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="J48:O48"/>
-    <mergeCell ref="R48:W48"/>
-    <mergeCell ref="Z48:AE48"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="J47:O47"/>
-    <mergeCell ref="R47:W47"/>
-    <mergeCell ref="Z47:AE47"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="J46:O46"/>
-    <mergeCell ref="R46:W46"/>
-    <mergeCell ref="Z46:AE46"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="J70:O70"/>
-    <mergeCell ref="R70:W70"/>
-    <mergeCell ref="Z70:AE70"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="J69:O69"/>
-    <mergeCell ref="R69:W69"/>
-    <mergeCell ref="Z69:AE69"/>
-    <mergeCell ref="B68:G68"/>
-    <mergeCell ref="J68:O68"/>
-    <mergeCell ref="R68:W68"/>
-    <mergeCell ref="Z68:AE68"/>
-    <mergeCell ref="B92:G92"/>
-    <mergeCell ref="J92:O92"/>
-    <mergeCell ref="R92:W92"/>
-    <mergeCell ref="Z92:AE92"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="J72:O72"/>
-    <mergeCell ref="R72:W72"/>
-    <mergeCell ref="Z72:AE72"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="J71:O71"/>
-    <mergeCell ref="R71:W71"/>
-    <mergeCell ref="Z71:AE71"/>
-    <mergeCell ref="B95:G95"/>
-    <mergeCell ref="J95:O95"/>
-    <mergeCell ref="R95:W95"/>
-    <mergeCell ref="Z95:AE95"/>
-    <mergeCell ref="B94:G94"/>
-    <mergeCell ref="J94:O94"/>
-    <mergeCell ref="R94:W94"/>
-    <mergeCell ref="Z94:AE94"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="J93:O93"/>
-    <mergeCell ref="R93:W93"/>
-    <mergeCell ref="Z93:AE93"/>
-    <mergeCell ref="B117:G117"/>
-    <mergeCell ref="J117:O117"/>
-    <mergeCell ref="R117:W117"/>
-    <mergeCell ref="Z117:AE117"/>
-    <mergeCell ref="B116:G116"/>
-    <mergeCell ref="J116:O116"/>
-    <mergeCell ref="R116:W116"/>
-    <mergeCell ref="Z116:AE116"/>
-    <mergeCell ref="B96:G96"/>
-    <mergeCell ref="J96:O96"/>
-    <mergeCell ref="R96:W96"/>
-    <mergeCell ref="Z96:AE96"/>
-    <mergeCell ref="B120:G120"/>
-    <mergeCell ref="J120:O120"/>
-    <mergeCell ref="R120:W120"/>
-    <mergeCell ref="Z120:AE120"/>
-    <mergeCell ref="B119:G119"/>
-    <mergeCell ref="J119:O119"/>
-    <mergeCell ref="R119:W119"/>
-    <mergeCell ref="Z119:AE119"/>
-    <mergeCell ref="B118:G118"/>
-    <mergeCell ref="J118:O118"/>
-    <mergeCell ref="R118:W118"/>
-    <mergeCell ref="Z118:AE118"/>
+    <mergeCell ref="D127:G127"/>
+    <mergeCell ref="D125:G125"/>
+    <mergeCell ref="D124:G124"/>
+    <mergeCell ref="D123:G123"/>
+    <mergeCell ref="A123:C123"/>
+    <mergeCell ref="A124:C124"/>
+    <mergeCell ref="A125:C125"/>
+    <mergeCell ref="A127:C127"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="D126:G126"/>
+    <mergeCell ref="I127:K127"/>
+    <mergeCell ref="L127:O127"/>
+    <mergeCell ref="Q122:W122"/>
+    <mergeCell ref="Q123:S123"/>
+    <mergeCell ref="T123:W123"/>
+    <mergeCell ref="Q124:S124"/>
+    <mergeCell ref="T124:W124"/>
+    <mergeCell ref="Q125:S125"/>
+    <mergeCell ref="T125:W125"/>
+    <mergeCell ref="Q126:S126"/>
+    <mergeCell ref="T126:W126"/>
+    <mergeCell ref="Q127:S127"/>
+    <mergeCell ref="T127:W127"/>
+    <mergeCell ref="I122:O122"/>
+    <mergeCell ref="I123:K123"/>
+    <mergeCell ref="L123:O123"/>
+    <mergeCell ref="I124:K124"/>
+    <mergeCell ref="L124:O124"/>
+    <mergeCell ref="I125:K125"/>
+    <mergeCell ref="L125:O125"/>
+    <mergeCell ref="I126:K126"/>
+    <mergeCell ref="L126:O126"/>
+    <mergeCell ref="Y127:AA127"/>
+    <mergeCell ref="AB127:AE127"/>
+    <mergeCell ref="Y122:AE122"/>
+    <mergeCell ref="Y123:AA123"/>
+    <mergeCell ref="AB123:AE123"/>
+    <mergeCell ref="Y124:AA124"/>
+    <mergeCell ref="AB124:AE124"/>
+    <mergeCell ref="Y125:AA125"/>
+    <mergeCell ref="AB125:AE125"/>
+    <mergeCell ref="Y126:AA126"/>
+    <mergeCell ref="AB126:AE126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39378,8 +39378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD63"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
* FIX - New engine cluster symmetry part null-ref. * FIX - Fairing interaction code / custom size reverting for MUS/MFT/Engines * CHANGE - Update ICPS and HUS with new RL10 mass statistics. * CHANGE - Add RCS ports to ICPS and HUS (MODEL node based) * CHANGE - Disable 'top fairing' sizing updates for engines, it is auto-sized by the plugin.
</commit_message>
<xml_diff>
--- a/GameData/SSTU/Parts/Parts-MassCalc.xlsx
+++ b/GameData/SSTU/Parts/Parts-MassCalc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="parts" sheetId="1" r:id="rId1"/>
@@ -1557,13 +1557,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1578,26 +1590,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1905,9 +1905,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC301"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S61" sqref="S61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7513,7 +7513,7 @@
         <v>64</v>
       </c>
       <c r="B59" s="6">
-        <v>1.6</v>
+        <v>0.68</v>
       </c>
       <c r="C59" s="6">
         <v>37</v>
@@ -7546,7 +7546,7 @@
       </c>
       <c r="L59" s="4">
         <f t="shared" si="14"/>
-        <v>6.317499999999999</v>
+        <v>5.3974999999999991</v>
       </c>
       <c r="M59" s="4">
         <f>IFERROR(VLOOKUP(I59,FuelTypes!$A$1:$B$32,2,FALSE)*J59,0)</f>
@@ -7554,11 +7554,11 @@
       </c>
       <c r="N59" s="4">
         <f t="shared" si="17"/>
-        <v>37.767499999999998</v>
+        <v>36.847499999999997</v>
       </c>
       <c r="O59" s="4">
         <f t="shared" si="15"/>
-        <v>0.83272655060567946</v>
+        <v>0.85351787773933108</v>
       </c>
       <c r="P59" s="4">
         <f>VLOOKUP(I59, FuelTypes!$A$1:$R$12,17,FALSE)*J59</f>
@@ -7570,11 +7570,11 @@
       </c>
       <c r="R59" s="4">
         <f t="shared" si="3"/>
-        <v>0.17872509432713313</v>
+        <v>0.18318746183594548</v>
       </c>
       <c r="S59" s="4">
         <f t="shared" si="4"/>
-        <v>1.0295185185185185</v>
+        <v>0.87959259259259248</v>
       </c>
       <c r="T59" s="4">
         <f t="shared" si="5"/>
@@ -7602,7 +7602,7 @@
       </c>
       <c r="AC59" s="3">
         <f t="shared" si="7"/>
-        <v>0.83272655060567946</v>
+        <v>0.85351787773933108</v>
       </c>
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.25">
@@ -7610,7 +7610,8 @@
         <v>65</v>
       </c>
       <c r="B60" s="6">
-        <v>6.4</v>
+        <f>4*0.68</f>
+        <v>2.72</v>
       </c>
       <c r="C60" s="6">
         <v>102</v>
@@ -7643,7 +7644,7 @@
       </c>
       <c r="L60" s="4">
         <f t="shared" si="14"/>
-        <v>19.405000000000001</v>
+        <v>15.725000000000001</v>
       </c>
       <c r="M60" s="4">
         <f>IFERROR(VLOOKUP(I60,FuelTypes!$A$1:$B$32,2,FALSE)*J60,0)</f>
@@ -7651,11 +7652,11 @@
       </c>
       <c r="N60" s="4">
         <f t="shared" si="17"/>
-        <v>106.105</v>
+        <v>102.42500000000001</v>
       </c>
       <c r="O60" s="4">
         <f t="shared" si="15"/>
-        <v>0.81711512181329815</v>
+        <v>0.84647302904564303</v>
       </c>
       <c r="P60" s="4">
         <f>VLOOKUP(I60, FuelTypes!$A$1:$R$12,17,FALSE)*J60</f>
@@ -7667,11 +7668,11 @@
       </c>
       <c r="R60" s="4">
         <f t="shared" si="3"/>
-        <v>0.2544649168276707</v>
+        <v>0.26360751769587498</v>
       </c>
       <c r="S60" s="4">
         <f t="shared" si="4"/>
-        <v>1.7967592592592592</v>
+        <v>1.4560185185185186</v>
       </c>
       <c r="T60" s="4">
         <f t="shared" si="5"/>
@@ -7699,7 +7700,7 @@
       </c>
       <c r="AC60" s="3">
         <f t="shared" si="7"/>
-        <v>0.81711512181329815</v>
+        <v>0.84647302904564303</v>
       </c>
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.25">
@@ -7707,7 +7708,8 @@
         <v>171</v>
       </c>
       <c r="B61" s="6">
-        <v>4</v>
+        <f>0.45*4</f>
+        <v>1.8</v>
       </c>
       <c r="C61" s="18">
         <v>102</v>
@@ -7722,8 +7724,8 @@
         <v>455</v>
       </c>
       <c r="G61" s="6">
-        <f>67*4</f>
-        <v>268</v>
+        <f>45*4</f>
+        <v>180</v>
       </c>
       <c r="H61" s="6">
         <v>60</v>
@@ -7741,7 +7743,7 @@
       </c>
       <c r="L61" s="4">
         <f t="shared" si="14"/>
-        <v>7.7119521250000007</v>
+        <v>5.5119521250000005</v>
       </c>
       <c r="M61" s="4">
         <f>IFERROR(VLOOKUP(I61,FuelTypes!$A$1:$B$32,2,FALSE)*J61,0)</f>
@@ -7749,11 +7751,11 @@
       </c>
       <c r="N61" s="4">
         <f t="shared" si="17"/>
-        <v>32.458299625000009</v>
+        <v>30.258299625000006</v>
       </c>
       <c r="O61" s="4">
         <f t="shared" si="15"/>
-        <v>0.76240430909510404</v>
+        <v>0.8178366863534553</v>
       </c>
       <c r="P61" s="4">
         <f>VLOOKUP(I61, FuelTypes!$A$1:$R$12,17,FALSE)*J61</f>
@@ -7765,19 +7767,19 @@
       </c>
       <c r="R61" s="4">
         <f t="shared" si="3"/>
-        <v>0.82567479842222302</v>
+        <v>0.59487810693526355</v>
       </c>
       <c r="S61" s="4">
         <f t="shared" si="4"/>
-        <v>1.7265564458955227</v>
+        <v>1.837317375</v>
       </c>
       <c r="T61" s="4">
         <f t="shared" si="5"/>
-        <v>6.0041894904280226E-2</v>
+        <v>4.0326645831232986E-2</v>
       </c>
       <c r="U61" s="4">
         <f t="shared" si="12"/>
-        <v>412.15134098367548</v>
+        <v>613.64755213125011</v>
       </c>
       <c r="W61" s="3">
         <f>IFERROR(VLOOKUP(I61,FuelTypes!$A$2:$G$40,5,FALSE)*M61,0)</f>
@@ -7797,7 +7799,7 @@
       </c>
       <c r="AC61" s="3">
         <f t="shared" si="7"/>
-        <v>0.76240430909510404</v>
+        <v>0.8178366863534553</v>
       </c>
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.25">
@@ -7805,7 +7807,7 @@
         <v>167</v>
       </c>
       <c r="B62" s="6">
-        <v>1</v>
+        <v>0.45</v>
       </c>
       <c r="C62" s="18">
         <v>37</v>
@@ -7820,7 +7822,7 @@
         <v>455</v>
       </c>
       <c r="G62" s="6">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="H62" s="6">
         <v>35</v>
@@ -7838,7 +7840,7 @@
       </c>
       <c r="L62" s="4">
         <f t="shared" si="14"/>
-        <v>2.3464924375000002</v>
+        <v>1.7964924375</v>
       </c>
       <c r="M62" s="4">
         <f>IFERROR(VLOOKUP(I62,FuelTypes!$A$1:$B$32,2,FALSE)*J62,0)</f>
@@ -7846,11 +7848,11 @@
       </c>
       <c r="N62" s="4">
         <f t="shared" si="17"/>
-        <v>11.323108687500001</v>
+        <v>10.773108687500001</v>
       </c>
       <c r="O62" s="4">
         <f t="shared" si="15"/>
-        <v>0.79276959161485572</v>
+        <v>0.83324289305792831</v>
       </c>
       <c r="P62" s="4">
         <f>VLOOKUP(I62, FuelTypes!$A$1:$R$12,17,FALSE)*J62</f>
@@ -7862,19 +7864,19 @@
       </c>
       <c r="R62" s="4">
         <f t="shared" si="3"/>
-        <v>0.5917102966075366</v>
+        <v>0.4177067298338254</v>
       </c>
       <c r="S62" s="4">
         <f t="shared" si="4"/>
-        <v>1.2257796315298508</v>
+        <v>1.3972718958333334</v>
       </c>
       <c r="T62" s="4">
         <f t="shared" si="5"/>
-        <v>1.5010473726070056E-2</v>
+        <v>1.0081661457808247E-2</v>
       </c>
       <c r="U62" s="4">
         <f t="shared" si="12"/>
-        <v>598.02351436847027</v>
+        <v>890.39056583750016</v>
       </c>
       <c r="W62" s="3">
         <f>IFERROR(VLOOKUP(I62,FuelTypes!$A$2:$G$40,5,FALSE)*M62,0)</f>
@@ -7894,7 +7896,7 @@
       </c>
       <c r="AC62" s="3">
         <f t="shared" si="7"/>
-        <v>0.79276959161485572</v>
+        <v>0.83324289305792831</v>
       </c>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.25">
@@ -27828,45 +27830,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
       <c r="H1" s="12"/>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
       <c r="P1" s="12"/>
-      <c r="Q1" s="46" t="s">
+      <c r="Q1" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
       <c r="X1" s="12"/>
-      <c r="Y1" s="46" t="s">
+      <c r="Y1" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="50"/>
       <c r="AF1" s="12"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -29577,270 +29579,270 @@
       <c r="A20" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="43">
+      <c r="B20" s="47">
         <f>E19</f>
         <v>0</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="45"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="49"/>
       <c r="H20" s="12"/>
       <c r="I20" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J20" s="43">
+      <c r="J20" s="47">
         <f>M19</f>
         <v>0</v>
       </c>
-      <c r="K20" s="44"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="44"/>
-      <c r="O20" s="45"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="49"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R20" s="43">
+      <c r="R20" s="47">
         <f>U19</f>
         <v>0</v>
       </c>
-      <c r="S20" s="44"/>
-      <c r="T20" s="44"/>
-      <c r="U20" s="44"/>
-      <c r="V20" s="44"/>
-      <c r="W20" s="45"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="48"/>
+      <c r="W20" s="49"/>
       <c r="X20" s="12"/>
       <c r="Y20" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z20" s="43">
+      <c r="Z20" s="47">
         <f>AC19</f>
         <v>0</v>
       </c>
-      <c r="AA20" s="44"/>
-      <c r="AB20" s="44"/>
-      <c r="AC20" s="44"/>
-      <c r="AD20" s="44"/>
-      <c r="AE20" s="45"/>
+      <c r="AA20" s="48"/>
+      <c r="AB20" s="48"/>
+      <c r="AC20" s="48"/>
+      <c r="AD20" s="48"/>
+      <c r="AE20" s="49"/>
       <c r="AF20" s="12"/>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="43">
+      <c r="B21" s="47">
         <f>C19</f>
         <v>0</v>
       </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="45"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="49"/>
       <c r="H21" s="12"/>
       <c r="I21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J21" s="43">
+      <c r="J21" s="47">
         <f>K19</f>
         <v>0</v>
       </c>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="45"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="49"/>
       <c r="P21" s="12"/>
       <c r="Q21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R21" s="43">
+      <c r="R21" s="47">
         <f>S19</f>
         <v>0</v>
       </c>
-      <c r="S21" s="44"/>
-      <c r="T21" s="44"/>
-      <c r="U21" s="44"/>
-      <c r="V21" s="44"/>
-      <c r="W21" s="45"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="48"/>
+      <c r="V21" s="48"/>
+      <c r="W21" s="49"/>
       <c r="X21" s="12"/>
       <c r="Y21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z21" s="43">
+      <c r="Z21" s="47">
         <f>AA19</f>
         <v>0</v>
       </c>
-      <c r="AA21" s="44"/>
-      <c r="AB21" s="44"/>
-      <c r="AC21" s="44"/>
-      <c r="AD21" s="44"/>
-      <c r="AE21" s="45"/>
+      <c r="AA21" s="48"/>
+      <c r="AB21" s="48"/>
+      <c r="AC21" s="48"/>
+      <c r="AD21" s="48"/>
+      <c r="AE21" s="49"/>
       <c r="AF21" s="12"/>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="43">
+      <c r="B22" s="47">
         <f>IFERROR((G19/10/B20),0)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="45"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="49"/>
       <c r="H22" s="12"/>
       <c r="I22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J22" s="43">
+      <c r="J22" s="47">
         <f>IFERROR((O19/10/J20),0)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="45"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="49"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R22" s="43">
+      <c r="R22" s="47">
         <f>IFERROR((W19/10/R20),0)</f>
         <v>0</v>
       </c>
-      <c r="S22" s="44"/>
-      <c r="T22" s="44"/>
-      <c r="U22" s="44"/>
-      <c r="V22" s="44"/>
-      <c r="W22" s="45"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="48"/>
+      <c r="V22" s="48"/>
+      <c r="W22" s="49"/>
       <c r="X22" s="12"/>
       <c r="Y22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z22" s="43">
+      <c r="Z22" s="47">
         <f>IFERROR((AE19/10/Z20),0)</f>
         <v>0</v>
       </c>
-      <c r="AA22" s="44"/>
-      <c r="AB22" s="44"/>
-      <c r="AC22" s="44"/>
-      <c r="AD22" s="44"/>
-      <c r="AE22" s="45"/>
+      <c r="AA22" s="48"/>
+      <c r="AB22" s="48"/>
+      <c r="AC22" s="48"/>
+      <c r="AD22" s="48"/>
+      <c r="AE22" s="49"/>
       <c r="AF22" s="12"/>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="43">
+      <c r="B23" s="47">
         <f>IFERROR((9.82 * F19) * LN(B20/C19),0)</f>
         <v>0</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="45"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="49"/>
       <c r="H23" s="12"/>
       <c r="I23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J23" s="43">
+      <c r="J23" s="47">
         <f>IFERROR((9.82 * N19) * LN(J20/K19),0)</f>
         <v>0</v>
       </c>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="44"/>
-      <c r="O23" s="45"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="49"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R23" s="43">
+      <c r="R23" s="47">
         <f>IFERROR((9.82 * V19) * LN(R20/S19),0)</f>
         <v>0</v>
       </c>
-      <c r="S23" s="44"/>
-      <c r="T23" s="44"/>
-      <c r="U23" s="44"/>
-      <c r="V23" s="44"/>
-      <c r="W23" s="45"/>
+      <c r="S23" s="48"/>
+      <c r="T23" s="48"/>
+      <c r="U23" s="48"/>
+      <c r="V23" s="48"/>
+      <c r="W23" s="49"/>
       <c r="X23" s="12"/>
       <c r="Y23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z23" s="43">
+      <c r="Z23" s="47">
         <f>IFERROR((9.82 * AD19) * LN(Z20/AA19),0)</f>
         <v>0</v>
       </c>
-      <c r="AA23" s="44"/>
-      <c r="AB23" s="44"/>
-      <c r="AC23" s="44"/>
-      <c r="AD23" s="44"/>
-      <c r="AE23" s="45"/>
+      <c r="AA23" s="48"/>
+      <c r="AB23" s="48"/>
+      <c r="AC23" s="48"/>
+      <c r="AD23" s="48"/>
+      <c r="AE23" s="49"/>
       <c r="AF23" s="12"/>
     </row>
     <row r="24" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="40">
+      <c r="B24" s="51">
         <f>B23</f>
         <v>0</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="42"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="53"/>
       <c r="H24" s="12"/>
       <c r="I24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J24" s="40">
+      <c r="J24" s="51">
         <f>J23</f>
         <v>0</v>
       </c>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="42"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="53"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R24" s="40">
+      <c r="R24" s="51">
         <f>R23</f>
         <v>0</v>
       </c>
-      <c r="S24" s="41"/>
-      <c r="T24" s="41"/>
-      <c r="U24" s="41"/>
-      <c r="V24" s="41"/>
-      <c r="W24" s="42"/>
+      <c r="S24" s="52"/>
+      <c r="T24" s="52"/>
+      <c r="U24" s="52"/>
+      <c r="V24" s="52"/>
+      <c r="W24" s="53"/>
       <c r="X24" s="12"/>
       <c r="Y24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z24" s="40">
+      <c r="Z24" s="51">
         <f>Z23</f>
         <v>0</v>
       </c>
-      <c r="AA24" s="41"/>
-      <c r="AB24" s="41"/>
-      <c r="AC24" s="41"/>
-      <c r="AD24" s="41"/>
-      <c r="AE24" s="42"/>
+      <c r="AA24" s="52"/>
+      <c r="AB24" s="52"/>
+      <c r="AC24" s="52"/>
+      <c r="AD24" s="52"/>
+      <c r="AE24" s="53"/>
       <c r="AF24" s="12"/>
     </row>
     <row r="25" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29976,7 +29978,7 @@
       </c>
       <c r="C27" s="4">
         <f>IFERROR(VLOOKUP(A27,parts!$A$2:$Z$300,12,FALSE)*B27,0)</f>
-        <v>2.3464924375000002</v>
+        <v>1.7964924375</v>
       </c>
       <c r="D27" s="4">
         <f>IFERROR(VLOOKUP(A27,parts!$A$2:$Z$300,13,FALSE)*B27,0)</f>
@@ -29984,7 +29986,7 @@
       </c>
       <c r="E27" s="4">
         <f>IFERROR(VLOOKUP(A27,parts!$A$2:$Z$300,14,FALSE)*B27,0)</f>
-        <v>11.323108687500001</v>
+        <v>10.773108687500001</v>
       </c>
       <c r="F27" s="4">
         <f>IFERROR(VLOOKUP(A27,parts!$A$2:$Z$300,6,FALSE),0)</f>
@@ -29992,7 +29994,7 @@
       </c>
       <c r="G27" s="4">
         <f>IFERROR(VLOOKUP(A27,parts!$A$2:$Z$300,7,FALSE)*B27,0)</f>
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="11"/>
@@ -31473,7 +31475,7 @@
       </c>
       <c r="C43" s="4">
         <f>SUM(C27:C41)</f>
-        <v>2.3464924375000002</v>
+        <v>1.7964924375</v>
       </c>
       <c r="D43" s="4">
         <f>SUM(D27:D41)</f>
@@ -31481,7 +31483,7 @@
       </c>
       <c r="E43" s="4">
         <f>SUM(E27:E41)</f>
-        <v>11.323108687500001</v>
+        <v>10.773108687500001</v>
       </c>
       <c r="F43" s="4">
         <f>LARGE(F27:F41,1)</f>
@@ -31489,7 +31491,7 @@
       </c>
       <c r="G43" s="10">
         <f>SUM(G27:G41)</f>
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="H43" s="12"/>
       <c r="I43" s="16" t="s">
@@ -31581,270 +31583,270 @@
       <c r="A44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="43">
+      <c r="B44" s="47">
         <f>E43+B20</f>
-        <v>11.323108687500001</v>
-      </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="45"/>
+        <v>10.773108687500001</v>
+      </c>
+      <c r="C44" s="48"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="48"/>
+      <c r="F44" s="48"/>
+      <c r="G44" s="49"/>
       <c r="H44" s="12"/>
       <c r="I44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J44" s="43">
+      <c r="J44" s="47">
         <f>M43+J20</f>
         <v>0</v>
       </c>
-      <c r="K44" s="44"/>
-      <c r="L44" s="44"/>
-      <c r="M44" s="44"/>
-      <c r="N44" s="44"/>
-      <c r="O44" s="45"/>
+      <c r="K44" s="48"/>
+      <c r="L44" s="48"/>
+      <c r="M44" s="48"/>
+      <c r="N44" s="48"/>
+      <c r="O44" s="49"/>
       <c r="P44" s="12"/>
       <c r="Q44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R44" s="43">
+      <c r="R44" s="47">
         <f>U43+R20</f>
         <v>0</v>
       </c>
-      <c r="S44" s="44"/>
-      <c r="T44" s="44"/>
-      <c r="U44" s="44"/>
-      <c r="V44" s="44"/>
-      <c r="W44" s="45"/>
+      <c r="S44" s="48"/>
+      <c r="T44" s="48"/>
+      <c r="U44" s="48"/>
+      <c r="V44" s="48"/>
+      <c r="W44" s="49"/>
       <c r="X44" s="12"/>
       <c r="Y44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z44" s="43">
+      <c r="Z44" s="47">
         <f>AC43+Z20</f>
         <v>0</v>
       </c>
-      <c r="AA44" s="44"/>
-      <c r="AB44" s="44"/>
-      <c r="AC44" s="44"/>
-      <c r="AD44" s="44"/>
-      <c r="AE44" s="45"/>
+      <c r="AA44" s="48"/>
+      <c r="AB44" s="48"/>
+      <c r="AC44" s="48"/>
+      <c r="AD44" s="48"/>
+      <c r="AE44" s="49"/>
       <c r="AF44" s="12"/>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="43">
+      <c r="B45" s="47">
         <f>C43+B20</f>
-        <v>2.3464924375000002</v>
-      </c>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="45"/>
+        <v>1.7964924375</v>
+      </c>
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="49"/>
       <c r="H45" s="12"/>
       <c r="I45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J45" s="43">
+      <c r="J45" s="47">
         <f>K43+J20</f>
         <v>0</v>
       </c>
-      <c r="K45" s="44"/>
-      <c r="L45" s="44"/>
-      <c r="M45" s="44"/>
-      <c r="N45" s="44"/>
-      <c r="O45" s="45"/>
+      <c r="K45" s="48"/>
+      <c r="L45" s="48"/>
+      <c r="M45" s="48"/>
+      <c r="N45" s="48"/>
+      <c r="O45" s="49"/>
       <c r="P45" s="12"/>
       <c r="Q45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R45" s="43">
+      <c r="R45" s="47">
         <f>S43+R20</f>
         <v>0</v>
       </c>
-      <c r="S45" s="44"/>
-      <c r="T45" s="44"/>
-      <c r="U45" s="44"/>
-      <c r="V45" s="44"/>
-      <c r="W45" s="45"/>
+      <c r="S45" s="48"/>
+      <c r="T45" s="48"/>
+      <c r="U45" s="48"/>
+      <c r="V45" s="48"/>
+      <c r="W45" s="49"/>
       <c r="X45" s="12"/>
       <c r="Y45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z45" s="43">
+      <c r="Z45" s="47">
         <f>AA43+Z20</f>
         <v>0</v>
       </c>
-      <c r="AA45" s="44"/>
-      <c r="AB45" s="44"/>
-      <c r="AC45" s="44"/>
-      <c r="AD45" s="44"/>
-      <c r="AE45" s="45"/>
+      <c r="AA45" s="48"/>
+      <c r="AB45" s="48"/>
+      <c r="AC45" s="48"/>
+      <c r="AD45" s="48"/>
+      <c r="AE45" s="49"/>
       <c r="AF45" s="12"/>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="43">
+      <c r="B46" s="47">
         <f>IFERROR((G43/10/B44),0)</f>
-        <v>0.5917102966075366</v>
-      </c>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="45"/>
+        <v>0.4177067298338254</v>
+      </c>
+      <c r="C46" s="48"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="49"/>
       <c r="H46" s="12"/>
       <c r="I46" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J46" s="43">
+      <c r="J46" s="47">
         <f>IFERROR((O43/10/J44),0)</f>
         <v>0</v>
       </c>
-      <c r="K46" s="44"/>
-      <c r="L46" s="44"/>
-      <c r="M46" s="44"/>
-      <c r="N46" s="44"/>
-      <c r="O46" s="45"/>
+      <c r="K46" s="48"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="48"/>
+      <c r="N46" s="48"/>
+      <c r="O46" s="49"/>
       <c r="P46" s="12"/>
       <c r="Q46" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R46" s="43">
+      <c r="R46" s="47">
         <f>IFERROR((W43/10/R44),0)</f>
         <v>0</v>
       </c>
-      <c r="S46" s="44"/>
-      <c r="T46" s="44"/>
-      <c r="U46" s="44"/>
-      <c r="V46" s="44"/>
-      <c r="W46" s="45"/>
+      <c r="S46" s="48"/>
+      <c r="T46" s="48"/>
+      <c r="U46" s="48"/>
+      <c r="V46" s="48"/>
+      <c r="W46" s="49"/>
       <c r="X46" s="12"/>
       <c r="Y46" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z46" s="43">
+      <c r="Z46" s="47">
         <f>IFERROR((AE43/10/Z44),0)</f>
         <v>0</v>
       </c>
-      <c r="AA46" s="44"/>
-      <c r="AB46" s="44"/>
-      <c r="AC46" s="44"/>
-      <c r="AD46" s="44"/>
-      <c r="AE46" s="45"/>
+      <c r="AA46" s="48"/>
+      <c r="AB46" s="48"/>
+      <c r="AC46" s="48"/>
+      <c r="AD46" s="48"/>
+      <c r="AE46" s="49"/>
       <c r="AF46" s="12"/>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="43">
+      <c r="B47" s="47">
         <f>IFERROR((9.82 * F43) * LN(B44/B45),0)</f>
-        <v>7032.4499171096795</v>
-      </c>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="45"/>
+        <v>8003.3365648910458</v>
+      </c>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="49"/>
       <c r="H47" s="12"/>
       <c r="I47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J47" s="43">
+      <c r="J47" s="47">
         <f>IFERROR((9.82 * N43) * LN(J44/J45),0)</f>
         <v>0</v>
       </c>
-      <c r="K47" s="44"/>
-      <c r="L47" s="44"/>
-      <c r="M47" s="44"/>
-      <c r="N47" s="44"/>
-      <c r="O47" s="45"/>
+      <c r="K47" s="48"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="48"/>
+      <c r="N47" s="48"/>
+      <c r="O47" s="49"/>
       <c r="P47" s="12"/>
       <c r="Q47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R47" s="43">
+      <c r="R47" s="47">
         <f>IFERROR((9.82 * V43) * LN(R44/R45),0)</f>
         <v>0</v>
       </c>
-      <c r="S47" s="44"/>
-      <c r="T47" s="44"/>
-      <c r="U47" s="44"/>
-      <c r="V47" s="44"/>
-      <c r="W47" s="45"/>
+      <c r="S47" s="48"/>
+      <c r="T47" s="48"/>
+      <c r="U47" s="48"/>
+      <c r="V47" s="48"/>
+      <c r="W47" s="49"/>
       <c r="X47" s="12"/>
       <c r="Y47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z47" s="43">
+      <c r="Z47" s="47">
         <f>IFERROR((9.82 * AD43) * LN(Z44/Z45),0)</f>
         <v>0</v>
       </c>
-      <c r="AA47" s="44"/>
-      <c r="AB47" s="44"/>
-      <c r="AC47" s="44"/>
-      <c r="AD47" s="44"/>
-      <c r="AE47" s="45"/>
+      <c r="AA47" s="48"/>
+      <c r="AB47" s="48"/>
+      <c r="AC47" s="48"/>
+      <c r="AD47" s="48"/>
+      <c r="AE47" s="49"/>
       <c r="AF47" s="12"/>
     </row>
     <row r="48" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B48" s="40">
+      <c r="B48" s="51">
         <f>B47+B24</f>
-        <v>7032.4499171096795</v>
-      </c>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="42"/>
+        <v>8003.3365648910458</v>
+      </c>
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="53"/>
       <c r="H48" s="12"/>
       <c r="I48" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J48" s="40">
+      <c r="J48" s="51">
         <f>J47+J24</f>
         <v>0</v>
       </c>
-      <c r="K48" s="41"/>
-      <c r="L48" s="41"/>
-      <c r="M48" s="41"/>
-      <c r="N48" s="41"/>
-      <c r="O48" s="42"/>
+      <c r="K48" s="52"/>
+      <c r="L48" s="52"/>
+      <c r="M48" s="52"/>
+      <c r="N48" s="52"/>
+      <c r="O48" s="53"/>
       <c r="P48" s="12"/>
       <c r="Q48" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R48" s="40">
+      <c r="R48" s="51">
         <f>R47+R24</f>
         <v>0</v>
       </c>
-      <c r="S48" s="41"/>
-      <c r="T48" s="41"/>
-      <c r="U48" s="41"/>
-      <c r="V48" s="41"/>
-      <c r="W48" s="42"/>
+      <c r="S48" s="52"/>
+      <c r="T48" s="52"/>
+      <c r="U48" s="52"/>
+      <c r="V48" s="52"/>
+      <c r="W48" s="53"/>
       <c r="X48" s="12"/>
       <c r="Y48" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z48" s="40">
+      <c r="Z48" s="51">
         <f>Z47+Z24</f>
         <v>0</v>
       </c>
-      <c r="AA48" s="41"/>
-      <c r="AB48" s="41"/>
-      <c r="AC48" s="41"/>
-      <c r="AD48" s="41"/>
-      <c r="AE48" s="42"/>
+      <c r="AA48" s="52"/>
+      <c r="AB48" s="52"/>
+      <c r="AC48" s="52"/>
+      <c r="AD48" s="52"/>
+      <c r="AE48" s="53"/>
       <c r="AF48" s="12"/>
     </row>
     <row r="49" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33581,270 +33583,270 @@
       <c r="A68" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="43">
+      <c r="B68" s="47">
         <f>E67+B44</f>
-        <v>11.323108687500001</v>
-      </c>
-      <c r="C68" s="44"/>
-      <c r="D68" s="44"/>
-      <c r="E68" s="44"/>
-      <c r="F68" s="44"/>
-      <c r="G68" s="45"/>
+        <v>10.773108687500001</v>
+      </c>
+      <c r="C68" s="48"/>
+      <c r="D68" s="48"/>
+      <c r="E68" s="48"/>
+      <c r="F68" s="48"/>
+      <c r="G68" s="49"/>
       <c r="H68" s="12"/>
       <c r="I68" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J68" s="43">
+      <c r="J68" s="47">
         <f>M67+J44</f>
         <v>0</v>
       </c>
-      <c r="K68" s="44"/>
-      <c r="L68" s="44"/>
-      <c r="M68" s="44"/>
-      <c r="N68" s="44"/>
-      <c r="O68" s="45"/>
+      <c r="K68" s="48"/>
+      <c r="L68" s="48"/>
+      <c r="M68" s="48"/>
+      <c r="N68" s="48"/>
+      <c r="O68" s="49"/>
       <c r="P68" s="12"/>
       <c r="Q68" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R68" s="43">
+      <c r="R68" s="47">
         <f>U67+R44</f>
         <v>0</v>
       </c>
-      <c r="S68" s="44"/>
-      <c r="T68" s="44"/>
-      <c r="U68" s="44"/>
-      <c r="V68" s="44"/>
-      <c r="W68" s="45"/>
+      <c r="S68" s="48"/>
+      <c r="T68" s="48"/>
+      <c r="U68" s="48"/>
+      <c r="V68" s="48"/>
+      <c r="W68" s="49"/>
       <c r="X68" s="12"/>
       <c r="Y68" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z68" s="43">
+      <c r="Z68" s="47">
         <f>AC67+Z44</f>
         <v>0</v>
       </c>
-      <c r="AA68" s="44"/>
-      <c r="AB68" s="44"/>
-      <c r="AC68" s="44"/>
-      <c r="AD68" s="44"/>
-      <c r="AE68" s="45"/>
+      <c r="AA68" s="48"/>
+      <c r="AB68" s="48"/>
+      <c r="AC68" s="48"/>
+      <c r="AD68" s="48"/>
+      <c r="AE68" s="49"/>
       <c r="AF68" s="12"/>
     </row>
     <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="43">
+      <c r="B69" s="47">
         <f>C67+B44</f>
-        <v>11.323108687500001</v>
-      </c>
-      <c r="C69" s="44"/>
-      <c r="D69" s="44"/>
-      <c r="E69" s="44"/>
-      <c r="F69" s="44"/>
-      <c r="G69" s="45"/>
+        <v>10.773108687500001</v>
+      </c>
+      <c r="C69" s="48"/>
+      <c r="D69" s="48"/>
+      <c r="E69" s="48"/>
+      <c r="F69" s="48"/>
+      <c r="G69" s="49"/>
       <c r="H69" s="12"/>
       <c r="I69" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J69" s="43">
+      <c r="J69" s="47">
         <f>K67+J44</f>
         <v>0</v>
       </c>
-      <c r="K69" s="44"/>
-      <c r="L69" s="44"/>
-      <c r="M69" s="44"/>
-      <c r="N69" s="44"/>
-      <c r="O69" s="45"/>
+      <c r="K69" s="48"/>
+      <c r="L69" s="48"/>
+      <c r="M69" s="48"/>
+      <c r="N69" s="48"/>
+      <c r="O69" s="49"/>
       <c r="P69" s="12"/>
       <c r="Q69" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R69" s="43">
+      <c r="R69" s="47">
         <f>S67+R44</f>
         <v>0</v>
       </c>
-      <c r="S69" s="44"/>
-      <c r="T69" s="44"/>
-      <c r="U69" s="44"/>
-      <c r="V69" s="44"/>
-      <c r="W69" s="45"/>
+      <c r="S69" s="48"/>
+      <c r="T69" s="48"/>
+      <c r="U69" s="48"/>
+      <c r="V69" s="48"/>
+      <c r="W69" s="49"/>
       <c r="X69" s="12"/>
       <c r="Y69" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z69" s="43">
+      <c r="Z69" s="47">
         <f>AA67+Z44</f>
         <v>0</v>
       </c>
-      <c r="AA69" s="44"/>
-      <c r="AB69" s="44"/>
-      <c r="AC69" s="44"/>
-      <c r="AD69" s="44"/>
-      <c r="AE69" s="45"/>
+      <c r="AA69" s="48"/>
+      <c r="AB69" s="48"/>
+      <c r="AC69" s="48"/>
+      <c r="AD69" s="48"/>
+      <c r="AE69" s="49"/>
       <c r="AF69" s="12"/>
     </row>
     <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B70" s="43">
+      <c r="B70" s="47">
         <f>IFERROR((G67/10/B68),0)</f>
         <v>0</v>
       </c>
-      <c r="C70" s="44"/>
-      <c r="D70" s="44"/>
-      <c r="E70" s="44"/>
-      <c r="F70" s="44"/>
-      <c r="G70" s="45"/>
+      <c r="C70" s="48"/>
+      <c r="D70" s="48"/>
+      <c r="E70" s="48"/>
+      <c r="F70" s="48"/>
+      <c r="G70" s="49"/>
       <c r="H70" s="12"/>
       <c r="I70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J70" s="43">
+      <c r="J70" s="47">
         <f>IFERROR((O67/10/J68),0)</f>
         <v>0</v>
       </c>
-      <c r="K70" s="44"/>
-      <c r="L70" s="44"/>
-      <c r="M70" s="44"/>
-      <c r="N70" s="44"/>
-      <c r="O70" s="45"/>
+      <c r="K70" s="48"/>
+      <c r="L70" s="48"/>
+      <c r="M70" s="48"/>
+      <c r="N70" s="48"/>
+      <c r="O70" s="49"/>
       <c r="P70" s="12"/>
       <c r="Q70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R70" s="43">
+      <c r="R70" s="47">
         <f>IFERROR((W67/10/R68),0)</f>
         <v>0</v>
       </c>
-      <c r="S70" s="44"/>
-      <c r="T70" s="44"/>
-      <c r="U70" s="44"/>
-      <c r="V70" s="44"/>
-      <c r="W70" s="45"/>
+      <c r="S70" s="48"/>
+      <c r="T70" s="48"/>
+      <c r="U70" s="48"/>
+      <c r="V70" s="48"/>
+      <c r="W70" s="49"/>
       <c r="X70" s="12"/>
       <c r="Y70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z70" s="43">
+      <c r="Z70" s="47">
         <f>IFERROR((AE67/10/Z68),0)</f>
         <v>0</v>
       </c>
-      <c r="AA70" s="44"/>
-      <c r="AB70" s="44"/>
-      <c r="AC70" s="44"/>
-      <c r="AD70" s="44"/>
-      <c r="AE70" s="45"/>
+      <c r="AA70" s="48"/>
+      <c r="AB70" s="48"/>
+      <c r="AC70" s="48"/>
+      <c r="AD70" s="48"/>
+      <c r="AE70" s="49"/>
       <c r="AF70" s="12"/>
     </row>
     <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="43">
+      <c r="B71" s="47">
         <f>IFERROR((9.82 * F67) * LN(B68/B69),0)</f>
         <v>0</v>
       </c>
-      <c r="C71" s="44"/>
-      <c r="D71" s="44"/>
-      <c r="E71" s="44"/>
-      <c r="F71" s="44"/>
-      <c r="G71" s="45"/>
+      <c r="C71" s="48"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="48"/>
+      <c r="F71" s="48"/>
+      <c r="G71" s="49"/>
       <c r="H71" s="12"/>
       <c r="I71" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J71" s="43">
+      <c r="J71" s="47">
         <f>IFERROR((9.82 * N67) * LN(J68/J69),0)</f>
         <v>0</v>
       </c>
-      <c r="K71" s="44"/>
-      <c r="L71" s="44"/>
-      <c r="M71" s="44"/>
-      <c r="N71" s="44"/>
-      <c r="O71" s="45"/>
+      <c r="K71" s="48"/>
+      <c r="L71" s="48"/>
+      <c r="M71" s="48"/>
+      <c r="N71" s="48"/>
+      <c r="O71" s="49"/>
       <c r="P71" s="12"/>
       <c r="Q71" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R71" s="43">
+      <c r="R71" s="47">
         <f>IFERROR((9.82 * V67) * LN(R68/R69),0)</f>
         <v>0</v>
       </c>
-      <c r="S71" s="44"/>
-      <c r="T71" s="44"/>
-      <c r="U71" s="44"/>
-      <c r="V71" s="44"/>
-      <c r="W71" s="45"/>
+      <c r="S71" s="48"/>
+      <c r="T71" s="48"/>
+      <c r="U71" s="48"/>
+      <c r="V71" s="48"/>
+      <c r="W71" s="49"/>
       <c r="X71" s="12"/>
       <c r="Y71" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z71" s="43">
+      <c r="Z71" s="47">
         <f>IFERROR((9.82 * AD67) * LN(Z68/Z69),0)</f>
         <v>0</v>
       </c>
-      <c r="AA71" s="44"/>
-      <c r="AB71" s="44"/>
-      <c r="AC71" s="44"/>
-      <c r="AD71" s="44"/>
-      <c r="AE71" s="45"/>
+      <c r="AA71" s="48"/>
+      <c r="AB71" s="48"/>
+      <c r="AC71" s="48"/>
+      <c r="AD71" s="48"/>
+      <c r="AE71" s="49"/>
       <c r="AF71" s="12"/>
     </row>
     <row r="72" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="40">
+      <c r="B72" s="51">
         <f>B71+B48</f>
-        <v>7032.4499171096795</v>
-      </c>
-      <c r="C72" s="41"/>
-      <c r="D72" s="41"/>
-      <c r="E72" s="41"/>
-      <c r="F72" s="41"/>
-      <c r="G72" s="42"/>
+        <v>8003.3365648910458</v>
+      </c>
+      <c r="C72" s="52"/>
+      <c r="D72" s="52"/>
+      <c r="E72" s="52"/>
+      <c r="F72" s="52"/>
+      <c r="G72" s="53"/>
       <c r="H72" s="12"/>
       <c r="I72" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J72" s="40">
+      <c r="J72" s="51">
         <f>J71+J48</f>
         <v>0</v>
       </c>
-      <c r="K72" s="41"/>
-      <c r="L72" s="41"/>
-      <c r="M72" s="41"/>
-      <c r="N72" s="41"/>
-      <c r="O72" s="42"/>
+      <c r="K72" s="52"/>
+      <c r="L72" s="52"/>
+      <c r="M72" s="52"/>
+      <c r="N72" s="52"/>
+      <c r="O72" s="53"/>
       <c r="P72" s="12"/>
       <c r="Q72" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R72" s="40">
+      <c r="R72" s="51">
         <f>R71+R48</f>
         <v>0</v>
       </c>
-      <c r="S72" s="41"/>
-      <c r="T72" s="41"/>
-      <c r="U72" s="41"/>
-      <c r="V72" s="41"/>
-      <c r="W72" s="42"/>
+      <c r="S72" s="52"/>
+      <c r="T72" s="52"/>
+      <c r="U72" s="52"/>
+      <c r="V72" s="52"/>
+      <c r="W72" s="53"/>
       <c r="X72" s="12"/>
       <c r="Y72" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z72" s="40">
+      <c r="Z72" s="51">
         <f>Z71+Z48</f>
         <v>0</v>
       </c>
-      <c r="AA72" s="41"/>
-      <c r="AB72" s="41"/>
-      <c r="AC72" s="41"/>
-      <c r="AD72" s="41"/>
-      <c r="AE72" s="42"/>
+      <c r="AA72" s="52"/>
+      <c r="AB72" s="52"/>
+      <c r="AC72" s="52"/>
+      <c r="AD72" s="52"/>
+      <c r="AE72" s="53"/>
       <c r="AF72" s="12"/>
     </row>
     <row r="73" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -35581,270 +35583,270 @@
       <c r="A92" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B92" s="43">
+      <c r="B92" s="47">
         <f>E91+B68</f>
-        <v>11.323108687500001</v>
-      </c>
-      <c r="C92" s="44"/>
-      <c r="D92" s="44"/>
-      <c r="E92" s="44"/>
-      <c r="F92" s="44"/>
-      <c r="G92" s="45"/>
+        <v>10.773108687500001</v>
+      </c>
+      <c r="C92" s="48"/>
+      <c r="D92" s="48"/>
+      <c r="E92" s="48"/>
+      <c r="F92" s="48"/>
+      <c r="G92" s="49"/>
       <c r="H92" s="12"/>
       <c r="I92" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J92" s="43">
+      <c r="J92" s="47">
         <f>M91+J68</f>
         <v>0</v>
       </c>
-      <c r="K92" s="44"/>
-      <c r="L92" s="44"/>
-      <c r="M92" s="44"/>
-      <c r="N92" s="44"/>
-      <c r="O92" s="45"/>
+      <c r="K92" s="48"/>
+      <c r="L92" s="48"/>
+      <c r="M92" s="48"/>
+      <c r="N92" s="48"/>
+      <c r="O92" s="49"/>
       <c r="P92" s="12"/>
       <c r="Q92" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R92" s="43">
+      <c r="R92" s="47">
         <f>U91+R68</f>
         <v>0</v>
       </c>
-      <c r="S92" s="44"/>
-      <c r="T92" s="44"/>
-      <c r="U92" s="44"/>
-      <c r="V92" s="44"/>
-      <c r="W92" s="45"/>
+      <c r="S92" s="48"/>
+      <c r="T92" s="48"/>
+      <c r="U92" s="48"/>
+      <c r="V92" s="48"/>
+      <c r="W92" s="49"/>
       <c r="X92" s="12"/>
       <c r="Y92" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z92" s="43">
+      <c r="Z92" s="47">
         <f>AC91+Z68</f>
         <v>0</v>
       </c>
-      <c r="AA92" s="44"/>
-      <c r="AB92" s="44"/>
-      <c r="AC92" s="44"/>
-      <c r="AD92" s="44"/>
-      <c r="AE92" s="45"/>
+      <c r="AA92" s="48"/>
+      <c r="AB92" s="48"/>
+      <c r="AC92" s="48"/>
+      <c r="AD92" s="48"/>
+      <c r="AE92" s="49"/>
       <c r="AF92" s="12"/>
     </row>
     <row r="93" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A93" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B93" s="43">
+      <c r="B93" s="47">
         <f>C91+B68</f>
-        <v>11.323108687500001</v>
-      </c>
-      <c r="C93" s="44"/>
-      <c r="D93" s="44"/>
-      <c r="E93" s="44"/>
-      <c r="F93" s="44"/>
-      <c r="G93" s="45"/>
+        <v>10.773108687500001</v>
+      </c>
+      <c r="C93" s="48"/>
+      <c r="D93" s="48"/>
+      <c r="E93" s="48"/>
+      <c r="F93" s="48"/>
+      <c r="G93" s="49"/>
       <c r="H93" s="12"/>
       <c r="I93" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J93" s="43">
+      <c r="J93" s="47">
         <f>K91+J68</f>
         <v>0</v>
       </c>
-      <c r="K93" s="44"/>
-      <c r="L93" s="44"/>
-      <c r="M93" s="44"/>
-      <c r="N93" s="44"/>
-      <c r="O93" s="45"/>
+      <c r="K93" s="48"/>
+      <c r="L93" s="48"/>
+      <c r="M93" s="48"/>
+      <c r="N93" s="48"/>
+      <c r="O93" s="49"/>
       <c r="P93" s="12"/>
       <c r="Q93" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R93" s="43">
+      <c r="R93" s="47">
         <f>S91+R68</f>
         <v>0</v>
       </c>
-      <c r="S93" s="44"/>
-      <c r="T93" s="44"/>
-      <c r="U93" s="44"/>
-      <c r="V93" s="44"/>
-      <c r="W93" s="45"/>
+      <c r="S93" s="48"/>
+      <c r="T93" s="48"/>
+      <c r="U93" s="48"/>
+      <c r="V93" s="48"/>
+      <c r="W93" s="49"/>
       <c r="X93" s="12"/>
       <c r="Y93" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z93" s="43">
+      <c r="Z93" s="47">
         <f>AA91+Z68</f>
         <v>0</v>
       </c>
-      <c r="AA93" s="44"/>
-      <c r="AB93" s="44"/>
-      <c r="AC93" s="44"/>
-      <c r="AD93" s="44"/>
-      <c r="AE93" s="45"/>
+      <c r="AA93" s="48"/>
+      <c r="AB93" s="48"/>
+      <c r="AC93" s="48"/>
+      <c r="AD93" s="48"/>
+      <c r="AE93" s="49"/>
       <c r="AF93" s="12"/>
     </row>
     <row r="94" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A94" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B94" s="43">
+      <c r="B94" s="47">
         <f>IFERROR((G91/10/B92),0)</f>
         <v>0</v>
       </c>
-      <c r="C94" s="44"/>
-      <c r="D94" s="44"/>
-      <c r="E94" s="44"/>
-      <c r="F94" s="44"/>
-      <c r="G94" s="45"/>
+      <c r="C94" s="48"/>
+      <c r="D94" s="48"/>
+      <c r="E94" s="48"/>
+      <c r="F94" s="48"/>
+      <c r="G94" s="49"/>
       <c r="H94" s="12"/>
       <c r="I94" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J94" s="43">
+      <c r="J94" s="47">
         <f>IFERROR((O91/10/J92),0)</f>
         <v>0</v>
       </c>
-      <c r="K94" s="44"/>
-      <c r="L94" s="44"/>
-      <c r="M94" s="44"/>
-      <c r="N94" s="44"/>
-      <c r="O94" s="45"/>
+      <c r="K94" s="48"/>
+      <c r="L94" s="48"/>
+      <c r="M94" s="48"/>
+      <c r="N94" s="48"/>
+      <c r="O94" s="49"/>
       <c r="P94" s="12"/>
       <c r="Q94" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R94" s="43">
+      <c r="R94" s="47">
         <f>IFERROR((W91/10/R92),0)</f>
         <v>0</v>
       </c>
-      <c r="S94" s="44"/>
-      <c r="T94" s="44"/>
-      <c r="U94" s="44"/>
-      <c r="V94" s="44"/>
-      <c r="W94" s="45"/>
+      <c r="S94" s="48"/>
+      <c r="T94" s="48"/>
+      <c r="U94" s="48"/>
+      <c r="V94" s="48"/>
+      <c r="W94" s="49"/>
       <c r="X94" s="12"/>
       <c r="Y94" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z94" s="43">
+      <c r="Z94" s="47">
         <f>IFERROR((AE91/10/Z92),0)</f>
         <v>0</v>
       </c>
-      <c r="AA94" s="44"/>
-      <c r="AB94" s="44"/>
-      <c r="AC94" s="44"/>
-      <c r="AD94" s="44"/>
-      <c r="AE94" s="45"/>
+      <c r="AA94" s="48"/>
+      <c r="AB94" s="48"/>
+      <c r="AC94" s="48"/>
+      <c r="AD94" s="48"/>
+      <c r="AE94" s="49"/>
       <c r="AF94" s="12"/>
     </row>
     <row r="95" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A95" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B95" s="43">
+      <c r="B95" s="47">
         <f>IFERROR((9.82 * F91) * LN(B92/B93),0)</f>
         <v>0</v>
       </c>
-      <c r="C95" s="44"/>
-      <c r="D95" s="44"/>
-      <c r="E95" s="44"/>
-      <c r="F95" s="44"/>
-      <c r="G95" s="45"/>
+      <c r="C95" s="48"/>
+      <c r="D95" s="48"/>
+      <c r="E95" s="48"/>
+      <c r="F95" s="48"/>
+      <c r="G95" s="49"/>
       <c r="H95" s="12"/>
       <c r="I95" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J95" s="43">
+      <c r="J95" s="47">
         <f>IFERROR((9.82 * N91) * LN(J92/J93),0)</f>
         <v>0</v>
       </c>
-      <c r="K95" s="44"/>
-      <c r="L95" s="44"/>
-      <c r="M95" s="44"/>
-      <c r="N95" s="44"/>
-      <c r="O95" s="45"/>
+      <c r="K95" s="48"/>
+      <c r="L95" s="48"/>
+      <c r="M95" s="48"/>
+      <c r="N95" s="48"/>
+      <c r="O95" s="49"/>
       <c r="P95" s="12"/>
       <c r="Q95" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R95" s="43">
+      <c r="R95" s="47">
         <f>IFERROR((9.82 * V91) * LN(R92/R93),0)</f>
         <v>0</v>
       </c>
-      <c r="S95" s="44"/>
-      <c r="T95" s="44"/>
-      <c r="U95" s="44"/>
-      <c r="V95" s="44"/>
-      <c r="W95" s="45"/>
+      <c r="S95" s="48"/>
+      <c r="T95" s="48"/>
+      <c r="U95" s="48"/>
+      <c r="V95" s="48"/>
+      <c r="W95" s="49"/>
       <c r="X95" s="12"/>
       <c r="Y95" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z95" s="43">
+      <c r="Z95" s="47">
         <f>IFERROR((9.82 * AD91) * LN(Z92/Z93),0)</f>
         <v>0</v>
       </c>
-      <c r="AA95" s="44"/>
-      <c r="AB95" s="44"/>
-      <c r="AC95" s="44"/>
-      <c r="AD95" s="44"/>
-      <c r="AE95" s="45"/>
+      <c r="AA95" s="48"/>
+      <c r="AB95" s="48"/>
+      <c r="AC95" s="48"/>
+      <c r="AD95" s="48"/>
+      <c r="AE95" s="49"/>
       <c r="AF95" s="12"/>
     </row>
     <row r="96" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B96" s="40">
+      <c r="B96" s="51">
         <f>B95+B72</f>
-        <v>7032.4499171096795</v>
-      </c>
-      <c r="C96" s="41"/>
-      <c r="D96" s="41"/>
-      <c r="E96" s="41"/>
-      <c r="F96" s="41"/>
-      <c r="G96" s="42"/>
+        <v>8003.3365648910458</v>
+      </c>
+      <c r="C96" s="52"/>
+      <c r="D96" s="52"/>
+      <c r="E96" s="52"/>
+      <c r="F96" s="52"/>
+      <c r="G96" s="53"/>
       <c r="H96" s="12"/>
       <c r="I96" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J96" s="40">
+      <c r="J96" s="51">
         <f>J95+J72</f>
         <v>0</v>
       </c>
-      <c r="K96" s="41"/>
-      <c r="L96" s="41"/>
-      <c r="M96" s="41"/>
-      <c r="N96" s="41"/>
-      <c r="O96" s="42"/>
+      <c r="K96" s="52"/>
+      <c r="L96" s="52"/>
+      <c r="M96" s="52"/>
+      <c r="N96" s="52"/>
+      <c r="O96" s="53"/>
       <c r="P96" s="12"/>
       <c r="Q96" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R96" s="40">
+      <c r="R96" s="51">
         <f>R95+R72</f>
         <v>0</v>
       </c>
-      <c r="S96" s="41"/>
-      <c r="T96" s="41"/>
-      <c r="U96" s="41"/>
-      <c r="V96" s="41"/>
-      <c r="W96" s="42"/>
+      <c r="S96" s="52"/>
+      <c r="T96" s="52"/>
+      <c r="U96" s="52"/>
+      <c r="V96" s="52"/>
+      <c r="W96" s="53"/>
       <c r="X96" s="12"/>
       <c r="Y96" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z96" s="40">
+      <c r="Z96" s="51">
         <f>Z95+Z72</f>
         <v>0</v>
       </c>
-      <c r="AA96" s="41"/>
-      <c r="AB96" s="41"/>
-      <c r="AC96" s="41"/>
-      <c r="AD96" s="41"/>
-      <c r="AE96" s="42"/>
+      <c r="AA96" s="52"/>
+      <c r="AB96" s="52"/>
+      <c r="AC96" s="52"/>
+      <c r="AD96" s="52"/>
+      <c r="AE96" s="53"/>
       <c r="AF96" s="12"/>
     </row>
     <row r="97" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -37581,270 +37583,270 @@
       <c r="A116" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B116" s="43">
+      <c r="B116" s="47">
         <f>E115+B92</f>
-        <v>11.323108687500001</v>
-      </c>
-      <c r="C116" s="44"/>
-      <c r="D116" s="44"/>
-      <c r="E116" s="44"/>
-      <c r="F116" s="44"/>
-      <c r="G116" s="45"/>
+        <v>10.773108687500001</v>
+      </c>
+      <c r="C116" s="48"/>
+      <c r="D116" s="48"/>
+      <c r="E116" s="48"/>
+      <c r="F116" s="48"/>
+      <c r="G116" s="49"/>
       <c r="H116" s="12"/>
       <c r="I116" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J116" s="43">
+      <c r="J116" s="47">
         <f>M115+J92</f>
         <v>0</v>
       </c>
-      <c r="K116" s="44"/>
-      <c r="L116" s="44"/>
-      <c r="M116" s="44"/>
-      <c r="N116" s="44"/>
-      <c r="O116" s="45"/>
+      <c r="K116" s="48"/>
+      <c r="L116" s="48"/>
+      <c r="M116" s="48"/>
+      <c r="N116" s="48"/>
+      <c r="O116" s="49"/>
       <c r="P116" s="12"/>
       <c r="Q116" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R116" s="43">
+      <c r="R116" s="47">
         <f>U115+R92</f>
         <v>0</v>
       </c>
-      <c r="S116" s="44"/>
-      <c r="T116" s="44"/>
-      <c r="U116" s="44"/>
-      <c r="V116" s="44"/>
-      <c r="W116" s="45"/>
+      <c r="S116" s="48"/>
+      <c r="T116" s="48"/>
+      <c r="U116" s="48"/>
+      <c r="V116" s="48"/>
+      <c r="W116" s="49"/>
       <c r="X116" s="12"/>
       <c r="Y116" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z116" s="43">
+      <c r="Z116" s="47">
         <f>AC115+Z92</f>
         <v>0</v>
       </c>
-      <c r="AA116" s="44"/>
-      <c r="AB116" s="44"/>
-      <c r="AC116" s="44"/>
-      <c r="AD116" s="44"/>
-      <c r="AE116" s="45"/>
+      <c r="AA116" s="48"/>
+      <c r="AB116" s="48"/>
+      <c r="AC116" s="48"/>
+      <c r="AD116" s="48"/>
+      <c r="AE116" s="49"/>
       <c r="AF116" s="12"/>
     </row>
     <row r="117" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A117" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B117" s="43">
+      <c r="B117" s="47">
         <f>C115+B92</f>
-        <v>11.323108687500001</v>
-      </c>
-      <c r="C117" s="44"/>
-      <c r="D117" s="44"/>
-      <c r="E117" s="44"/>
-      <c r="F117" s="44"/>
-      <c r="G117" s="45"/>
+        <v>10.773108687500001</v>
+      </c>
+      <c r="C117" s="48"/>
+      <c r="D117" s="48"/>
+      <c r="E117" s="48"/>
+      <c r="F117" s="48"/>
+      <c r="G117" s="49"/>
       <c r="H117" s="12"/>
       <c r="I117" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J117" s="43">
+      <c r="J117" s="47">
         <f>K115+J92</f>
         <v>0</v>
       </c>
-      <c r="K117" s="44"/>
-      <c r="L117" s="44"/>
-      <c r="M117" s="44"/>
-      <c r="N117" s="44"/>
-      <c r="O117" s="45"/>
+      <c r="K117" s="48"/>
+      <c r="L117" s="48"/>
+      <c r="M117" s="48"/>
+      <c r="N117" s="48"/>
+      <c r="O117" s="49"/>
       <c r="P117" s="12"/>
       <c r="Q117" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R117" s="43">
+      <c r="R117" s="47">
         <f>S115+R92</f>
         <v>0</v>
       </c>
-      <c r="S117" s="44"/>
-      <c r="T117" s="44"/>
-      <c r="U117" s="44"/>
-      <c r="V117" s="44"/>
-      <c r="W117" s="45"/>
+      <c r="S117" s="48"/>
+      <c r="T117" s="48"/>
+      <c r="U117" s="48"/>
+      <c r="V117" s="48"/>
+      <c r="W117" s="49"/>
       <c r="X117" s="12"/>
       <c r="Y117" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z117" s="43">
+      <c r="Z117" s="47">
         <f>AA115+Z92</f>
         <v>0</v>
       </c>
-      <c r="AA117" s="44"/>
-      <c r="AB117" s="44"/>
-      <c r="AC117" s="44"/>
-      <c r="AD117" s="44"/>
-      <c r="AE117" s="45"/>
+      <c r="AA117" s="48"/>
+      <c r="AB117" s="48"/>
+      <c r="AC117" s="48"/>
+      <c r="AD117" s="48"/>
+      <c r="AE117" s="49"/>
       <c r="AF117" s="12"/>
     </row>
     <row r="118" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A118" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B118" s="43">
+      <c r="B118" s="47">
         <f>IFERROR((G115/10/B116),0)</f>
         <v>0</v>
       </c>
-      <c r="C118" s="44"/>
-      <c r="D118" s="44"/>
-      <c r="E118" s="44"/>
-      <c r="F118" s="44"/>
-      <c r="G118" s="45"/>
+      <c r="C118" s="48"/>
+      <c r="D118" s="48"/>
+      <c r="E118" s="48"/>
+      <c r="F118" s="48"/>
+      <c r="G118" s="49"/>
       <c r="H118" s="12"/>
       <c r="I118" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J118" s="43">
+      <c r="J118" s="47">
         <f>IFERROR((O115/10/J116),0)</f>
         <v>0</v>
       </c>
-      <c r="K118" s="44"/>
-      <c r="L118" s="44"/>
-      <c r="M118" s="44"/>
-      <c r="N118" s="44"/>
-      <c r="O118" s="45"/>
+      <c r="K118" s="48"/>
+      <c r="L118" s="48"/>
+      <c r="M118" s="48"/>
+      <c r="N118" s="48"/>
+      <c r="O118" s="49"/>
       <c r="P118" s="12"/>
       <c r="Q118" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R118" s="43">
+      <c r="R118" s="47">
         <f>IFERROR((W115/10/R116),0)</f>
         <v>0</v>
       </c>
-      <c r="S118" s="44"/>
-      <c r="T118" s="44"/>
-      <c r="U118" s="44"/>
-      <c r="V118" s="44"/>
-      <c r="W118" s="45"/>
+      <c r="S118" s="48"/>
+      <c r="T118" s="48"/>
+      <c r="U118" s="48"/>
+      <c r="V118" s="48"/>
+      <c r="W118" s="49"/>
       <c r="X118" s="12"/>
       <c r="Y118" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z118" s="43">
+      <c r="Z118" s="47">
         <f>IFERROR((AE115/10/Z116),0)</f>
         <v>0</v>
       </c>
-      <c r="AA118" s="44"/>
-      <c r="AB118" s="44"/>
-      <c r="AC118" s="44"/>
-      <c r="AD118" s="44"/>
-      <c r="AE118" s="45"/>
+      <c r="AA118" s="48"/>
+      <c r="AB118" s="48"/>
+      <c r="AC118" s="48"/>
+      <c r="AD118" s="48"/>
+      <c r="AE118" s="49"/>
       <c r="AF118" s="12"/>
     </row>
     <row r="119" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A119" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B119" s="43">
+      <c r="B119" s="47">
         <f>IFERROR((9.82 * F115) * LN(B116/B117),0)</f>
         <v>0</v>
       </c>
-      <c r="C119" s="44"/>
-      <c r="D119" s="44"/>
-      <c r="E119" s="44"/>
-      <c r="F119" s="44"/>
-      <c r="G119" s="45"/>
+      <c r="C119" s="48"/>
+      <c r="D119" s="48"/>
+      <c r="E119" s="48"/>
+      <c r="F119" s="48"/>
+      <c r="G119" s="49"/>
       <c r="H119" s="12"/>
       <c r="I119" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J119" s="43">
+      <c r="J119" s="47">
         <f>IFERROR((9.82 * N115) * LN(J116/J117),0)</f>
         <v>0</v>
       </c>
-      <c r="K119" s="44"/>
-      <c r="L119" s="44"/>
-      <c r="M119" s="44"/>
-      <c r="N119" s="44"/>
-      <c r="O119" s="45"/>
+      <c r="K119" s="48"/>
+      <c r="L119" s="48"/>
+      <c r="M119" s="48"/>
+      <c r="N119" s="48"/>
+      <c r="O119" s="49"/>
       <c r="P119" s="12"/>
       <c r="Q119" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R119" s="43">
+      <c r="R119" s="47">
         <f>IFERROR((9.82 * V115) * LN(R116/R117),0)</f>
         <v>0</v>
       </c>
-      <c r="S119" s="44"/>
-      <c r="T119" s="44"/>
-      <c r="U119" s="44"/>
-      <c r="V119" s="44"/>
-      <c r="W119" s="45"/>
+      <c r="S119" s="48"/>
+      <c r="T119" s="48"/>
+      <c r="U119" s="48"/>
+      <c r="V119" s="48"/>
+      <c r="W119" s="49"/>
       <c r="X119" s="12"/>
       <c r="Y119" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z119" s="43">
+      <c r="Z119" s="47">
         <f>IFERROR((9.82 * AD115) * LN(Z116/Z117),0)</f>
         <v>0</v>
       </c>
-      <c r="AA119" s="44"/>
-      <c r="AB119" s="44"/>
-      <c r="AC119" s="44"/>
-      <c r="AD119" s="44"/>
-      <c r="AE119" s="45"/>
+      <c r="AA119" s="48"/>
+      <c r="AB119" s="48"/>
+      <c r="AC119" s="48"/>
+      <c r="AD119" s="48"/>
+      <c r="AE119" s="49"/>
       <c r="AF119" s="12"/>
     </row>
     <row r="120" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B120" s="40">
+      <c r="B120" s="51">
         <f>B119+B96</f>
-        <v>7032.4499171096795</v>
-      </c>
-      <c r="C120" s="41"/>
-      <c r="D120" s="41"/>
-      <c r="E120" s="41"/>
-      <c r="F120" s="41"/>
-      <c r="G120" s="42"/>
+        <v>8003.3365648910458</v>
+      </c>
+      <c r="C120" s="52"/>
+      <c r="D120" s="52"/>
+      <c r="E120" s="52"/>
+      <c r="F120" s="52"/>
+      <c r="G120" s="53"/>
       <c r="H120" s="12"/>
       <c r="I120" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J120" s="40">
+      <c r="J120" s="51">
         <f>J119+J96</f>
         <v>0</v>
       </c>
-      <c r="K120" s="41"/>
-      <c r="L120" s="41"/>
-      <c r="M120" s="41"/>
-      <c r="N120" s="41"/>
-      <c r="O120" s="42"/>
+      <c r="K120" s="52"/>
+      <c r="L120" s="52"/>
+      <c r="M120" s="52"/>
+      <c r="N120" s="52"/>
+      <c r="O120" s="53"/>
       <c r="P120" s="12"/>
       <c r="Q120" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R120" s="40">
+      <c r="R120" s="51">
         <f>R119+R96</f>
         <v>0</v>
       </c>
-      <c r="S120" s="41"/>
-      <c r="T120" s="41"/>
-      <c r="U120" s="41"/>
-      <c r="V120" s="41"/>
-      <c r="W120" s="42"/>
+      <c r="S120" s="52"/>
+      <c r="T120" s="52"/>
+      <c r="U120" s="52"/>
+      <c r="V120" s="52"/>
+      <c r="W120" s="53"/>
       <c r="X120" s="12"/>
       <c r="Y120" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z120" s="40">
+      <c r="Z120" s="51">
         <f>Z119+Z96</f>
         <v>0</v>
       </c>
-      <c r="AA120" s="41"/>
-      <c r="AB120" s="41"/>
-      <c r="AC120" s="41"/>
-      <c r="AD120" s="41"/>
-      <c r="AE120" s="42"/>
+      <c r="AA120" s="52"/>
+      <c r="AB120" s="52"/>
+      <c r="AC120" s="52"/>
+      <c r="AD120" s="52"/>
+      <c r="AE120" s="53"/>
       <c r="AF120" s="12"/>
     </row>
     <row r="121" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -37882,315 +37884,315 @@
       <c r="AF121" s="12"/>
     </row>
     <row r="122" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="47" t="s">
+      <c r="A122" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="B122" s="48"/>
-      <c r="C122" s="48"/>
-      <c r="D122" s="48"/>
-      <c r="E122" s="48"/>
-      <c r="F122" s="48"/>
-      <c r="G122" s="49"/>
+      <c r="B122" s="43"/>
+      <c r="C122" s="43"/>
+      <c r="D122" s="43"/>
+      <c r="E122" s="43"/>
+      <c r="F122" s="43"/>
+      <c r="G122" s="44"/>
       <c r="H122" s="12"/>
-      <c r="I122" s="47" t="s">
+      <c r="I122" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="J122" s="48"/>
-      <c r="K122" s="48"/>
-      <c r="L122" s="48"/>
-      <c r="M122" s="48"/>
-      <c r="N122" s="48"/>
-      <c r="O122" s="49"/>
+      <c r="J122" s="43"/>
+      <c r="K122" s="43"/>
+      <c r="L122" s="43"/>
+      <c r="M122" s="43"/>
+      <c r="N122" s="43"/>
+      <c r="O122" s="44"/>
       <c r="P122" s="12"/>
-      <c r="Q122" s="47" t="s">
+      <c r="Q122" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="R122" s="48"/>
-      <c r="S122" s="48"/>
-      <c r="T122" s="48"/>
-      <c r="U122" s="48"/>
-      <c r="V122" s="48"/>
-      <c r="W122" s="49"/>
+      <c r="R122" s="43"/>
+      <c r="S122" s="43"/>
+      <c r="T122" s="43"/>
+      <c r="U122" s="43"/>
+      <c r="V122" s="43"/>
+      <c r="W122" s="44"/>
       <c r="X122" s="12"/>
-      <c r="Y122" s="47" t="s">
+      <c r="Y122" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="Z122" s="48"/>
-      <c r="AA122" s="48"/>
-      <c r="AB122" s="48"/>
-      <c r="AC122" s="48"/>
-      <c r="AD122" s="48"/>
-      <c r="AE122" s="49"/>
+      <c r="Z122" s="43"/>
+      <c r="AA122" s="43"/>
+      <c r="AB122" s="43"/>
+      <c r="AC122" s="43"/>
+      <c r="AD122" s="43"/>
+      <c r="AE122" s="44"/>
       <c r="AF122" s="12"/>
     </row>
     <row r="123" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A123" s="52" t="s">
+      <c r="A123" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="B123" s="52"/>
-      <c r="C123" s="52"/>
-      <c r="D123" s="51">
+      <c r="B123" s="45"/>
+      <c r="C123" s="45"/>
+      <c r="D123" s="46">
         <f>B115</f>
         <v>3</v>
       </c>
-      <c r="E123" s="51"/>
-      <c r="F123" s="51"/>
-      <c r="G123" s="51"/>
+      <c r="E123" s="46"/>
+      <c r="F123" s="46"/>
+      <c r="G123" s="46"/>
       <c r="H123" s="12"/>
-      <c r="I123" s="52" t="s">
+      <c r="I123" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="J123" s="52"/>
-      <c r="K123" s="52"/>
-      <c r="L123" s="51">
+      <c r="J123" s="45"/>
+      <c r="K123" s="45"/>
+      <c r="L123" s="46">
         <f>J115</f>
         <v>0</v>
       </c>
-      <c r="M123" s="51"/>
-      <c r="N123" s="51"/>
-      <c r="O123" s="51"/>
+      <c r="M123" s="46"/>
+      <c r="N123" s="46"/>
+      <c r="O123" s="46"/>
       <c r="P123" s="12"/>
-      <c r="Q123" s="52" t="s">
+      <c r="Q123" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="R123" s="52"/>
-      <c r="S123" s="52"/>
-      <c r="T123" s="51">
+      <c r="R123" s="45"/>
+      <c r="S123" s="45"/>
+      <c r="T123" s="46">
         <f>R115</f>
         <v>0</v>
       </c>
-      <c r="U123" s="51"/>
-      <c r="V123" s="51"/>
-      <c r="W123" s="51"/>
+      <c r="U123" s="46"/>
+      <c r="V123" s="46"/>
+      <c r="W123" s="46"/>
       <c r="X123" s="12"/>
-      <c r="Y123" s="52" t="s">
+      <c r="Y123" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="Z123" s="52"/>
-      <c r="AA123" s="52"/>
-      <c r="AB123" s="51">
+      <c r="Z123" s="45"/>
+      <c r="AA123" s="45"/>
+      <c r="AB123" s="46">
         <f>Z115</f>
         <v>0</v>
       </c>
-      <c r="AC123" s="51"/>
-      <c r="AD123" s="51"/>
-      <c r="AE123" s="51"/>
+      <c r="AC123" s="46"/>
+      <c r="AD123" s="46"/>
+      <c r="AE123" s="46"/>
       <c r="AF123" s="12"/>
     </row>
     <row r="124" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A124" s="53" t="s">
+      <c r="A124" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B124" s="53"/>
-      <c r="C124" s="53"/>
-      <c r="D124" s="50">
+      <c r="B124" s="40"/>
+      <c r="C124" s="40"/>
+      <c r="D124" s="41">
         <f>B116</f>
-        <v>11.323108687500001</v>
-      </c>
-      <c r="E124" s="50"/>
-      <c r="F124" s="50"/>
-      <c r="G124" s="50"/>
+        <v>10.773108687500001</v>
+      </c>
+      <c r="E124" s="41"/>
+      <c r="F124" s="41"/>
+      <c r="G124" s="41"/>
       <c r="H124" s="12"/>
-      <c r="I124" s="53" t="s">
+      <c r="I124" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="J124" s="53"/>
-      <c r="K124" s="53"/>
-      <c r="L124" s="50">
+      <c r="J124" s="40"/>
+      <c r="K124" s="40"/>
+      <c r="L124" s="41">
         <f>J116</f>
         <v>0</v>
       </c>
-      <c r="M124" s="50"/>
-      <c r="N124" s="50"/>
-      <c r="O124" s="50"/>
+      <c r="M124" s="41"/>
+      <c r="N124" s="41"/>
+      <c r="O124" s="41"/>
       <c r="P124" s="12"/>
-      <c r="Q124" s="53" t="s">
+      <c r="Q124" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="R124" s="53"/>
-      <c r="S124" s="53"/>
-      <c r="T124" s="50">
+      <c r="R124" s="40"/>
+      <c r="S124" s="40"/>
+      <c r="T124" s="41">
         <f>R116</f>
         <v>0</v>
       </c>
-      <c r="U124" s="50"/>
-      <c r="V124" s="50"/>
-      <c r="W124" s="50"/>
+      <c r="U124" s="41"/>
+      <c r="V124" s="41"/>
+      <c r="W124" s="41"/>
       <c r="X124" s="12"/>
-      <c r="Y124" s="53" t="s">
+      <c r="Y124" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="Z124" s="53"/>
-      <c r="AA124" s="53"/>
-      <c r="AB124" s="50">
+      <c r="Z124" s="40"/>
+      <c r="AA124" s="40"/>
+      <c r="AB124" s="41">
         <f>Z116</f>
         <v>0</v>
       </c>
-      <c r="AC124" s="50"/>
-      <c r="AD124" s="50"/>
-      <c r="AE124" s="50"/>
+      <c r="AC124" s="41"/>
+      <c r="AD124" s="41"/>
+      <c r="AE124" s="41"/>
       <c r="AF124" s="12"/>
     </row>
     <row r="125" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A125" s="53" t="s">
+      <c r="A125" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B125" s="53"/>
-      <c r="C125" s="53"/>
-      <c r="D125" s="50">
+      <c r="B125" s="40"/>
+      <c r="C125" s="40"/>
+      <c r="D125" s="41">
         <f>D115+D91+D67+D43+D19</f>
         <v>8.9766162500000011</v>
       </c>
-      <c r="E125" s="50"/>
-      <c r="F125" s="50"/>
-      <c r="G125" s="50"/>
+      <c r="E125" s="41"/>
+      <c r="F125" s="41"/>
+      <c r="G125" s="41"/>
       <c r="H125" s="12"/>
-      <c r="I125" s="53" t="s">
+      <c r="I125" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="J125" s="53"/>
-      <c r="K125" s="53"/>
-      <c r="L125" s="50">
+      <c r="J125" s="40"/>
+      <c r="K125" s="40"/>
+      <c r="L125" s="41">
         <f>L115+L91+L67+L43+L19</f>
         <v>0</v>
       </c>
-      <c r="M125" s="50"/>
-      <c r="N125" s="50"/>
-      <c r="O125" s="50"/>
+      <c r="M125" s="41"/>
+      <c r="N125" s="41"/>
+      <c r="O125" s="41"/>
       <c r="P125" s="12"/>
-      <c r="Q125" s="53" t="s">
+      <c r="Q125" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="R125" s="53"/>
-      <c r="S125" s="53"/>
-      <c r="T125" s="50">
+      <c r="R125" s="40"/>
+      <c r="S125" s="40"/>
+      <c r="T125" s="41">
         <f>T115+T91+T67+T43+T19</f>
         <v>0</v>
       </c>
-      <c r="U125" s="50"/>
-      <c r="V125" s="50"/>
-      <c r="W125" s="50"/>
+      <c r="U125" s="41"/>
+      <c r="V125" s="41"/>
+      <c r="W125" s="41"/>
       <c r="X125" s="12"/>
-      <c r="Y125" s="53" t="s">
+      <c r="Y125" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="Z125" s="53"/>
-      <c r="AA125" s="53"/>
-      <c r="AB125" s="50">
+      <c r="Z125" s="40"/>
+      <c r="AA125" s="40"/>
+      <c r="AB125" s="41">
         <f>AB115+AB91+AB67+AB43+AB19</f>
         <v>0</v>
       </c>
-      <c r="AC125" s="50"/>
-      <c r="AD125" s="50"/>
-      <c r="AE125" s="50"/>
+      <c r="AC125" s="41"/>
+      <c r="AD125" s="41"/>
+      <c r="AE125" s="41"/>
       <c r="AF125" s="12"/>
     </row>
     <row r="126" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A126" s="53" t="s">
+      <c r="A126" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B126" s="53"/>
-      <c r="C126" s="53"/>
-      <c r="D126" s="50">
+      <c r="B126" s="40"/>
+      <c r="C126" s="40"/>
+      <c r="D126" s="41">
         <f>D124-D125</f>
-        <v>2.3464924375000002</v>
-      </c>
-      <c r="E126" s="50"/>
-      <c r="F126" s="50"/>
-      <c r="G126" s="50"/>
+        <v>1.7964924374999995</v>
+      </c>
+      <c r="E126" s="41"/>
+      <c r="F126" s="41"/>
+      <c r="G126" s="41"/>
       <c r="H126" s="12"/>
-      <c r="I126" s="53" t="s">
+      <c r="I126" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="J126" s="53"/>
-      <c r="K126" s="53"/>
-      <c r="L126" s="50">
+      <c r="J126" s="40"/>
+      <c r="K126" s="40"/>
+      <c r="L126" s="41">
         <f>L124-L125</f>
         <v>0</v>
       </c>
-      <c r="M126" s="50"/>
-      <c r="N126" s="50"/>
-      <c r="O126" s="50"/>
+      <c r="M126" s="41"/>
+      <c r="N126" s="41"/>
+      <c r="O126" s="41"/>
       <c r="P126" s="12"/>
-      <c r="Q126" s="53" t="s">
+      <c r="Q126" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="R126" s="53"/>
-      <c r="S126" s="53"/>
-      <c r="T126" s="50">
+      <c r="R126" s="40"/>
+      <c r="S126" s="40"/>
+      <c r="T126" s="41">
         <f>T124-T125</f>
         <v>0</v>
       </c>
-      <c r="U126" s="50"/>
-      <c r="V126" s="50"/>
-      <c r="W126" s="50"/>
+      <c r="U126" s="41"/>
+      <c r="V126" s="41"/>
+      <c r="W126" s="41"/>
       <c r="X126" s="12"/>
-      <c r="Y126" s="53" t="s">
+      <c r="Y126" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="Z126" s="53"/>
-      <c r="AA126" s="53"/>
-      <c r="AB126" s="50">
+      <c r="Z126" s="40"/>
+      <c r="AA126" s="40"/>
+      <c r="AB126" s="41">
         <f>AB124-AB125</f>
         <v>0</v>
       </c>
-      <c r="AC126" s="50"/>
-      <c r="AD126" s="50"/>
-      <c r="AE126" s="50"/>
+      <c r="AC126" s="41"/>
+      <c r="AD126" s="41"/>
+      <c r="AE126" s="41"/>
       <c r="AF126" s="12"/>
     </row>
     <row r="127" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A127" s="53" t="s">
+      <c r="A127" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="B127" s="53"/>
-      <c r="C127" s="53"/>
-      <c r="D127" s="50">
+      <c r="B127" s="40"/>
+      <c r="C127" s="40"/>
+      <c r="D127" s="41">
         <f>B120</f>
-        <v>7032.4499171096795</v>
-      </c>
-      <c r="E127" s="50"/>
-      <c r="F127" s="50"/>
-      <c r="G127" s="50"/>
+        <v>8003.3365648910458</v>
+      </c>
+      <c r="E127" s="41"/>
+      <c r="F127" s="41"/>
+      <c r="G127" s="41"/>
       <c r="H127" s="12"/>
-      <c r="I127" s="53" t="s">
+      <c r="I127" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="J127" s="53"/>
-      <c r="K127" s="53"/>
-      <c r="L127" s="50">
+      <c r="J127" s="40"/>
+      <c r="K127" s="40"/>
+      <c r="L127" s="41">
         <f>J120</f>
         <v>0</v>
       </c>
-      <c r="M127" s="50"/>
-      <c r="N127" s="50"/>
-      <c r="O127" s="50"/>
+      <c r="M127" s="41"/>
+      <c r="N127" s="41"/>
+      <c r="O127" s="41"/>
       <c r="P127" s="12"/>
-      <c r="Q127" s="53" t="s">
+      <c r="Q127" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="R127" s="53"/>
-      <c r="S127" s="53"/>
-      <c r="T127" s="50">
+      <c r="R127" s="40"/>
+      <c r="S127" s="40"/>
+      <c r="T127" s="41">
         <f>R120</f>
         <v>0</v>
       </c>
-      <c r="U127" s="50"/>
-      <c r="V127" s="50"/>
-      <c r="W127" s="50"/>
+      <c r="U127" s="41"/>
+      <c r="V127" s="41"/>
+      <c r="W127" s="41"/>
       <c r="X127" s="12"/>
-      <c r="Y127" s="53" t="s">
+      <c r="Y127" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="Z127" s="53"/>
-      <c r="AA127" s="53"/>
-      <c r="AB127" s="50">
+      <c r="Z127" s="40"/>
+      <c r="AA127" s="40"/>
+      <c r="AB127" s="41">
         <f>Z120</f>
         <v>0</v>
       </c>
-      <c r="AC127" s="50"/>
-      <c r="AD127" s="50"/>
-      <c r="AE127" s="50"/>
+      <c r="AC127" s="41"/>
+      <c r="AD127" s="41"/>
+      <c r="AE127" s="41"/>
       <c r="AF127" s="12"/>
     </row>
     <row r="128" spans="1:32" x14ac:dyDescent="0.25">
@@ -38229,49 +38231,87 @@
     </row>
   </sheetData>
   <mergeCells count="148">
-    <mergeCell ref="Y127:AA127"/>
-    <mergeCell ref="AB127:AE127"/>
-    <mergeCell ref="Y122:AE122"/>
-    <mergeCell ref="Y123:AA123"/>
-    <mergeCell ref="AB123:AE123"/>
-    <mergeCell ref="Y124:AA124"/>
-    <mergeCell ref="AB124:AE124"/>
-    <mergeCell ref="Y125:AA125"/>
-    <mergeCell ref="AB125:AE125"/>
-    <mergeCell ref="Y126:AA126"/>
-    <mergeCell ref="AB126:AE126"/>
-    <mergeCell ref="I127:K127"/>
-    <mergeCell ref="L127:O127"/>
-    <mergeCell ref="Q122:W122"/>
-    <mergeCell ref="Q123:S123"/>
-    <mergeCell ref="T123:W123"/>
-    <mergeCell ref="Q124:S124"/>
-    <mergeCell ref="T124:W124"/>
-    <mergeCell ref="Q125:S125"/>
-    <mergeCell ref="T125:W125"/>
-    <mergeCell ref="Q126:S126"/>
-    <mergeCell ref="T126:W126"/>
-    <mergeCell ref="Q127:S127"/>
-    <mergeCell ref="T127:W127"/>
-    <mergeCell ref="I122:O122"/>
-    <mergeCell ref="I123:K123"/>
-    <mergeCell ref="L123:O123"/>
-    <mergeCell ref="I124:K124"/>
-    <mergeCell ref="L124:O124"/>
-    <mergeCell ref="I125:K125"/>
-    <mergeCell ref="L125:O125"/>
-    <mergeCell ref="I126:K126"/>
-    <mergeCell ref="L126:O126"/>
-    <mergeCell ref="D127:G127"/>
-    <mergeCell ref="D125:G125"/>
-    <mergeCell ref="D124:G124"/>
-    <mergeCell ref="D123:G123"/>
-    <mergeCell ref="A123:C123"/>
-    <mergeCell ref="A124:C124"/>
-    <mergeCell ref="A125:C125"/>
-    <mergeCell ref="A127:C127"/>
-    <mergeCell ref="A126:C126"/>
-    <mergeCell ref="D126:G126"/>
+    <mergeCell ref="B120:G120"/>
+    <mergeCell ref="J120:O120"/>
+    <mergeCell ref="R120:W120"/>
+    <mergeCell ref="Z120:AE120"/>
+    <mergeCell ref="B119:G119"/>
+    <mergeCell ref="J119:O119"/>
+    <mergeCell ref="R119:W119"/>
+    <mergeCell ref="Z119:AE119"/>
+    <mergeCell ref="B118:G118"/>
+    <mergeCell ref="J118:O118"/>
+    <mergeCell ref="R118:W118"/>
+    <mergeCell ref="Z118:AE118"/>
+    <mergeCell ref="B117:G117"/>
+    <mergeCell ref="J117:O117"/>
+    <mergeCell ref="R117:W117"/>
+    <mergeCell ref="Z117:AE117"/>
+    <mergeCell ref="B116:G116"/>
+    <mergeCell ref="J116:O116"/>
+    <mergeCell ref="R116:W116"/>
+    <mergeCell ref="Z116:AE116"/>
+    <mergeCell ref="B96:G96"/>
+    <mergeCell ref="J96:O96"/>
+    <mergeCell ref="R96:W96"/>
+    <mergeCell ref="Z96:AE96"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="J95:O95"/>
+    <mergeCell ref="R95:W95"/>
+    <mergeCell ref="Z95:AE95"/>
+    <mergeCell ref="B94:G94"/>
+    <mergeCell ref="J94:O94"/>
+    <mergeCell ref="R94:W94"/>
+    <mergeCell ref="Z94:AE94"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="J93:O93"/>
+    <mergeCell ref="R93:W93"/>
+    <mergeCell ref="Z93:AE93"/>
+    <mergeCell ref="B92:G92"/>
+    <mergeCell ref="J92:O92"/>
+    <mergeCell ref="R92:W92"/>
+    <mergeCell ref="Z92:AE92"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="J72:O72"/>
+    <mergeCell ref="R72:W72"/>
+    <mergeCell ref="Z72:AE72"/>
+    <mergeCell ref="B71:G71"/>
+    <mergeCell ref="J71:O71"/>
+    <mergeCell ref="R71:W71"/>
+    <mergeCell ref="Z71:AE71"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="J70:O70"/>
+    <mergeCell ref="R70:W70"/>
+    <mergeCell ref="Z70:AE70"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="J69:O69"/>
+    <mergeCell ref="R69:W69"/>
+    <mergeCell ref="Z69:AE69"/>
+    <mergeCell ref="B68:G68"/>
+    <mergeCell ref="J68:O68"/>
+    <mergeCell ref="R68:W68"/>
+    <mergeCell ref="Z68:AE68"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="J48:O48"/>
+    <mergeCell ref="R48:W48"/>
+    <mergeCell ref="Z48:AE48"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="J47:O47"/>
+    <mergeCell ref="R47:W47"/>
+    <mergeCell ref="Z47:AE47"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="J46:O46"/>
+    <mergeCell ref="R46:W46"/>
+    <mergeCell ref="Z46:AE46"/>
+    <mergeCell ref="Z45:AE45"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="J44:O44"/>
+    <mergeCell ref="R44:W44"/>
+    <mergeCell ref="Z44:AE44"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="R24:W24"/>
+    <mergeCell ref="Z24:AE24"/>
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="J20:O20"/>
     <mergeCell ref="R20:W20"/>
@@ -38296,87 +38336,49 @@
     <mergeCell ref="B45:G45"/>
     <mergeCell ref="J45:O45"/>
     <mergeCell ref="R45:W45"/>
-    <mergeCell ref="Z45:AE45"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="J44:O44"/>
-    <mergeCell ref="R44:W44"/>
-    <mergeCell ref="Z44:AE44"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="R24:W24"/>
-    <mergeCell ref="Z24:AE24"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="J48:O48"/>
-    <mergeCell ref="R48:W48"/>
-    <mergeCell ref="Z48:AE48"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="J47:O47"/>
-    <mergeCell ref="R47:W47"/>
-    <mergeCell ref="Z47:AE47"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="J46:O46"/>
-    <mergeCell ref="R46:W46"/>
-    <mergeCell ref="Z46:AE46"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="J70:O70"/>
-    <mergeCell ref="R70:W70"/>
-    <mergeCell ref="Z70:AE70"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="J69:O69"/>
-    <mergeCell ref="R69:W69"/>
-    <mergeCell ref="Z69:AE69"/>
-    <mergeCell ref="B68:G68"/>
-    <mergeCell ref="J68:O68"/>
-    <mergeCell ref="R68:W68"/>
-    <mergeCell ref="Z68:AE68"/>
-    <mergeCell ref="B92:G92"/>
-    <mergeCell ref="J92:O92"/>
-    <mergeCell ref="R92:W92"/>
-    <mergeCell ref="Z92:AE92"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="J72:O72"/>
-    <mergeCell ref="R72:W72"/>
-    <mergeCell ref="Z72:AE72"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="J71:O71"/>
-    <mergeCell ref="R71:W71"/>
-    <mergeCell ref="Z71:AE71"/>
-    <mergeCell ref="B95:G95"/>
-    <mergeCell ref="J95:O95"/>
-    <mergeCell ref="R95:W95"/>
-    <mergeCell ref="Z95:AE95"/>
-    <mergeCell ref="B94:G94"/>
-    <mergeCell ref="J94:O94"/>
-    <mergeCell ref="R94:W94"/>
-    <mergeCell ref="Z94:AE94"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="J93:O93"/>
-    <mergeCell ref="R93:W93"/>
-    <mergeCell ref="Z93:AE93"/>
-    <mergeCell ref="B117:G117"/>
-    <mergeCell ref="J117:O117"/>
-    <mergeCell ref="R117:W117"/>
-    <mergeCell ref="Z117:AE117"/>
-    <mergeCell ref="B116:G116"/>
-    <mergeCell ref="J116:O116"/>
-    <mergeCell ref="R116:W116"/>
-    <mergeCell ref="Z116:AE116"/>
-    <mergeCell ref="B96:G96"/>
-    <mergeCell ref="J96:O96"/>
-    <mergeCell ref="R96:W96"/>
-    <mergeCell ref="Z96:AE96"/>
-    <mergeCell ref="B120:G120"/>
-    <mergeCell ref="J120:O120"/>
-    <mergeCell ref="R120:W120"/>
-    <mergeCell ref="Z120:AE120"/>
-    <mergeCell ref="B119:G119"/>
-    <mergeCell ref="J119:O119"/>
-    <mergeCell ref="R119:W119"/>
-    <mergeCell ref="Z119:AE119"/>
-    <mergeCell ref="B118:G118"/>
-    <mergeCell ref="J118:O118"/>
-    <mergeCell ref="R118:W118"/>
-    <mergeCell ref="Z118:AE118"/>
+    <mergeCell ref="D127:G127"/>
+    <mergeCell ref="D125:G125"/>
+    <mergeCell ref="D124:G124"/>
+    <mergeCell ref="D123:G123"/>
+    <mergeCell ref="A123:C123"/>
+    <mergeCell ref="A124:C124"/>
+    <mergeCell ref="A125:C125"/>
+    <mergeCell ref="A127:C127"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="D126:G126"/>
+    <mergeCell ref="I127:K127"/>
+    <mergeCell ref="L127:O127"/>
+    <mergeCell ref="Q122:W122"/>
+    <mergeCell ref="Q123:S123"/>
+    <mergeCell ref="T123:W123"/>
+    <mergeCell ref="Q124:S124"/>
+    <mergeCell ref="T124:W124"/>
+    <mergeCell ref="Q125:S125"/>
+    <mergeCell ref="T125:W125"/>
+    <mergeCell ref="Q126:S126"/>
+    <mergeCell ref="T126:W126"/>
+    <mergeCell ref="Q127:S127"/>
+    <mergeCell ref="T127:W127"/>
+    <mergeCell ref="I122:O122"/>
+    <mergeCell ref="I123:K123"/>
+    <mergeCell ref="L123:O123"/>
+    <mergeCell ref="I124:K124"/>
+    <mergeCell ref="L124:O124"/>
+    <mergeCell ref="I125:K125"/>
+    <mergeCell ref="L125:O125"/>
+    <mergeCell ref="I126:K126"/>
+    <mergeCell ref="L126:O126"/>
+    <mergeCell ref="Y127:AA127"/>
+    <mergeCell ref="AB127:AE127"/>
+    <mergeCell ref="Y122:AE122"/>
+    <mergeCell ref="Y123:AA123"/>
+    <mergeCell ref="AB123:AE123"/>
+    <mergeCell ref="Y124:AA124"/>
+    <mergeCell ref="AB124:AE124"/>
+    <mergeCell ref="Y125:AA125"/>
+    <mergeCell ref="AB125:AE125"/>
+    <mergeCell ref="Y126:AA126"/>
+    <mergeCell ref="AB126:AE126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39442,9 +39444,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
+      <selection pane="bottomLeft" activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
* FIX - Hopefully fix up in-editor lag issues and memory issues (.dll recompile) * FIX - Add compound colliders for LC-DC parts; untested, but should solve issues of the colliders sticking/exploding various craft. * UPDATE - Add initial texture pass for SC-E parts
</commit_message>
<xml_diff>
--- a/GameData/SSTU/Parts/Parts-MassCalc.xlsx
+++ b/GameData/SSTU/Parts/Parts-MassCalc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="parts" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="ChuteCalc" sheetId="9" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="10" r:id="rId6"/>
     <sheet name="StockChuteCalc" sheetId="11" r:id="rId7"/>
+    <sheet name="RealRocketDims" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="377">
   <si>
     <t>Part</t>
   </si>
@@ -1104,6 +1105,54 @@
   <si>
     <t>KSP Heat</t>
   </si>
+  <si>
+    <t>Saturn-V</t>
+  </si>
+  <si>
+    <t>SLS</t>
+  </si>
+  <si>
+    <t>Shuttle</t>
+  </si>
+  <si>
+    <t>Scaled</t>
+  </si>
+  <si>
+    <t>S-I</t>
+  </si>
+  <si>
+    <t>S-II</t>
+  </si>
+  <si>
+    <t>S-IVB</t>
+  </si>
+  <si>
+    <t>IPA-B</t>
+  </si>
+  <si>
+    <t>IPA-T</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Tank</t>
+  </si>
+  <si>
+    <t>Booster</t>
+  </si>
+  <si>
+    <t>ICPS</t>
+  </si>
+  <si>
+    <t>HUS</t>
+  </si>
 </sst>
 </file>
 
@@ -1557,25 +1606,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1590,14 +1627,26 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1905,7 +1954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G63" sqref="G63"/>
     </sheetView>
@@ -27830,45 +27879,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="H1" s="12"/>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
       <c r="P1" s="12"/>
-      <c r="Q1" s="50" t="s">
+      <c r="Q1" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
       <c r="X1" s="12"/>
-      <c r="Y1" s="50" t="s">
+      <c r="Y1" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="50"/>
-      <c r="AC1" s="50"/>
-      <c r="AD1" s="50"/>
-      <c r="AE1" s="50"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
       <c r="AF1" s="12"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -29579,270 +29628,270 @@
       <c r="A20" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="47">
+      <c r="B20" s="43">
         <f>E19</f>
         <v>0</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="49"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="45"/>
       <c r="H20" s="12"/>
       <c r="I20" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J20" s="47">
+      <c r="J20" s="43">
         <f>M19</f>
         <v>0</v>
       </c>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="49"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="45"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R20" s="47">
+      <c r="R20" s="43">
         <f>U19</f>
         <v>0</v>
       </c>
-      <c r="S20" s="48"/>
-      <c r="T20" s="48"/>
-      <c r="U20" s="48"/>
-      <c r="V20" s="48"/>
-      <c r="W20" s="49"/>
+      <c r="S20" s="44"/>
+      <c r="T20" s="44"/>
+      <c r="U20" s="44"/>
+      <c r="V20" s="44"/>
+      <c r="W20" s="45"/>
       <c r="X20" s="12"/>
       <c r="Y20" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z20" s="47">
+      <c r="Z20" s="43">
         <f>AC19</f>
         <v>0</v>
       </c>
-      <c r="AA20" s="48"/>
-      <c r="AB20" s="48"/>
-      <c r="AC20" s="48"/>
-      <c r="AD20" s="48"/>
-      <c r="AE20" s="49"/>
+      <c r="AA20" s="44"/>
+      <c r="AB20" s="44"/>
+      <c r="AC20" s="44"/>
+      <c r="AD20" s="44"/>
+      <c r="AE20" s="45"/>
       <c r="AF20" s="12"/>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="47">
+      <c r="B21" s="43">
         <f>C19</f>
         <v>0</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="49"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="45"/>
       <c r="H21" s="12"/>
       <c r="I21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J21" s="47">
+      <c r="J21" s="43">
         <f>K19</f>
         <v>0</v>
       </c>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="49"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="45"/>
       <c r="P21" s="12"/>
       <c r="Q21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R21" s="47">
+      <c r="R21" s="43">
         <f>S19</f>
         <v>0</v>
       </c>
-      <c r="S21" s="48"/>
-      <c r="T21" s="48"/>
-      <c r="U21" s="48"/>
-      <c r="V21" s="48"/>
-      <c r="W21" s="49"/>
+      <c r="S21" s="44"/>
+      <c r="T21" s="44"/>
+      <c r="U21" s="44"/>
+      <c r="V21" s="44"/>
+      <c r="W21" s="45"/>
       <c r="X21" s="12"/>
       <c r="Y21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z21" s="47">
+      <c r="Z21" s="43">
         <f>AA19</f>
         <v>0</v>
       </c>
-      <c r="AA21" s="48"/>
-      <c r="AB21" s="48"/>
-      <c r="AC21" s="48"/>
-      <c r="AD21" s="48"/>
-      <c r="AE21" s="49"/>
+      <c r="AA21" s="44"/>
+      <c r="AB21" s="44"/>
+      <c r="AC21" s="44"/>
+      <c r="AD21" s="44"/>
+      <c r="AE21" s="45"/>
       <c r="AF21" s="12"/>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="47">
+      <c r="B22" s="43">
         <f>IFERROR((G19/10/B20),0)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="49"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="45"/>
       <c r="H22" s="12"/>
       <c r="I22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J22" s="47">
+      <c r="J22" s="43">
         <f>IFERROR((O19/10/J20),0)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="48"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="49"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="45"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R22" s="47">
+      <c r="R22" s="43">
         <f>IFERROR((W19/10/R20),0)</f>
         <v>0</v>
       </c>
-      <c r="S22" s="48"/>
-      <c r="T22" s="48"/>
-      <c r="U22" s="48"/>
-      <c r="V22" s="48"/>
-      <c r="W22" s="49"/>
+      <c r="S22" s="44"/>
+      <c r="T22" s="44"/>
+      <c r="U22" s="44"/>
+      <c r="V22" s="44"/>
+      <c r="W22" s="45"/>
       <c r="X22" s="12"/>
       <c r="Y22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z22" s="47">
+      <c r="Z22" s="43">
         <f>IFERROR((AE19/10/Z20),0)</f>
         <v>0</v>
       </c>
-      <c r="AA22" s="48"/>
-      <c r="AB22" s="48"/>
-      <c r="AC22" s="48"/>
-      <c r="AD22" s="48"/>
-      <c r="AE22" s="49"/>
+      <c r="AA22" s="44"/>
+      <c r="AB22" s="44"/>
+      <c r="AC22" s="44"/>
+      <c r="AD22" s="44"/>
+      <c r="AE22" s="45"/>
       <c r="AF22" s="12"/>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="47">
+      <c r="B23" s="43">
         <f>IFERROR((9.82 * F19) * LN(B20/C19),0)</f>
         <v>0</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="49"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="45"/>
       <c r="H23" s="12"/>
       <c r="I23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J23" s="47">
+      <c r="J23" s="43">
         <f>IFERROR((9.82 * N19) * LN(J20/K19),0)</f>
         <v>0</v>
       </c>
-      <c r="K23" s="48"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="49"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="45"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R23" s="47">
+      <c r="R23" s="43">
         <f>IFERROR((9.82 * V19) * LN(R20/S19),0)</f>
         <v>0</v>
       </c>
-      <c r="S23" s="48"/>
-      <c r="T23" s="48"/>
-      <c r="U23" s="48"/>
-      <c r="V23" s="48"/>
-      <c r="W23" s="49"/>
+      <c r="S23" s="44"/>
+      <c r="T23" s="44"/>
+      <c r="U23" s="44"/>
+      <c r="V23" s="44"/>
+      <c r="W23" s="45"/>
       <c r="X23" s="12"/>
       <c r="Y23" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z23" s="47">
+      <c r="Z23" s="43">
         <f>IFERROR((9.82 * AD19) * LN(Z20/AA19),0)</f>
         <v>0</v>
       </c>
-      <c r="AA23" s="48"/>
-      <c r="AB23" s="48"/>
-      <c r="AC23" s="48"/>
-      <c r="AD23" s="48"/>
-      <c r="AE23" s="49"/>
+      <c r="AA23" s="44"/>
+      <c r="AB23" s="44"/>
+      <c r="AC23" s="44"/>
+      <c r="AD23" s="44"/>
+      <c r="AE23" s="45"/>
       <c r="AF23" s="12"/>
     </row>
     <row r="24" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="51">
+      <c r="B24" s="40">
         <f>B23</f>
         <v>0</v>
       </c>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="53"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="42"/>
       <c r="H24" s="12"/>
       <c r="I24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J24" s="51">
+      <c r="J24" s="40">
         <f>J23</f>
         <v>0</v>
       </c>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="53"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="42"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R24" s="51">
+      <c r="R24" s="40">
         <f>R23</f>
         <v>0</v>
       </c>
-      <c r="S24" s="52"/>
-      <c r="T24" s="52"/>
-      <c r="U24" s="52"/>
-      <c r="V24" s="52"/>
-      <c r="W24" s="53"/>
+      <c r="S24" s="41"/>
+      <c r="T24" s="41"/>
+      <c r="U24" s="41"/>
+      <c r="V24" s="41"/>
+      <c r="W24" s="42"/>
       <c r="X24" s="12"/>
       <c r="Y24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z24" s="51">
+      <c r="Z24" s="40">
         <f>Z23</f>
         <v>0</v>
       </c>
-      <c r="AA24" s="52"/>
-      <c r="AB24" s="52"/>
-      <c r="AC24" s="52"/>
-      <c r="AD24" s="52"/>
-      <c r="AE24" s="53"/>
+      <c r="AA24" s="41"/>
+      <c r="AB24" s="41"/>
+      <c r="AC24" s="41"/>
+      <c r="AD24" s="41"/>
+      <c r="AE24" s="42"/>
       <c r="AF24" s="12"/>
     </row>
     <row r="25" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31583,270 +31632,270 @@
       <c r="A44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="47">
+      <c r="B44" s="43">
         <f>E43+B20</f>
         <v>10.773108687500001</v>
       </c>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="48"/>
-      <c r="G44" s="49"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="45"/>
       <c r="H44" s="12"/>
       <c r="I44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J44" s="47">
+      <c r="J44" s="43">
         <f>M43+J20</f>
         <v>0</v>
       </c>
-      <c r="K44" s="48"/>
-      <c r="L44" s="48"/>
-      <c r="M44" s="48"/>
-      <c r="N44" s="48"/>
-      <c r="O44" s="49"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="44"/>
+      <c r="M44" s="44"/>
+      <c r="N44" s="44"/>
+      <c r="O44" s="45"/>
       <c r="P44" s="12"/>
       <c r="Q44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R44" s="47">
+      <c r="R44" s="43">
         <f>U43+R20</f>
         <v>0</v>
       </c>
-      <c r="S44" s="48"/>
-      <c r="T44" s="48"/>
-      <c r="U44" s="48"/>
-      <c r="V44" s="48"/>
-      <c r="W44" s="49"/>
+      <c r="S44" s="44"/>
+      <c r="T44" s="44"/>
+      <c r="U44" s="44"/>
+      <c r="V44" s="44"/>
+      <c r="W44" s="45"/>
       <c r="X44" s="12"/>
       <c r="Y44" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z44" s="47">
+      <c r="Z44" s="43">
         <f>AC43+Z20</f>
         <v>0</v>
       </c>
-      <c r="AA44" s="48"/>
-      <c r="AB44" s="48"/>
-      <c r="AC44" s="48"/>
-      <c r="AD44" s="48"/>
-      <c r="AE44" s="49"/>
+      <c r="AA44" s="44"/>
+      <c r="AB44" s="44"/>
+      <c r="AC44" s="44"/>
+      <c r="AD44" s="44"/>
+      <c r="AE44" s="45"/>
       <c r="AF44" s="12"/>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="47">
+      <c r="B45" s="43">
         <f>C43+B20</f>
         <v>1.7964924375</v>
       </c>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
-      <c r="E45" s="48"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="49"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="45"/>
       <c r="H45" s="12"/>
       <c r="I45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J45" s="47">
+      <c r="J45" s="43">
         <f>K43+J20</f>
         <v>0</v>
       </c>
-      <c r="K45" s="48"/>
-      <c r="L45" s="48"/>
-      <c r="M45" s="48"/>
-      <c r="N45" s="48"/>
-      <c r="O45" s="49"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="44"/>
+      <c r="M45" s="44"/>
+      <c r="N45" s="44"/>
+      <c r="O45" s="45"/>
       <c r="P45" s="12"/>
       <c r="Q45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R45" s="47">
+      <c r="R45" s="43">
         <f>S43+R20</f>
         <v>0</v>
       </c>
-      <c r="S45" s="48"/>
-      <c r="T45" s="48"/>
-      <c r="U45" s="48"/>
-      <c r="V45" s="48"/>
-      <c r="W45" s="49"/>
+      <c r="S45" s="44"/>
+      <c r="T45" s="44"/>
+      <c r="U45" s="44"/>
+      <c r="V45" s="44"/>
+      <c r="W45" s="45"/>
       <c r="X45" s="12"/>
       <c r="Y45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z45" s="47">
+      <c r="Z45" s="43">
         <f>AA43+Z20</f>
         <v>0</v>
       </c>
-      <c r="AA45" s="48"/>
-      <c r="AB45" s="48"/>
-      <c r="AC45" s="48"/>
-      <c r="AD45" s="48"/>
-      <c r="AE45" s="49"/>
+      <c r="AA45" s="44"/>
+      <c r="AB45" s="44"/>
+      <c r="AC45" s="44"/>
+      <c r="AD45" s="44"/>
+      <c r="AE45" s="45"/>
       <c r="AF45" s="12"/>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="47">
+      <c r="B46" s="43">
         <f>IFERROR((G43/10/B44),0)</f>
         <v>0.4177067298338254</v>
       </c>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="49"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="45"/>
       <c r="H46" s="12"/>
       <c r="I46" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J46" s="47">
+      <c r="J46" s="43">
         <f>IFERROR((O43/10/J44),0)</f>
         <v>0</v>
       </c>
-      <c r="K46" s="48"/>
-      <c r="L46" s="48"/>
-      <c r="M46" s="48"/>
-      <c r="N46" s="48"/>
-      <c r="O46" s="49"/>
+      <c r="K46" s="44"/>
+      <c r="L46" s="44"/>
+      <c r="M46" s="44"/>
+      <c r="N46" s="44"/>
+      <c r="O46" s="45"/>
       <c r="P46" s="12"/>
       <c r="Q46" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R46" s="47">
+      <c r="R46" s="43">
         <f>IFERROR((W43/10/R44),0)</f>
         <v>0</v>
       </c>
-      <c r="S46" s="48"/>
-      <c r="T46" s="48"/>
-      <c r="U46" s="48"/>
-      <c r="V46" s="48"/>
-      <c r="W46" s="49"/>
+      <c r="S46" s="44"/>
+      <c r="T46" s="44"/>
+      <c r="U46" s="44"/>
+      <c r="V46" s="44"/>
+      <c r="W46" s="45"/>
       <c r="X46" s="12"/>
       <c r="Y46" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z46" s="47">
+      <c r="Z46" s="43">
         <f>IFERROR((AE43/10/Z44),0)</f>
         <v>0</v>
       </c>
-      <c r="AA46" s="48"/>
-      <c r="AB46" s="48"/>
-      <c r="AC46" s="48"/>
-      <c r="AD46" s="48"/>
-      <c r="AE46" s="49"/>
+      <c r="AA46" s="44"/>
+      <c r="AB46" s="44"/>
+      <c r="AC46" s="44"/>
+      <c r="AD46" s="44"/>
+      <c r="AE46" s="45"/>
       <c r="AF46" s="12"/>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="47">
+      <c r="B47" s="43">
         <f>IFERROR((9.82 * F43) * LN(B44/B45),0)</f>
         <v>8003.3365648910458</v>
       </c>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="49"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="45"/>
       <c r="H47" s="12"/>
       <c r="I47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J47" s="47">
+      <c r="J47" s="43">
         <f>IFERROR((9.82 * N43) * LN(J44/J45),0)</f>
         <v>0</v>
       </c>
-      <c r="K47" s="48"/>
-      <c r="L47" s="48"/>
-      <c r="M47" s="48"/>
-      <c r="N47" s="48"/>
-      <c r="O47" s="49"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="44"/>
+      <c r="M47" s="44"/>
+      <c r="N47" s="44"/>
+      <c r="O47" s="45"/>
       <c r="P47" s="12"/>
       <c r="Q47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R47" s="47">
+      <c r="R47" s="43">
         <f>IFERROR((9.82 * V43) * LN(R44/R45),0)</f>
         <v>0</v>
       </c>
-      <c r="S47" s="48"/>
-      <c r="T47" s="48"/>
-      <c r="U47" s="48"/>
-      <c r="V47" s="48"/>
-      <c r="W47" s="49"/>
+      <c r="S47" s="44"/>
+      <c r="T47" s="44"/>
+      <c r="U47" s="44"/>
+      <c r="V47" s="44"/>
+      <c r="W47" s="45"/>
       <c r="X47" s="12"/>
       <c r="Y47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z47" s="47">
+      <c r="Z47" s="43">
         <f>IFERROR((9.82 * AD43) * LN(Z44/Z45),0)</f>
         <v>0</v>
       </c>
-      <c r="AA47" s="48"/>
-      <c r="AB47" s="48"/>
-      <c r="AC47" s="48"/>
-      <c r="AD47" s="48"/>
-      <c r="AE47" s="49"/>
+      <c r="AA47" s="44"/>
+      <c r="AB47" s="44"/>
+      <c r="AC47" s="44"/>
+      <c r="AD47" s="44"/>
+      <c r="AE47" s="45"/>
       <c r="AF47" s="12"/>
     </row>
     <row r="48" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B48" s="51">
+      <c r="B48" s="40">
         <f>B47+B24</f>
         <v>8003.3365648910458</v>
       </c>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="53"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="41"/>
+      <c r="G48" s="42"/>
       <c r="H48" s="12"/>
       <c r="I48" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J48" s="51">
+      <c r="J48" s="40">
         <f>J47+J24</f>
         <v>0</v>
       </c>
-      <c r="K48" s="52"/>
-      <c r="L48" s="52"/>
-      <c r="M48" s="52"/>
-      <c r="N48" s="52"/>
-      <c r="O48" s="53"/>
+      <c r="K48" s="41"/>
+      <c r="L48" s="41"/>
+      <c r="M48" s="41"/>
+      <c r="N48" s="41"/>
+      <c r="O48" s="42"/>
       <c r="P48" s="12"/>
       <c r="Q48" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R48" s="51">
+      <c r="R48" s="40">
         <f>R47+R24</f>
         <v>0</v>
       </c>
-      <c r="S48" s="52"/>
-      <c r="T48" s="52"/>
-      <c r="U48" s="52"/>
-      <c r="V48" s="52"/>
-      <c r="W48" s="53"/>
+      <c r="S48" s="41"/>
+      <c r="T48" s="41"/>
+      <c r="U48" s="41"/>
+      <c r="V48" s="41"/>
+      <c r="W48" s="42"/>
       <c r="X48" s="12"/>
       <c r="Y48" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z48" s="51">
+      <c r="Z48" s="40">
         <f>Z47+Z24</f>
         <v>0</v>
       </c>
-      <c r="AA48" s="52"/>
-      <c r="AB48" s="52"/>
-      <c r="AC48" s="52"/>
-      <c r="AD48" s="52"/>
-      <c r="AE48" s="53"/>
+      <c r="AA48" s="41"/>
+      <c r="AB48" s="41"/>
+      <c r="AC48" s="41"/>
+      <c r="AD48" s="41"/>
+      <c r="AE48" s="42"/>
       <c r="AF48" s="12"/>
     </row>
     <row r="49" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33583,270 +33632,270 @@
       <c r="A68" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="47">
+      <c r="B68" s="43">
         <f>E67+B44</f>
         <v>10.773108687500001</v>
       </c>
-      <c r="C68" s="48"/>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
-      <c r="F68" s="48"/>
-      <c r="G68" s="49"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="44"/>
+      <c r="E68" s="44"/>
+      <c r="F68" s="44"/>
+      <c r="G68" s="45"/>
       <c r="H68" s="12"/>
       <c r="I68" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J68" s="47">
+      <c r="J68" s="43">
         <f>M67+J44</f>
         <v>0</v>
       </c>
-      <c r="K68" s="48"/>
-      <c r="L68" s="48"/>
-      <c r="M68" s="48"/>
-      <c r="N68" s="48"/>
-      <c r="O68" s="49"/>
+      <c r="K68" s="44"/>
+      <c r="L68" s="44"/>
+      <c r="M68" s="44"/>
+      <c r="N68" s="44"/>
+      <c r="O68" s="45"/>
       <c r="P68" s="12"/>
       <c r="Q68" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R68" s="47">
+      <c r="R68" s="43">
         <f>U67+R44</f>
         <v>0</v>
       </c>
-      <c r="S68" s="48"/>
-      <c r="T68" s="48"/>
-      <c r="U68" s="48"/>
-      <c r="V68" s="48"/>
-      <c r="W68" s="49"/>
+      <c r="S68" s="44"/>
+      <c r="T68" s="44"/>
+      <c r="U68" s="44"/>
+      <c r="V68" s="44"/>
+      <c r="W68" s="45"/>
       <c r="X68" s="12"/>
       <c r="Y68" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z68" s="47">
+      <c r="Z68" s="43">
         <f>AC67+Z44</f>
         <v>0</v>
       </c>
-      <c r="AA68" s="48"/>
-      <c r="AB68" s="48"/>
-      <c r="AC68" s="48"/>
-      <c r="AD68" s="48"/>
-      <c r="AE68" s="49"/>
+      <c r="AA68" s="44"/>
+      <c r="AB68" s="44"/>
+      <c r="AC68" s="44"/>
+      <c r="AD68" s="44"/>
+      <c r="AE68" s="45"/>
       <c r="AF68" s="12"/>
     </row>
     <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="47">
+      <c r="B69" s="43">
         <f>C67+B44</f>
         <v>10.773108687500001</v>
       </c>
-      <c r="C69" s="48"/>
-      <c r="D69" s="48"/>
-      <c r="E69" s="48"/>
-      <c r="F69" s="48"/>
-      <c r="G69" s="49"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="44"/>
+      <c r="E69" s="44"/>
+      <c r="F69" s="44"/>
+      <c r="G69" s="45"/>
       <c r="H69" s="12"/>
       <c r="I69" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J69" s="47">
+      <c r="J69" s="43">
         <f>K67+J44</f>
         <v>0</v>
       </c>
-      <c r="K69" s="48"/>
-      <c r="L69" s="48"/>
-      <c r="M69" s="48"/>
-      <c r="N69" s="48"/>
-      <c r="O69" s="49"/>
+      <c r="K69" s="44"/>
+      <c r="L69" s="44"/>
+      <c r="M69" s="44"/>
+      <c r="N69" s="44"/>
+      <c r="O69" s="45"/>
       <c r="P69" s="12"/>
       <c r="Q69" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R69" s="47">
+      <c r="R69" s="43">
         <f>S67+R44</f>
         <v>0</v>
       </c>
-      <c r="S69" s="48"/>
-      <c r="T69" s="48"/>
-      <c r="U69" s="48"/>
-      <c r="V69" s="48"/>
-      <c r="W69" s="49"/>
+      <c r="S69" s="44"/>
+      <c r="T69" s="44"/>
+      <c r="U69" s="44"/>
+      <c r="V69" s="44"/>
+      <c r="W69" s="45"/>
       <c r="X69" s="12"/>
       <c r="Y69" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z69" s="47">
+      <c r="Z69" s="43">
         <f>AA67+Z44</f>
         <v>0</v>
       </c>
-      <c r="AA69" s="48"/>
-      <c r="AB69" s="48"/>
-      <c r="AC69" s="48"/>
-      <c r="AD69" s="48"/>
-      <c r="AE69" s="49"/>
+      <c r="AA69" s="44"/>
+      <c r="AB69" s="44"/>
+      <c r="AC69" s="44"/>
+      <c r="AD69" s="44"/>
+      <c r="AE69" s="45"/>
       <c r="AF69" s="12"/>
     </row>
     <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B70" s="47">
+      <c r="B70" s="43">
         <f>IFERROR((G67/10/B68),0)</f>
         <v>0</v>
       </c>
-      <c r="C70" s="48"/>
-      <c r="D70" s="48"/>
-      <c r="E70" s="48"/>
-      <c r="F70" s="48"/>
-      <c r="G70" s="49"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="44"/>
+      <c r="E70" s="44"/>
+      <c r="F70" s="44"/>
+      <c r="G70" s="45"/>
       <c r="H70" s="12"/>
       <c r="I70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J70" s="47">
+      <c r="J70" s="43">
         <f>IFERROR((O67/10/J68),0)</f>
         <v>0</v>
       </c>
-      <c r="K70" s="48"/>
-      <c r="L70" s="48"/>
-      <c r="M70" s="48"/>
-      <c r="N70" s="48"/>
-      <c r="O70" s="49"/>
+      <c r="K70" s="44"/>
+      <c r="L70" s="44"/>
+      <c r="M70" s="44"/>
+      <c r="N70" s="44"/>
+      <c r="O70" s="45"/>
       <c r="P70" s="12"/>
       <c r="Q70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R70" s="47">
+      <c r="R70" s="43">
         <f>IFERROR((W67/10/R68),0)</f>
         <v>0</v>
       </c>
-      <c r="S70" s="48"/>
-      <c r="T70" s="48"/>
-      <c r="U70" s="48"/>
-      <c r="V70" s="48"/>
-      <c r="W70" s="49"/>
+      <c r="S70" s="44"/>
+      <c r="T70" s="44"/>
+      <c r="U70" s="44"/>
+      <c r="V70" s="44"/>
+      <c r="W70" s="45"/>
       <c r="X70" s="12"/>
       <c r="Y70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z70" s="47">
+      <c r="Z70" s="43">
         <f>IFERROR((AE67/10/Z68),0)</f>
         <v>0</v>
       </c>
-      <c r="AA70" s="48"/>
-      <c r="AB70" s="48"/>
-      <c r="AC70" s="48"/>
-      <c r="AD70" s="48"/>
-      <c r="AE70" s="49"/>
+      <c r="AA70" s="44"/>
+      <c r="AB70" s="44"/>
+      <c r="AC70" s="44"/>
+      <c r="AD70" s="44"/>
+      <c r="AE70" s="45"/>
       <c r="AF70" s="12"/>
     </row>
     <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="47">
+      <c r="B71" s="43">
         <f>IFERROR((9.82 * F67) * LN(B68/B69),0)</f>
         <v>0</v>
       </c>
-      <c r="C71" s="48"/>
-      <c r="D71" s="48"/>
-      <c r="E71" s="48"/>
-      <c r="F71" s="48"/>
-      <c r="G71" s="49"/>
+      <c r="C71" s="44"/>
+      <c r="D71" s="44"/>
+      <c r="E71" s="44"/>
+      <c r="F71" s="44"/>
+      <c r="G71" s="45"/>
       <c r="H71" s="12"/>
       <c r="I71" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J71" s="47">
+      <c r="J71" s="43">
         <f>IFERROR((9.82 * N67) * LN(J68/J69),0)</f>
         <v>0</v>
       </c>
-      <c r="K71" s="48"/>
-      <c r="L71" s="48"/>
-      <c r="M71" s="48"/>
-      <c r="N71" s="48"/>
-      <c r="O71" s="49"/>
+      <c r="K71" s="44"/>
+      <c r="L71" s="44"/>
+      <c r="M71" s="44"/>
+      <c r="N71" s="44"/>
+      <c r="O71" s="45"/>
       <c r="P71" s="12"/>
       <c r="Q71" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R71" s="47">
+      <c r="R71" s="43">
         <f>IFERROR((9.82 * V67) * LN(R68/R69),0)</f>
         <v>0</v>
       </c>
-      <c r="S71" s="48"/>
-      <c r="T71" s="48"/>
-      <c r="U71" s="48"/>
-      <c r="V71" s="48"/>
-      <c r="W71" s="49"/>
+      <c r="S71" s="44"/>
+      <c r="T71" s="44"/>
+      <c r="U71" s="44"/>
+      <c r="V71" s="44"/>
+      <c r="W71" s="45"/>
       <c r="X71" s="12"/>
       <c r="Y71" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z71" s="47">
+      <c r="Z71" s="43">
         <f>IFERROR((9.82 * AD67) * LN(Z68/Z69),0)</f>
         <v>0</v>
       </c>
-      <c r="AA71" s="48"/>
-      <c r="AB71" s="48"/>
-      <c r="AC71" s="48"/>
-      <c r="AD71" s="48"/>
-      <c r="AE71" s="49"/>
+      <c r="AA71" s="44"/>
+      <c r="AB71" s="44"/>
+      <c r="AC71" s="44"/>
+      <c r="AD71" s="44"/>
+      <c r="AE71" s="45"/>
       <c r="AF71" s="12"/>
     </row>
     <row r="72" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="51">
+      <c r="B72" s="40">
         <f>B71+B48</f>
         <v>8003.3365648910458</v>
       </c>
-      <c r="C72" s="52"/>
-      <c r="D72" s="52"/>
-      <c r="E72" s="52"/>
-      <c r="F72" s="52"/>
-      <c r="G72" s="53"/>
+      <c r="C72" s="41"/>
+      <c r="D72" s="41"/>
+      <c r="E72" s="41"/>
+      <c r="F72" s="41"/>
+      <c r="G72" s="42"/>
       <c r="H72" s="12"/>
       <c r="I72" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J72" s="51">
+      <c r="J72" s="40">
         <f>J71+J48</f>
         <v>0</v>
       </c>
-      <c r="K72" s="52"/>
-      <c r="L72" s="52"/>
-      <c r="M72" s="52"/>
-      <c r="N72" s="52"/>
-      <c r="O72" s="53"/>
+      <c r="K72" s="41"/>
+      <c r="L72" s="41"/>
+      <c r="M72" s="41"/>
+      <c r="N72" s="41"/>
+      <c r="O72" s="42"/>
       <c r="P72" s="12"/>
       <c r="Q72" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R72" s="51">
+      <c r="R72" s="40">
         <f>R71+R48</f>
         <v>0</v>
       </c>
-      <c r="S72" s="52"/>
-      <c r="T72" s="52"/>
-      <c r="U72" s="52"/>
-      <c r="V72" s="52"/>
-      <c r="W72" s="53"/>
+      <c r="S72" s="41"/>
+      <c r="T72" s="41"/>
+      <c r="U72" s="41"/>
+      <c r="V72" s="41"/>
+      <c r="W72" s="42"/>
       <c r="X72" s="12"/>
       <c r="Y72" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z72" s="51">
+      <c r="Z72" s="40">
         <f>Z71+Z48</f>
         <v>0</v>
       </c>
-      <c r="AA72" s="52"/>
-      <c r="AB72" s="52"/>
-      <c r="AC72" s="52"/>
-      <c r="AD72" s="52"/>
-      <c r="AE72" s="53"/>
+      <c r="AA72" s="41"/>
+      <c r="AB72" s="41"/>
+      <c r="AC72" s="41"/>
+      <c r="AD72" s="41"/>
+      <c r="AE72" s="42"/>
       <c r="AF72" s="12"/>
     </row>
     <row r="73" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -35583,270 +35632,270 @@
       <c r="A92" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B92" s="47">
+      <c r="B92" s="43">
         <f>E91+B68</f>
         <v>10.773108687500001</v>
       </c>
-      <c r="C92" s="48"/>
-      <c r="D92" s="48"/>
-      <c r="E92" s="48"/>
-      <c r="F92" s="48"/>
-      <c r="G92" s="49"/>
+      <c r="C92" s="44"/>
+      <c r="D92" s="44"/>
+      <c r="E92" s="44"/>
+      <c r="F92" s="44"/>
+      <c r="G92" s="45"/>
       <c r="H92" s="12"/>
       <c r="I92" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J92" s="47">
+      <c r="J92" s="43">
         <f>M91+J68</f>
         <v>0</v>
       </c>
-      <c r="K92" s="48"/>
-      <c r="L92" s="48"/>
-      <c r="M92" s="48"/>
-      <c r="N92" s="48"/>
-      <c r="O92" s="49"/>
+      <c r="K92" s="44"/>
+      <c r="L92" s="44"/>
+      <c r="M92" s="44"/>
+      <c r="N92" s="44"/>
+      <c r="O92" s="45"/>
       <c r="P92" s="12"/>
       <c r="Q92" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R92" s="47">
+      <c r="R92" s="43">
         <f>U91+R68</f>
         <v>0</v>
       </c>
-      <c r="S92" s="48"/>
-      <c r="T92" s="48"/>
-      <c r="U92" s="48"/>
-      <c r="V92" s="48"/>
-      <c r="W92" s="49"/>
+      <c r="S92" s="44"/>
+      <c r="T92" s="44"/>
+      <c r="U92" s="44"/>
+      <c r="V92" s="44"/>
+      <c r="W92" s="45"/>
       <c r="X92" s="12"/>
       <c r="Y92" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z92" s="47">
+      <c r="Z92" s="43">
         <f>AC91+Z68</f>
         <v>0</v>
       </c>
-      <c r="AA92" s="48"/>
-      <c r="AB92" s="48"/>
-      <c r="AC92" s="48"/>
-      <c r="AD92" s="48"/>
-      <c r="AE92" s="49"/>
+      <c r="AA92" s="44"/>
+      <c r="AB92" s="44"/>
+      <c r="AC92" s="44"/>
+      <c r="AD92" s="44"/>
+      <c r="AE92" s="45"/>
       <c r="AF92" s="12"/>
     </row>
     <row r="93" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A93" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B93" s="47">
+      <c r="B93" s="43">
         <f>C91+B68</f>
         <v>10.773108687500001</v>
       </c>
-      <c r="C93" s="48"/>
-      <c r="D93" s="48"/>
-      <c r="E93" s="48"/>
-      <c r="F93" s="48"/>
-      <c r="G93" s="49"/>
+      <c r="C93" s="44"/>
+      <c r="D93" s="44"/>
+      <c r="E93" s="44"/>
+      <c r="F93" s="44"/>
+      <c r="G93" s="45"/>
       <c r="H93" s="12"/>
       <c r="I93" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J93" s="47">
+      <c r="J93" s="43">
         <f>K91+J68</f>
         <v>0</v>
       </c>
-      <c r="K93" s="48"/>
-      <c r="L93" s="48"/>
-      <c r="M93" s="48"/>
-      <c r="N93" s="48"/>
-      <c r="O93" s="49"/>
+      <c r="K93" s="44"/>
+      <c r="L93" s="44"/>
+      <c r="M93" s="44"/>
+      <c r="N93" s="44"/>
+      <c r="O93" s="45"/>
       <c r="P93" s="12"/>
       <c r="Q93" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R93" s="47">
+      <c r="R93" s="43">
         <f>S91+R68</f>
         <v>0</v>
       </c>
-      <c r="S93" s="48"/>
-      <c r="T93" s="48"/>
-      <c r="U93" s="48"/>
-      <c r="V93" s="48"/>
-      <c r="W93" s="49"/>
+      <c r="S93" s="44"/>
+      <c r="T93" s="44"/>
+      <c r="U93" s="44"/>
+      <c r="V93" s="44"/>
+      <c r="W93" s="45"/>
       <c r="X93" s="12"/>
       <c r="Y93" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z93" s="47">
+      <c r="Z93" s="43">
         <f>AA91+Z68</f>
         <v>0</v>
       </c>
-      <c r="AA93" s="48"/>
-      <c r="AB93" s="48"/>
-      <c r="AC93" s="48"/>
-      <c r="AD93" s="48"/>
-      <c r="AE93" s="49"/>
+      <c r="AA93" s="44"/>
+      <c r="AB93" s="44"/>
+      <c r="AC93" s="44"/>
+      <c r="AD93" s="44"/>
+      <c r="AE93" s="45"/>
       <c r="AF93" s="12"/>
     </row>
     <row r="94" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A94" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B94" s="47">
+      <c r="B94" s="43">
         <f>IFERROR((G91/10/B92),0)</f>
         <v>0</v>
       </c>
-      <c r="C94" s="48"/>
-      <c r="D94" s="48"/>
-      <c r="E94" s="48"/>
-      <c r="F94" s="48"/>
-      <c r="G94" s="49"/>
+      <c r="C94" s="44"/>
+      <c r="D94" s="44"/>
+      <c r="E94" s="44"/>
+      <c r="F94" s="44"/>
+      <c r="G94" s="45"/>
       <c r="H94" s="12"/>
       <c r="I94" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J94" s="47">
+      <c r="J94" s="43">
         <f>IFERROR((O91/10/J92),0)</f>
         <v>0</v>
       </c>
-      <c r="K94" s="48"/>
-      <c r="L94" s="48"/>
-      <c r="M94" s="48"/>
-      <c r="N94" s="48"/>
-      <c r="O94" s="49"/>
+      <c r="K94" s="44"/>
+      <c r="L94" s="44"/>
+      <c r="M94" s="44"/>
+      <c r="N94" s="44"/>
+      <c r="O94" s="45"/>
       <c r="P94" s="12"/>
       <c r="Q94" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R94" s="47">
+      <c r="R94" s="43">
         <f>IFERROR((W91/10/R92),0)</f>
         <v>0</v>
       </c>
-      <c r="S94" s="48"/>
-      <c r="T94" s="48"/>
-      <c r="U94" s="48"/>
-      <c r="V94" s="48"/>
-      <c r="W94" s="49"/>
+      <c r="S94" s="44"/>
+      <c r="T94" s="44"/>
+      <c r="U94" s="44"/>
+      <c r="V94" s="44"/>
+      <c r="W94" s="45"/>
       <c r="X94" s="12"/>
       <c r="Y94" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z94" s="47">
+      <c r="Z94" s="43">
         <f>IFERROR((AE91/10/Z92),0)</f>
         <v>0</v>
       </c>
-      <c r="AA94" s="48"/>
-      <c r="AB94" s="48"/>
-      <c r="AC94" s="48"/>
-      <c r="AD94" s="48"/>
-      <c r="AE94" s="49"/>
+      <c r="AA94" s="44"/>
+      <c r="AB94" s="44"/>
+      <c r="AC94" s="44"/>
+      <c r="AD94" s="44"/>
+      <c r="AE94" s="45"/>
       <c r="AF94" s="12"/>
     </row>
     <row r="95" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A95" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B95" s="47">
+      <c r="B95" s="43">
         <f>IFERROR((9.82 * F91) * LN(B92/B93),0)</f>
         <v>0</v>
       </c>
-      <c r="C95" s="48"/>
-      <c r="D95" s="48"/>
-      <c r="E95" s="48"/>
-      <c r="F95" s="48"/>
-      <c r="G95" s="49"/>
+      <c r="C95" s="44"/>
+      <c r="D95" s="44"/>
+      <c r="E95" s="44"/>
+      <c r="F95" s="44"/>
+      <c r="G95" s="45"/>
       <c r="H95" s="12"/>
       <c r="I95" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J95" s="47">
+      <c r="J95" s="43">
         <f>IFERROR((9.82 * N91) * LN(J92/J93),0)</f>
         <v>0</v>
       </c>
-      <c r="K95" s="48"/>
-      <c r="L95" s="48"/>
-      <c r="M95" s="48"/>
-      <c r="N95" s="48"/>
-      <c r="O95" s="49"/>
+      <c r="K95" s="44"/>
+      <c r="L95" s="44"/>
+      <c r="M95" s="44"/>
+      <c r="N95" s="44"/>
+      <c r="O95" s="45"/>
       <c r="P95" s="12"/>
       <c r="Q95" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R95" s="47">
+      <c r="R95" s="43">
         <f>IFERROR((9.82 * V91) * LN(R92/R93),0)</f>
         <v>0</v>
       </c>
-      <c r="S95" s="48"/>
-      <c r="T95" s="48"/>
-      <c r="U95" s="48"/>
-      <c r="V95" s="48"/>
-      <c r="W95" s="49"/>
+      <c r="S95" s="44"/>
+      <c r="T95" s="44"/>
+      <c r="U95" s="44"/>
+      <c r="V95" s="44"/>
+      <c r="W95" s="45"/>
       <c r="X95" s="12"/>
       <c r="Y95" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z95" s="47">
+      <c r="Z95" s="43">
         <f>IFERROR((9.82 * AD91) * LN(Z92/Z93),0)</f>
         <v>0</v>
       </c>
-      <c r="AA95" s="48"/>
-      <c r="AB95" s="48"/>
-      <c r="AC95" s="48"/>
-      <c r="AD95" s="48"/>
-      <c r="AE95" s="49"/>
+      <c r="AA95" s="44"/>
+      <c r="AB95" s="44"/>
+      <c r="AC95" s="44"/>
+      <c r="AD95" s="44"/>
+      <c r="AE95" s="45"/>
       <c r="AF95" s="12"/>
     </row>
     <row r="96" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B96" s="51">
+      <c r="B96" s="40">
         <f>B95+B72</f>
         <v>8003.3365648910458</v>
       </c>
-      <c r="C96" s="52"/>
-      <c r="D96" s="52"/>
-      <c r="E96" s="52"/>
-      <c r="F96" s="52"/>
-      <c r="G96" s="53"/>
+      <c r="C96" s="41"/>
+      <c r="D96" s="41"/>
+      <c r="E96" s="41"/>
+      <c r="F96" s="41"/>
+      <c r="G96" s="42"/>
       <c r="H96" s="12"/>
       <c r="I96" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J96" s="51">
+      <c r="J96" s="40">
         <f>J95+J72</f>
         <v>0</v>
       </c>
-      <c r="K96" s="52"/>
-      <c r="L96" s="52"/>
-      <c r="M96" s="52"/>
-      <c r="N96" s="52"/>
-      <c r="O96" s="53"/>
+      <c r="K96" s="41"/>
+      <c r="L96" s="41"/>
+      <c r="M96" s="41"/>
+      <c r="N96" s="41"/>
+      <c r="O96" s="42"/>
       <c r="P96" s="12"/>
       <c r="Q96" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R96" s="51">
+      <c r="R96" s="40">
         <f>R95+R72</f>
         <v>0</v>
       </c>
-      <c r="S96" s="52"/>
-      <c r="T96" s="52"/>
-      <c r="U96" s="52"/>
-      <c r="V96" s="52"/>
-      <c r="W96" s="53"/>
+      <c r="S96" s="41"/>
+      <c r="T96" s="41"/>
+      <c r="U96" s="41"/>
+      <c r="V96" s="41"/>
+      <c r="W96" s="42"/>
       <c r="X96" s="12"/>
       <c r="Y96" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z96" s="51">
+      <c r="Z96" s="40">
         <f>Z95+Z72</f>
         <v>0</v>
       </c>
-      <c r="AA96" s="52"/>
-      <c r="AB96" s="52"/>
-      <c r="AC96" s="52"/>
-      <c r="AD96" s="52"/>
-      <c r="AE96" s="53"/>
+      <c r="AA96" s="41"/>
+      <c r="AB96" s="41"/>
+      <c r="AC96" s="41"/>
+      <c r="AD96" s="41"/>
+      <c r="AE96" s="42"/>
       <c r="AF96" s="12"/>
     </row>
     <row r="97" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -37583,270 +37632,270 @@
       <c r="A116" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B116" s="47">
+      <c r="B116" s="43">
         <f>E115+B92</f>
         <v>10.773108687500001</v>
       </c>
-      <c r="C116" s="48"/>
-      <c r="D116" s="48"/>
-      <c r="E116" s="48"/>
-      <c r="F116" s="48"/>
-      <c r="G116" s="49"/>
+      <c r="C116" s="44"/>
+      <c r="D116" s="44"/>
+      <c r="E116" s="44"/>
+      <c r="F116" s="44"/>
+      <c r="G116" s="45"/>
       <c r="H116" s="12"/>
       <c r="I116" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J116" s="47">
+      <c r="J116" s="43">
         <f>M115+J92</f>
         <v>0</v>
       </c>
-      <c r="K116" s="48"/>
-      <c r="L116" s="48"/>
-      <c r="M116" s="48"/>
-      <c r="N116" s="48"/>
-      <c r="O116" s="49"/>
+      <c r="K116" s="44"/>
+      <c r="L116" s="44"/>
+      <c r="M116" s="44"/>
+      <c r="N116" s="44"/>
+      <c r="O116" s="45"/>
       <c r="P116" s="12"/>
       <c r="Q116" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="R116" s="47">
+      <c r="R116" s="43">
         <f>U115+R92</f>
         <v>0</v>
       </c>
-      <c r="S116" s="48"/>
-      <c r="T116" s="48"/>
-      <c r="U116" s="48"/>
-      <c r="V116" s="48"/>
-      <c r="W116" s="49"/>
+      <c r="S116" s="44"/>
+      <c r="T116" s="44"/>
+      <c r="U116" s="44"/>
+      <c r="V116" s="44"/>
+      <c r="W116" s="45"/>
       <c r="X116" s="12"/>
       <c r="Y116" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="Z116" s="47">
+      <c r="Z116" s="43">
         <f>AC115+Z92</f>
         <v>0</v>
       </c>
-      <c r="AA116" s="48"/>
-      <c r="AB116" s="48"/>
-      <c r="AC116" s="48"/>
-      <c r="AD116" s="48"/>
-      <c r="AE116" s="49"/>
+      <c r="AA116" s="44"/>
+      <c r="AB116" s="44"/>
+      <c r="AC116" s="44"/>
+      <c r="AD116" s="44"/>
+      <c r="AE116" s="45"/>
       <c r="AF116" s="12"/>
     </row>
     <row r="117" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A117" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B117" s="47">
+      <c r="B117" s="43">
         <f>C115+B92</f>
         <v>10.773108687500001</v>
       </c>
-      <c r="C117" s="48"/>
-      <c r="D117" s="48"/>
-      <c r="E117" s="48"/>
-      <c r="F117" s="48"/>
-      <c r="G117" s="49"/>
+      <c r="C117" s="44"/>
+      <c r="D117" s="44"/>
+      <c r="E117" s="44"/>
+      <c r="F117" s="44"/>
+      <c r="G117" s="45"/>
       <c r="H117" s="12"/>
       <c r="I117" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="J117" s="47">
+      <c r="J117" s="43">
         <f>K115+J92</f>
         <v>0</v>
       </c>
-      <c r="K117" s="48"/>
-      <c r="L117" s="48"/>
-      <c r="M117" s="48"/>
-      <c r="N117" s="48"/>
-      <c r="O117" s="49"/>
+      <c r="K117" s="44"/>
+      <c r="L117" s="44"/>
+      <c r="M117" s="44"/>
+      <c r="N117" s="44"/>
+      <c r="O117" s="45"/>
       <c r="P117" s="12"/>
       <c r="Q117" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R117" s="47">
+      <c r="R117" s="43">
         <f>S115+R92</f>
         <v>0</v>
       </c>
-      <c r="S117" s="48"/>
-      <c r="T117" s="48"/>
-      <c r="U117" s="48"/>
-      <c r="V117" s="48"/>
-      <c r="W117" s="49"/>
+      <c r="S117" s="44"/>
+      <c r="T117" s="44"/>
+      <c r="U117" s="44"/>
+      <c r="V117" s="44"/>
+      <c r="W117" s="45"/>
       <c r="X117" s="12"/>
       <c r="Y117" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z117" s="47">
+      <c r="Z117" s="43">
         <f>AA115+Z92</f>
         <v>0</v>
       </c>
-      <c r="AA117" s="48"/>
-      <c r="AB117" s="48"/>
-      <c r="AC117" s="48"/>
-      <c r="AD117" s="48"/>
-      <c r="AE117" s="49"/>
+      <c r="AA117" s="44"/>
+      <c r="AB117" s="44"/>
+      <c r="AC117" s="44"/>
+      <c r="AD117" s="44"/>
+      <c r="AE117" s="45"/>
       <c r="AF117" s="12"/>
     </row>
     <row r="118" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A118" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B118" s="47">
+      <c r="B118" s="43">
         <f>IFERROR((G115/10/B116),0)</f>
         <v>0</v>
       </c>
-      <c r="C118" s="48"/>
-      <c r="D118" s="48"/>
-      <c r="E118" s="48"/>
-      <c r="F118" s="48"/>
-      <c r="G118" s="49"/>
+      <c r="C118" s="44"/>
+      <c r="D118" s="44"/>
+      <c r="E118" s="44"/>
+      <c r="F118" s="44"/>
+      <c r="G118" s="45"/>
       <c r="H118" s="12"/>
       <c r="I118" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J118" s="47">
+      <c r="J118" s="43">
         <f>IFERROR((O115/10/J116),0)</f>
         <v>0</v>
       </c>
-      <c r="K118" s="48"/>
-      <c r="L118" s="48"/>
-      <c r="M118" s="48"/>
-      <c r="N118" s="48"/>
-      <c r="O118" s="49"/>
+      <c r="K118" s="44"/>
+      <c r="L118" s="44"/>
+      <c r="M118" s="44"/>
+      <c r="N118" s="44"/>
+      <c r="O118" s="45"/>
       <c r="P118" s="12"/>
       <c r="Q118" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="R118" s="47">
+      <c r="R118" s="43">
         <f>IFERROR((W115/10/R116),0)</f>
         <v>0</v>
       </c>
-      <c r="S118" s="48"/>
-      <c r="T118" s="48"/>
-      <c r="U118" s="48"/>
-      <c r="V118" s="48"/>
-      <c r="W118" s="49"/>
+      <c r="S118" s="44"/>
+      <c r="T118" s="44"/>
+      <c r="U118" s="44"/>
+      <c r="V118" s="44"/>
+      <c r="W118" s="45"/>
       <c r="X118" s="12"/>
       <c r="Y118" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z118" s="47">
+      <c r="Z118" s="43">
         <f>IFERROR((AE115/10/Z116),0)</f>
         <v>0</v>
       </c>
-      <c r="AA118" s="48"/>
-      <c r="AB118" s="48"/>
-      <c r="AC118" s="48"/>
-      <c r="AD118" s="48"/>
-      <c r="AE118" s="49"/>
+      <c r="AA118" s="44"/>
+      <c r="AB118" s="44"/>
+      <c r="AC118" s="44"/>
+      <c r="AD118" s="44"/>
+      <c r="AE118" s="45"/>
       <c r="AF118" s="12"/>
     </row>
     <row r="119" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A119" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B119" s="47">
+      <c r="B119" s="43">
         <f>IFERROR((9.82 * F115) * LN(B116/B117),0)</f>
         <v>0</v>
       </c>
-      <c r="C119" s="48"/>
-      <c r="D119" s="48"/>
-      <c r="E119" s="48"/>
-      <c r="F119" s="48"/>
-      <c r="G119" s="49"/>
+      <c r="C119" s="44"/>
+      <c r="D119" s="44"/>
+      <c r="E119" s="44"/>
+      <c r="F119" s="44"/>
+      <c r="G119" s="45"/>
       <c r="H119" s="12"/>
       <c r="I119" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="J119" s="47">
+      <c r="J119" s="43">
         <f>IFERROR((9.82 * N115) * LN(J116/J117),0)</f>
         <v>0</v>
       </c>
-      <c r="K119" s="48"/>
-      <c r="L119" s="48"/>
-      <c r="M119" s="48"/>
-      <c r="N119" s="48"/>
-      <c r="O119" s="49"/>
+      <c r="K119" s="44"/>
+      <c r="L119" s="44"/>
+      <c r="M119" s="44"/>
+      <c r="N119" s="44"/>
+      <c r="O119" s="45"/>
       <c r="P119" s="12"/>
       <c r="Q119" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="R119" s="47">
+      <c r="R119" s="43">
         <f>IFERROR((9.82 * V115) * LN(R116/R117),0)</f>
         <v>0</v>
       </c>
-      <c r="S119" s="48"/>
-      <c r="T119" s="48"/>
-      <c r="U119" s="48"/>
-      <c r="V119" s="48"/>
-      <c r="W119" s="49"/>
+      <c r="S119" s="44"/>
+      <c r="T119" s="44"/>
+      <c r="U119" s="44"/>
+      <c r="V119" s="44"/>
+      <c r="W119" s="45"/>
       <c r="X119" s="12"/>
       <c r="Y119" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Z119" s="47">
+      <c r="Z119" s="43">
         <f>IFERROR((9.82 * AD115) * LN(Z116/Z117),0)</f>
         <v>0</v>
       </c>
-      <c r="AA119" s="48"/>
-      <c r="AB119" s="48"/>
-      <c r="AC119" s="48"/>
-      <c r="AD119" s="48"/>
-      <c r="AE119" s="49"/>
+      <c r="AA119" s="44"/>
+      <c r="AB119" s="44"/>
+      <c r="AC119" s="44"/>
+      <c r="AD119" s="44"/>
+      <c r="AE119" s="45"/>
       <c r="AF119" s="12"/>
     </row>
     <row r="120" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B120" s="51">
+      <c r="B120" s="40">
         <f>B119+B96</f>
         <v>8003.3365648910458</v>
       </c>
-      <c r="C120" s="52"/>
-      <c r="D120" s="52"/>
-      <c r="E120" s="52"/>
-      <c r="F120" s="52"/>
-      <c r="G120" s="53"/>
+      <c r="C120" s="41"/>
+      <c r="D120" s="41"/>
+      <c r="E120" s="41"/>
+      <c r="F120" s="41"/>
+      <c r="G120" s="42"/>
       <c r="H120" s="12"/>
       <c r="I120" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="J120" s="51">
+      <c r="J120" s="40">
         <f>J119+J96</f>
         <v>0</v>
       </c>
-      <c r="K120" s="52"/>
-      <c r="L120" s="52"/>
-      <c r="M120" s="52"/>
-      <c r="N120" s="52"/>
-      <c r="O120" s="53"/>
+      <c r="K120" s="41"/>
+      <c r="L120" s="41"/>
+      <c r="M120" s="41"/>
+      <c r="N120" s="41"/>
+      <c r="O120" s="42"/>
       <c r="P120" s="12"/>
       <c r="Q120" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R120" s="51">
+      <c r="R120" s="40">
         <f>R119+R96</f>
         <v>0</v>
       </c>
-      <c r="S120" s="52"/>
-      <c r="T120" s="52"/>
-      <c r="U120" s="52"/>
-      <c r="V120" s="52"/>
-      <c r="W120" s="53"/>
+      <c r="S120" s="41"/>
+      <c r="T120" s="41"/>
+      <c r="U120" s="41"/>
+      <c r="V120" s="41"/>
+      <c r="W120" s="42"/>
       <c r="X120" s="12"/>
       <c r="Y120" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="Z120" s="51">
+      <c r="Z120" s="40">
         <f>Z119+Z96</f>
         <v>0</v>
       </c>
-      <c r="AA120" s="52"/>
-      <c r="AB120" s="52"/>
-      <c r="AC120" s="52"/>
-      <c r="AD120" s="52"/>
-      <c r="AE120" s="53"/>
+      <c r="AA120" s="41"/>
+      <c r="AB120" s="41"/>
+      <c r="AC120" s="41"/>
+      <c r="AD120" s="41"/>
+      <c r="AE120" s="42"/>
       <c r="AF120" s="12"/>
     </row>
     <row r="121" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -37884,315 +37933,315 @@
       <c r="AF121" s="12"/>
     </row>
     <row r="122" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="42" t="s">
+      <c r="A122" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="B122" s="43"/>
-      <c r="C122" s="43"/>
-      <c r="D122" s="43"/>
-      <c r="E122" s="43"/>
-      <c r="F122" s="43"/>
-      <c r="G122" s="44"/>
+      <c r="B122" s="48"/>
+      <c r="C122" s="48"/>
+      <c r="D122" s="48"/>
+      <c r="E122" s="48"/>
+      <c r="F122" s="48"/>
+      <c r="G122" s="49"/>
       <c r="H122" s="12"/>
-      <c r="I122" s="42" t="s">
+      <c r="I122" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="J122" s="43"/>
-      <c r="K122" s="43"/>
-      <c r="L122" s="43"/>
-      <c r="M122" s="43"/>
-      <c r="N122" s="43"/>
-      <c r="O122" s="44"/>
+      <c r="J122" s="48"/>
+      <c r="K122" s="48"/>
+      <c r="L122" s="48"/>
+      <c r="M122" s="48"/>
+      <c r="N122" s="48"/>
+      <c r="O122" s="49"/>
       <c r="P122" s="12"/>
-      <c r="Q122" s="42" t="s">
+      <c r="Q122" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="R122" s="43"/>
-      <c r="S122" s="43"/>
-      <c r="T122" s="43"/>
-      <c r="U122" s="43"/>
-      <c r="V122" s="43"/>
-      <c r="W122" s="44"/>
+      <c r="R122" s="48"/>
+      <c r="S122" s="48"/>
+      <c r="T122" s="48"/>
+      <c r="U122" s="48"/>
+      <c r="V122" s="48"/>
+      <c r="W122" s="49"/>
       <c r="X122" s="12"/>
-      <c r="Y122" s="42" t="s">
+      <c r="Y122" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="Z122" s="43"/>
-      <c r="AA122" s="43"/>
-      <c r="AB122" s="43"/>
-      <c r="AC122" s="43"/>
-      <c r="AD122" s="43"/>
-      <c r="AE122" s="44"/>
+      <c r="Z122" s="48"/>
+      <c r="AA122" s="48"/>
+      <c r="AB122" s="48"/>
+      <c r="AC122" s="48"/>
+      <c r="AD122" s="48"/>
+      <c r="AE122" s="49"/>
       <c r="AF122" s="12"/>
     </row>
     <row r="123" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A123" s="45" t="s">
+      <c r="A123" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="B123" s="45"/>
-      <c r="C123" s="45"/>
-      <c r="D123" s="46">
+      <c r="B123" s="52"/>
+      <c r="C123" s="52"/>
+      <c r="D123" s="51">
         <f>B115</f>
         <v>3</v>
       </c>
-      <c r="E123" s="46"/>
-      <c r="F123" s="46"/>
-      <c r="G123" s="46"/>
+      <c r="E123" s="51"/>
+      <c r="F123" s="51"/>
+      <c r="G123" s="51"/>
       <c r="H123" s="12"/>
-      <c r="I123" s="45" t="s">
+      <c r="I123" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="J123" s="45"/>
-      <c r="K123" s="45"/>
-      <c r="L123" s="46">
+      <c r="J123" s="52"/>
+      <c r="K123" s="52"/>
+      <c r="L123" s="51">
         <f>J115</f>
         <v>0</v>
       </c>
-      <c r="M123" s="46"/>
-      <c r="N123" s="46"/>
-      <c r="O123" s="46"/>
+      <c r="M123" s="51"/>
+      <c r="N123" s="51"/>
+      <c r="O123" s="51"/>
       <c r="P123" s="12"/>
-      <c r="Q123" s="45" t="s">
+      <c r="Q123" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="R123" s="45"/>
-      <c r="S123" s="45"/>
-      <c r="T123" s="46">
+      <c r="R123" s="52"/>
+      <c r="S123" s="52"/>
+      <c r="T123" s="51">
         <f>R115</f>
         <v>0</v>
       </c>
-      <c r="U123" s="46"/>
-      <c r="V123" s="46"/>
-      <c r="W123" s="46"/>
+      <c r="U123" s="51"/>
+      <c r="V123" s="51"/>
+      <c r="W123" s="51"/>
       <c r="X123" s="12"/>
-      <c r="Y123" s="45" t="s">
+      <c r="Y123" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="Z123" s="45"/>
-      <c r="AA123" s="45"/>
-      <c r="AB123" s="46">
+      <c r="Z123" s="52"/>
+      <c r="AA123" s="52"/>
+      <c r="AB123" s="51">
         <f>Z115</f>
         <v>0</v>
       </c>
-      <c r="AC123" s="46"/>
-      <c r="AD123" s="46"/>
-      <c r="AE123" s="46"/>
+      <c r="AC123" s="51"/>
+      <c r="AD123" s="51"/>
+      <c r="AE123" s="51"/>
       <c r="AF123" s="12"/>
     </row>
     <row r="124" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A124" s="40" t="s">
+      <c r="A124" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B124" s="40"/>
-      <c r="C124" s="40"/>
-      <c r="D124" s="41">
+      <c r="B124" s="53"/>
+      <c r="C124" s="53"/>
+      <c r="D124" s="50">
         <f>B116</f>
         <v>10.773108687500001</v>
       </c>
-      <c r="E124" s="41"/>
-      <c r="F124" s="41"/>
-      <c r="G124" s="41"/>
+      <c r="E124" s="50"/>
+      <c r="F124" s="50"/>
+      <c r="G124" s="50"/>
       <c r="H124" s="12"/>
-      <c r="I124" s="40" t="s">
+      <c r="I124" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="J124" s="40"/>
-      <c r="K124" s="40"/>
-      <c r="L124" s="41">
+      <c r="J124" s="53"/>
+      <c r="K124" s="53"/>
+      <c r="L124" s="50">
         <f>J116</f>
         <v>0</v>
       </c>
-      <c r="M124" s="41"/>
-      <c r="N124" s="41"/>
-      <c r="O124" s="41"/>
+      <c r="M124" s="50"/>
+      <c r="N124" s="50"/>
+      <c r="O124" s="50"/>
       <c r="P124" s="12"/>
-      <c r="Q124" s="40" t="s">
+      <c r="Q124" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="R124" s="40"/>
-      <c r="S124" s="40"/>
-      <c r="T124" s="41">
+      <c r="R124" s="53"/>
+      <c r="S124" s="53"/>
+      <c r="T124" s="50">
         <f>R116</f>
         <v>0</v>
       </c>
-      <c r="U124" s="41"/>
-      <c r="V124" s="41"/>
-      <c r="W124" s="41"/>
+      <c r="U124" s="50"/>
+      <c r="V124" s="50"/>
+      <c r="W124" s="50"/>
       <c r="X124" s="12"/>
-      <c r="Y124" s="40" t="s">
+      <c r="Y124" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="Z124" s="40"/>
-      <c r="AA124" s="40"/>
-      <c r="AB124" s="41">
+      <c r="Z124" s="53"/>
+      <c r="AA124" s="53"/>
+      <c r="AB124" s="50">
         <f>Z116</f>
         <v>0</v>
       </c>
-      <c r="AC124" s="41"/>
-      <c r="AD124" s="41"/>
-      <c r="AE124" s="41"/>
+      <c r="AC124" s="50"/>
+      <c r="AD124" s="50"/>
+      <c r="AE124" s="50"/>
       <c r="AF124" s="12"/>
     </row>
     <row r="125" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A125" s="40" t="s">
+      <c r="A125" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B125" s="40"/>
-      <c r="C125" s="40"/>
-      <c r="D125" s="41">
+      <c r="B125" s="53"/>
+      <c r="C125" s="53"/>
+      <c r="D125" s="50">
         <f>D115+D91+D67+D43+D19</f>
         <v>8.9766162500000011</v>
       </c>
-      <c r="E125" s="41"/>
-      <c r="F125" s="41"/>
-      <c r="G125" s="41"/>
+      <c r="E125" s="50"/>
+      <c r="F125" s="50"/>
+      <c r="G125" s="50"/>
       <c r="H125" s="12"/>
-      <c r="I125" s="40" t="s">
+      <c r="I125" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="J125" s="40"/>
-      <c r="K125" s="40"/>
-      <c r="L125" s="41">
+      <c r="J125" s="53"/>
+      <c r="K125" s="53"/>
+      <c r="L125" s="50">
         <f>L115+L91+L67+L43+L19</f>
         <v>0</v>
       </c>
-      <c r="M125" s="41"/>
-      <c r="N125" s="41"/>
-      <c r="O125" s="41"/>
+      <c r="M125" s="50"/>
+      <c r="N125" s="50"/>
+      <c r="O125" s="50"/>
       <c r="P125" s="12"/>
-      <c r="Q125" s="40" t="s">
+      <c r="Q125" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="R125" s="40"/>
-      <c r="S125" s="40"/>
-      <c r="T125" s="41">
+      <c r="R125" s="53"/>
+      <c r="S125" s="53"/>
+      <c r="T125" s="50">
         <f>T115+T91+T67+T43+T19</f>
         <v>0</v>
       </c>
-      <c r="U125" s="41"/>
-      <c r="V125" s="41"/>
-      <c r="W125" s="41"/>
+      <c r="U125" s="50"/>
+      <c r="V125" s="50"/>
+      <c r="W125" s="50"/>
       <c r="X125" s="12"/>
-      <c r="Y125" s="40" t="s">
+      <c r="Y125" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="Z125" s="40"/>
-      <c r="AA125" s="40"/>
-      <c r="AB125" s="41">
+      <c r="Z125" s="53"/>
+      <c r="AA125" s="53"/>
+      <c r="AB125" s="50">
         <f>AB115+AB91+AB67+AB43+AB19</f>
         <v>0</v>
       </c>
-      <c r="AC125" s="41"/>
-      <c r="AD125" s="41"/>
-      <c r="AE125" s="41"/>
+      <c r="AC125" s="50"/>
+      <c r="AD125" s="50"/>
+      <c r="AE125" s="50"/>
       <c r="AF125" s="12"/>
     </row>
     <row r="126" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A126" s="40" t="s">
+      <c r="A126" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B126" s="40"/>
-      <c r="C126" s="40"/>
-      <c r="D126" s="41">
+      <c r="B126" s="53"/>
+      <c r="C126" s="53"/>
+      <c r="D126" s="50">
         <f>D124-D125</f>
         <v>1.7964924374999995</v>
       </c>
-      <c r="E126" s="41"/>
-      <c r="F126" s="41"/>
-      <c r="G126" s="41"/>
+      <c r="E126" s="50"/>
+      <c r="F126" s="50"/>
+      <c r="G126" s="50"/>
       <c r="H126" s="12"/>
-      <c r="I126" s="40" t="s">
+      <c r="I126" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="J126" s="40"/>
-      <c r="K126" s="40"/>
-      <c r="L126" s="41">
+      <c r="J126" s="53"/>
+      <c r="K126" s="53"/>
+      <c r="L126" s="50">
         <f>L124-L125</f>
         <v>0</v>
       </c>
-      <c r="M126" s="41"/>
-      <c r="N126" s="41"/>
-      <c r="O126" s="41"/>
+      <c r="M126" s="50"/>
+      <c r="N126" s="50"/>
+      <c r="O126" s="50"/>
       <c r="P126" s="12"/>
-      <c r="Q126" s="40" t="s">
+      <c r="Q126" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="R126" s="40"/>
-      <c r="S126" s="40"/>
-      <c r="T126" s="41">
+      <c r="R126" s="53"/>
+      <c r="S126" s="53"/>
+      <c r="T126" s="50">
         <f>T124-T125</f>
         <v>0</v>
       </c>
-      <c r="U126" s="41"/>
-      <c r="V126" s="41"/>
-      <c r="W126" s="41"/>
+      <c r="U126" s="50"/>
+      <c r="V126" s="50"/>
+      <c r="W126" s="50"/>
       <c r="X126" s="12"/>
-      <c r="Y126" s="40" t="s">
+      <c r="Y126" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="Z126" s="40"/>
-      <c r="AA126" s="40"/>
-      <c r="AB126" s="41">
+      <c r="Z126" s="53"/>
+      <c r="AA126" s="53"/>
+      <c r="AB126" s="50">
         <f>AB124-AB125</f>
         <v>0</v>
       </c>
-      <c r="AC126" s="41"/>
-      <c r="AD126" s="41"/>
-      <c r="AE126" s="41"/>
+      <c r="AC126" s="50"/>
+      <c r="AD126" s="50"/>
+      <c r="AE126" s="50"/>
       <c r="AF126" s="12"/>
     </row>
     <row r="127" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A127" s="40" t="s">
+      <c r="A127" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="B127" s="40"/>
-      <c r="C127" s="40"/>
-      <c r="D127" s="41">
+      <c r="B127" s="53"/>
+      <c r="C127" s="53"/>
+      <c r="D127" s="50">
         <f>B120</f>
         <v>8003.3365648910458</v>
       </c>
-      <c r="E127" s="41"/>
-      <c r="F127" s="41"/>
-      <c r="G127" s="41"/>
+      <c r="E127" s="50"/>
+      <c r="F127" s="50"/>
+      <c r="G127" s="50"/>
       <c r="H127" s="12"/>
-      <c r="I127" s="40" t="s">
+      <c r="I127" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="J127" s="40"/>
-      <c r="K127" s="40"/>
-      <c r="L127" s="41">
+      <c r="J127" s="53"/>
+      <c r="K127" s="53"/>
+      <c r="L127" s="50">
         <f>J120</f>
         <v>0</v>
       </c>
-      <c r="M127" s="41"/>
-      <c r="N127" s="41"/>
-      <c r="O127" s="41"/>
+      <c r="M127" s="50"/>
+      <c r="N127" s="50"/>
+      <c r="O127" s="50"/>
       <c r="P127" s="12"/>
-      <c r="Q127" s="40" t="s">
+      <c r="Q127" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="R127" s="40"/>
-      <c r="S127" s="40"/>
-      <c r="T127" s="41">
+      <c r="R127" s="53"/>
+      <c r="S127" s="53"/>
+      <c r="T127" s="50">
         <f>R120</f>
         <v>0</v>
       </c>
-      <c r="U127" s="41"/>
-      <c r="V127" s="41"/>
-      <c r="W127" s="41"/>
+      <c r="U127" s="50"/>
+      <c r="V127" s="50"/>
+      <c r="W127" s="50"/>
       <c r="X127" s="12"/>
-      <c r="Y127" s="40" t="s">
+      <c r="Y127" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="Z127" s="40"/>
-      <c r="AA127" s="40"/>
-      <c r="AB127" s="41">
+      <c r="Z127" s="53"/>
+      <c r="AA127" s="53"/>
+      <c r="AB127" s="50">
         <f>Z120</f>
         <v>0</v>
       </c>
-      <c r="AC127" s="41"/>
-      <c r="AD127" s="41"/>
-      <c r="AE127" s="41"/>
+      <c r="AC127" s="50"/>
+      <c r="AD127" s="50"/>
+      <c r="AE127" s="50"/>
       <c r="AF127" s="12"/>
     </row>
     <row r="128" spans="1:32" x14ac:dyDescent="0.25">
@@ -38231,87 +38280,49 @@
     </row>
   </sheetData>
   <mergeCells count="148">
-    <mergeCell ref="B120:G120"/>
-    <mergeCell ref="J120:O120"/>
-    <mergeCell ref="R120:W120"/>
-    <mergeCell ref="Z120:AE120"/>
-    <mergeCell ref="B119:G119"/>
-    <mergeCell ref="J119:O119"/>
-    <mergeCell ref="R119:W119"/>
-    <mergeCell ref="Z119:AE119"/>
-    <mergeCell ref="B118:G118"/>
-    <mergeCell ref="J118:O118"/>
-    <mergeCell ref="R118:W118"/>
-    <mergeCell ref="Z118:AE118"/>
-    <mergeCell ref="B117:G117"/>
-    <mergeCell ref="J117:O117"/>
-    <mergeCell ref="R117:W117"/>
-    <mergeCell ref="Z117:AE117"/>
-    <mergeCell ref="B116:G116"/>
-    <mergeCell ref="J116:O116"/>
-    <mergeCell ref="R116:W116"/>
-    <mergeCell ref="Z116:AE116"/>
-    <mergeCell ref="B96:G96"/>
-    <mergeCell ref="J96:O96"/>
-    <mergeCell ref="R96:W96"/>
-    <mergeCell ref="Z96:AE96"/>
-    <mergeCell ref="B95:G95"/>
-    <mergeCell ref="J95:O95"/>
-    <mergeCell ref="R95:W95"/>
-    <mergeCell ref="Z95:AE95"/>
-    <mergeCell ref="B94:G94"/>
-    <mergeCell ref="J94:O94"/>
-    <mergeCell ref="R94:W94"/>
-    <mergeCell ref="Z94:AE94"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="J93:O93"/>
-    <mergeCell ref="R93:W93"/>
-    <mergeCell ref="Z93:AE93"/>
-    <mergeCell ref="B92:G92"/>
-    <mergeCell ref="J92:O92"/>
-    <mergeCell ref="R92:W92"/>
-    <mergeCell ref="Z92:AE92"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="J72:O72"/>
-    <mergeCell ref="R72:W72"/>
-    <mergeCell ref="Z72:AE72"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="J71:O71"/>
-    <mergeCell ref="R71:W71"/>
-    <mergeCell ref="Z71:AE71"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="J70:O70"/>
-    <mergeCell ref="R70:W70"/>
-    <mergeCell ref="Z70:AE70"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="J69:O69"/>
-    <mergeCell ref="R69:W69"/>
-    <mergeCell ref="Z69:AE69"/>
-    <mergeCell ref="B68:G68"/>
-    <mergeCell ref="J68:O68"/>
-    <mergeCell ref="R68:W68"/>
-    <mergeCell ref="Z68:AE68"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="J48:O48"/>
-    <mergeCell ref="R48:W48"/>
-    <mergeCell ref="Z48:AE48"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="J47:O47"/>
-    <mergeCell ref="R47:W47"/>
-    <mergeCell ref="Z47:AE47"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="J46:O46"/>
-    <mergeCell ref="R46:W46"/>
-    <mergeCell ref="Z46:AE46"/>
-    <mergeCell ref="Z45:AE45"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="J44:O44"/>
-    <mergeCell ref="R44:W44"/>
-    <mergeCell ref="Z44:AE44"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="R24:W24"/>
-    <mergeCell ref="Z24:AE24"/>
+    <mergeCell ref="Y127:AA127"/>
+    <mergeCell ref="AB127:AE127"/>
+    <mergeCell ref="Y122:AE122"/>
+    <mergeCell ref="Y123:AA123"/>
+    <mergeCell ref="AB123:AE123"/>
+    <mergeCell ref="Y124:AA124"/>
+    <mergeCell ref="AB124:AE124"/>
+    <mergeCell ref="Y125:AA125"/>
+    <mergeCell ref="AB125:AE125"/>
+    <mergeCell ref="Y126:AA126"/>
+    <mergeCell ref="AB126:AE126"/>
+    <mergeCell ref="I127:K127"/>
+    <mergeCell ref="L127:O127"/>
+    <mergeCell ref="Q122:W122"/>
+    <mergeCell ref="Q123:S123"/>
+    <mergeCell ref="T123:W123"/>
+    <mergeCell ref="Q124:S124"/>
+    <mergeCell ref="T124:W124"/>
+    <mergeCell ref="Q125:S125"/>
+    <mergeCell ref="T125:W125"/>
+    <mergeCell ref="Q126:S126"/>
+    <mergeCell ref="T126:W126"/>
+    <mergeCell ref="Q127:S127"/>
+    <mergeCell ref="T127:W127"/>
+    <mergeCell ref="I122:O122"/>
+    <mergeCell ref="I123:K123"/>
+    <mergeCell ref="L123:O123"/>
+    <mergeCell ref="I124:K124"/>
+    <mergeCell ref="L124:O124"/>
+    <mergeCell ref="I125:K125"/>
+    <mergeCell ref="L125:O125"/>
+    <mergeCell ref="I126:K126"/>
+    <mergeCell ref="L126:O126"/>
+    <mergeCell ref="D127:G127"/>
+    <mergeCell ref="D125:G125"/>
+    <mergeCell ref="D124:G124"/>
+    <mergeCell ref="D123:G123"/>
+    <mergeCell ref="A123:C123"/>
+    <mergeCell ref="A124:C124"/>
+    <mergeCell ref="A125:C125"/>
+    <mergeCell ref="A127:C127"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="D126:G126"/>
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="J20:O20"/>
     <mergeCell ref="R20:W20"/>
@@ -38336,49 +38347,87 @@
     <mergeCell ref="B45:G45"/>
     <mergeCell ref="J45:O45"/>
     <mergeCell ref="R45:W45"/>
-    <mergeCell ref="D127:G127"/>
-    <mergeCell ref="D125:G125"/>
-    <mergeCell ref="D124:G124"/>
-    <mergeCell ref="D123:G123"/>
-    <mergeCell ref="A123:C123"/>
-    <mergeCell ref="A124:C124"/>
-    <mergeCell ref="A125:C125"/>
-    <mergeCell ref="A127:C127"/>
-    <mergeCell ref="A126:C126"/>
-    <mergeCell ref="D126:G126"/>
-    <mergeCell ref="I127:K127"/>
-    <mergeCell ref="L127:O127"/>
-    <mergeCell ref="Q122:W122"/>
-    <mergeCell ref="Q123:S123"/>
-    <mergeCell ref="T123:W123"/>
-    <mergeCell ref="Q124:S124"/>
-    <mergeCell ref="T124:W124"/>
-    <mergeCell ref="Q125:S125"/>
-    <mergeCell ref="T125:W125"/>
-    <mergeCell ref="Q126:S126"/>
-    <mergeCell ref="T126:W126"/>
-    <mergeCell ref="Q127:S127"/>
-    <mergeCell ref="T127:W127"/>
-    <mergeCell ref="I122:O122"/>
-    <mergeCell ref="I123:K123"/>
-    <mergeCell ref="L123:O123"/>
-    <mergeCell ref="I124:K124"/>
-    <mergeCell ref="L124:O124"/>
-    <mergeCell ref="I125:K125"/>
-    <mergeCell ref="L125:O125"/>
-    <mergeCell ref="I126:K126"/>
-    <mergeCell ref="L126:O126"/>
-    <mergeCell ref="Y127:AA127"/>
-    <mergeCell ref="AB127:AE127"/>
-    <mergeCell ref="Y122:AE122"/>
-    <mergeCell ref="Y123:AA123"/>
-    <mergeCell ref="AB123:AE123"/>
-    <mergeCell ref="Y124:AA124"/>
-    <mergeCell ref="AB124:AE124"/>
-    <mergeCell ref="Y125:AA125"/>
-    <mergeCell ref="AB125:AE125"/>
-    <mergeCell ref="Y126:AA126"/>
-    <mergeCell ref="AB126:AE126"/>
+    <mergeCell ref="Z45:AE45"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="J44:O44"/>
+    <mergeCell ref="R44:W44"/>
+    <mergeCell ref="Z44:AE44"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="R24:W24"/>
+    <mergeCell ref="Z24:AE24"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="J48:O48"/>
+    <mergeCell ref="R48:W48"/>
+    <mergeCell ref="Z48:AE48"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="J47:O47"/>
+    <mergeCell ref="R47:W47"/>
+    <mergeCell ref="Z47:AE47"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="J46:O46"/>
+    <mergeCell ref="R46:W46"/>
+    <mergeCell ref="Z46:AE46"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="J70:O70"/>
+    <mergeCell ref="R70:W70"/>
+    <mergeCell ref="Z70:AE70"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="J69:O69"/>
+    <mergeCell ref="R69:W69"/>
+    <mergeCell ref="Z69:AE69"/>
+    <mergeCell ref="B68:G68"/>
+    <mergeCell ref="J68:O68"/>
+    <mergeCell ref="R68:W68"/>
+    <mergeCell ref="Z68:AE68"/>
+    <mergeCell ref="B92:G92"/>
+    <mergeCell ref="J92:O92"/>
+    <mergeCell ref="R92:W92"/>
+    <mergeCell ref="Z92:AE92"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="J72:O72"/>
+    <mergeCell ref="R72:W72"/>
+    <mergeCell ref="Z72:AE72"/>
+    <mergeCell ref="B71:G71"/>
+    <mergeCell ref="J71:O71"/>
+    <mergeCell ref="R71:W71"/>
+    <mergeCell ref="Z71:AE71"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="J95:O95"/>
+    <mergeCell ref="R95:W95"/>
+    <mergeCell ref="Z95:AE95"/>
+    <mergeCell ref="B94:G94"/>
+    <mergeCell ref="J94:O94"/>
+    <mergeCell ref="R94:W94"/>
+    <mergeCell ref="Z94:AE94"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="J93:O93"/>
+    <mergeCell ref="R93:W93"/>
+    <mergeCell ref="Z93:AE93"/>
+    <mergeCell ref="B117:G117"/>
+    <mergeCell ref="J117:O117"/>
+    <mergeCell ref="R117:W117"/>
+    <mergeCell ref="Z117:AE117"/>
+    <mergeCell ref="B116:G116"/>
+    <mergeCell ref="J116:O116"/>
+    <mergeCell ref="R116:W116"/>
+    <mergeCell ref="Z116:AE116"/>
+    <mergeCell ref="B96:G96"/>
+    <mergeCell ref="J96:O96"/>
+    <mergeCell ref="R96:W96"/>
+    <mergeCell ref="Z96:AE96"/>
+    <mergeCell ref="B120:G120"/>
+    <mergeCell ref="J120:O120"/>
+    <mergeCell ref="R120:W120"/>
+    <mergeCell ref="Z120:AE120"/>
+    <mergeCell ref="B119:G119"/>
+    <mergeCell ref="J119:O119"/>
+    <mergeCell ref="R119:W119"/>
+    <mergeCell ref="Z119:AE119"/>
+    <mergeCell ref="B118:G118"/>
+    <mergeCell ref="J118:O118"/>
+    <mergeCell ref="R118:W118"/>
+    <mergeCell ref="Z118:AE118"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -51178,4 +51227,322 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="6" width="9.140625" style="20"/>
+    <col min="10" max="12" width="9.140625" style="20"/>
+    <col min="16" max="17" width="9.140625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="G1" t="s">
+        <v>362</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="M1" t="s">
+        <v>363</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B2">
+        <v>10.1</v>
+      </c>
+      <c r="C2">
+        <f>B2*0.64</f>
+        <v>6.4639999999999995</v>
+      </c>
+      <c r="D2" s="20">
+        <v>42.1</v>
+      </c>
+      <c r="E2" s="20">
+        <f>D2*0.64</f>
+        <v>26.944000000000003</v>
+      </c>
+      <c r="G2" t="s">
+        <v>373</v>
+      </c>
+      <c r="H2">
+        <v>8.4</v>
+      </c>
+      <c r="I2" s="20">
+        <f>H2*0.64</f>
+        <v>5.3760000000000003</v>
+      </c>
+      <c r="K2" s="20">
+        <f>J2*0.64</f>
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>373</v>
+      </c>
+      <c r="O2" s="20">
+        <f>N2*0.64</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="20">
+        <f>P2*0.64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B3">
+        <v>10.1</v>
+      </c>
+      <c r="C3" s="20">
+        <f t="shared" ref="C3:C8" si="0">B3*0.64</f>
+        <v>6.4639999999999995</v>
+      </c>
+      <c r="D3" s="20">
+        <v>24.8</v>
+      </c>
+      <c r="E3" s="20">
+        <f t="shared" ref="E3:E8" si="1">D3*0.64</f>
+        <v>15.872000000000002</v>
+      </c>
+      <c r="G3" t="s">
+        <v>374</v>
+      </c>
+      <c r="I3" s="20">
+        <f t="shared" ref="I3:I8" si="2">H3*0.64</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="20">
+        <f t="shared" ref="K3:K8" si="3">J3*0.64</f>
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>374</v>
+      </c>
+      <c r="O3" s="20">
+        <f t="shared" ref="O3:O8" si="4">N3*0.64</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="20">
+        <f t="shared" ref="Q3:Q8" si="5">P3*0.64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>367</v>
+      </c>
+      <c r="B4">
+        <v>6.6</v>
+      </c>
+      <c r="C4" s="20">
+        <f t="shared" si="0"/>
+        <v>4.2240000000000002</v>
+      </c>
+      <c r="D4" s="20">
+        <v>18.8</v>
+      </c>
+      <c r="E4" s="20">
+        <f t="shared" si="1"/>
+        <v>12.032</v>
+      </c>
+      <c r="G4" t="s">
+        <v>375</v>
+      </c>
+      <c r="I4" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>363</v>
+      </c>
+      <c r="O4" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>368</v>
+      </c>
+      <c r="C5" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>376</v>
+      </c>
+      <c r="I5" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>369</v>
+      </c>
+      <c r="C6" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>370</v>
+      </c>
+      <c r="I6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>370</v>
+      </c>
+      <c r="C7" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>371</v>
+      </c>
+      <c r="I7" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>371</v>
+      </c>
+      <c r="C8" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
* FIX - Change base animation module to stop the animation from playing when it is in full retracted or full-deployed states; this fixes some minor misalignment issues, and could potentially clean up a few other issues as well. * FIX - Fix missing colliders on SC-E-FS * FIX - Wheel module will now only deploy on gear deploy commands, and only retract on retract commands * FIX - Add start-bounds-collider support to wheel module * FIX - Add bounds colliders to SC-E landing gear * UPDATE - More work on SC-E textures
</commit_message>
<xml_diff>
--- a/GameData/SSTU/Parts/Parts-MassCalc.xlsx
+++ b/GameData/SSTU/Parts/Parts-MassCalc.xlsx
@@ -51234,7 +51234,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51309,6 +51309,10 @@
         <f>D2*0.64</f>
         <v>26.944000000000003</v>
       </c>
+      <c r="F2" s="20">
+        <f>E2</f>
+        <v>26.944000000000003</v>
+      </c>
       <c r="G2" t="s">
         <v>373</v>
       </c>
@@ -51353,6 +51357,10 @@
         <f t="shared" ref="E3:E8" si="1">D3*0.64</f>
         <v>15.872000000000002</v>
       </c>
+      <c r="F3" s="20">
+        <f>F2+E3</f>
+        <v>42.816000000000003</v>
+      </c>
       <c r="G3" t="s">
         <v>374</v>
       </c>
@@ -51393,6 +51401,10 @@
       <c r="E4" s="20">
         <f t="shared" si="1"/>
         <v>12.032</v>
+      </c>
+      <c r="F4" s="20">
+        <f>F3+E4</f>
+        <v>54.847999999999999</v>
       </c>
       <c r="G4" t="s">
         <v>375</v>

</xml_diff>